<commit_message>
Improvements to xloSort: * Add help strings, * Avoid storing permutation during inplace rearrangement * Support default sort ordering * Use "at" for faster array access (also in xloFillNA) * Simplify ExcelObj::compare so it doesn't do a whole lot of string conversion if types don't match.  Numbers generally sort before strings lexically, so it provided little benefit.
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -8,19 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C50EB2-654A-4BBB-909F-F66A4035903A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CC06AF-02B6-44C8-92DC-395F95739B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="-108" windowWidth="22260" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="888" yWindow="-108" windowWidth="22260" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
     <sheet name="Concat" sheetId="2" r:id="rId2"/>
+    <sheet name="Sort" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>1, 2; 3, 4;</t>
   </si>
@@ -88,9 +86,6 @@
     <t>1,2;3;,4</t>
   </si>
   <si>
-    <t>xloBlock / xloFill</t>
-  </si>
-  <si>
     <t>Foo</t>
   </si>
   <si>
@@ -125,12 +120,75 @@
   </si>
   <si>
     <t>Check numbers are converted to string</t>
+  </si>
+  <si>
+    <t>Fox</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>BOX</t>
+  </si>
+  <si>
+    <t>Sort ascending, no case, 1st column</t>
+  </si>
+  <si>
+    <t>Repeat with named column</t>
+  </si>
+  <si>
+    <t>xloSort</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>FOO</t>
+  </si>
+  <si>
+    <t>FOOD</t>
+  </si>
+  <si>
+    <t>FooDs</t>
+  </si>
+  <si>
+    <t>first col ascending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort by second col descending, </t>
+  </si>
+  <si>
+    <t>Sort mixed data case insensitive</t>
+  </si>
+  <si>
+    <t>and case sensitive</t>
+  </si>
+  <si>
+    <t>Sort array of doubles, no descriptors specified</t>
+  </si>
+  <si>
+    <t>xloBlock / xloFill / xloFillNA</t>
+  </si>
+  <si>
+    <t>xloFillNA applied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000E+00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -209,6 +267,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,50 +589,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S29"/>
+  <dimension ref="B2:R29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="C2" s="6"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="4" t="str">
-        <f t="array" ref="K6:M8">_xll.xloBlock(C6,C7,D7,E7,F7)</f>
+      <c r="J6" s="4" t="str">
+        <f t="array" ref="J6:L8">_xll.xloBlock(C6,C7,D7,E7,F7)</f>
         <v>A</v>
       </c>
-      <c r="L6" s="5" t="str">
+      <c r="K6" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="M6" s="5" t="e">
+      <c r="L6" s="5" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -582,64 +649,67 @@
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="J7" s="5" t="str">
+        <v>C</v>
+      </c>
       <c r="K7" s="5" t="str">
-        <v>C</v>
-      </c>
-      <c r="L7" s="5" t="str">
         <v>D</v>
       </c>
-      <c r="M7" s="5" t="e">
+      <c r="L7" s="5" t="e">
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J8" s="5" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="K8" s="5" t="e">
         <v>#N/A</v>
       </c>
       <c r="L8" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M8" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="N10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="4" t="str">
-        <f t="array" ref="K12:M15">_xll.xloBlock(C12,C13:D14,E13:F14,G13,_xll.xloFill(H13,2,1))</f>
+      <c r="J12" s="4" t="str">
+        <f t="array" ref="J12:L15">_xll.xloBlock(C12,C13:D14,E13:F14,G13,_xll.xloFill(H13,2,1))</f>
         <v>A</v>
       </c>
+      <c r="K12" s="5" t="str">
+        <v>A</v>
+      </c>
       <c r="L12" s="5" t="str">
+        <v>C</v>
+      </c>
+      <c r="N12" s="5" t="str">
+        <f t="array" ref="N12:P15">_xll.xloFillNA("NOPE",J12:L15)</f>
         <v>A</v>
       </c>
-      <c r="M12" s="5" t="str">
+      <c r="O12" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="P12" s="5" t="str">
         <v>C</v>
       </c>
-      <c r="P12" t="str">
-        <f t="array" ref="P12:R15">_xll.xloFillNA("NOPE",K12:M15)</f>
-        <v>A</v>
-      </c>
-      <c r="Q12" t="str">
-        <v>A</v>
-      </c>
-      <c r="R12" t="str">
-        <v>C</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
@@ -661,26 +731,26 @@
       <c r="H13" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="J13" s="5" t="str">
+        <v>A</v>
+      </c>
       <c r="K13" s="5" t="str">
         <v>A</v>
       </c>
-      <c r="L13" s="5" t="str">
+      <c r="L13" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N13" s="5" t="str">
         <v>A</v>
       </c>
-      <c r="M13" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P13" t="str">
+      <c r="O13" s="5" t="str">
         <v>A</v>
       </c>
-      <c r="Q13" t="str">
-        <v>A</v>
-      </c>
-      <c r="R13" t="str">
+      <c r="P13" s="5" t="str">
         <v>NOPE</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
@@ -695,75 +765,75 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
+      <c r="J14" s="5" t="str">
+        <v>B</v>
+      </c>
       <c r="K14" s="5" t="str">
         <v>B</v>
       </c>
       <c r="L14" s="5" t="str">
+        <v>F</v>
+      </c>
+      <c r="N14" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="M14" s="5" t="str">
+      <c r="O14" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="P14" s="5" t="str">
         <v>F</v>
       </c>
-      <c r="P14" t="str">
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J15" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="Q14" t="str">
-        <v>B</v>
-      </c>
-      <c r="R14" t="str">
-        <v>F</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="K15" s="5" t="str">
         <v>B</v>
       </c>
       <c r="L15" s="5" t="str">
+        <v>F</v>
+      </c>
+      <c r="N15" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="M15" s="5" t="str">
+      <c r="O15" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="P15" s="5" t="str">
         <v>F</v>
       </c>
-      <c r="P15" t="str">
-        <v>B</v>
-      </c>
-      <c r="Q15" t="str">
-        <v>B</v>
-      </c>
-      <c r="R15" t="str">
-        <v>F</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="4" t="str">
-        <f t="array" ref="K19:N22">_xll.xloBlock(C19,C20:D21,_xll.xloFill(E20,2,2),F20,G20)</f>
+      <c r="J19" s="4" t="str">
+        <f t="array" ref="J19:M22">_xll.xloBlock(C19,C20:D21,_xll.xloFill(E20,2,2),F20,G20)</f>
         <v>A</v>
       </c>
+      <c r="K19" s="5" t="str">
+        <v>A</v>
+      </c>
       <c r="L19" s="5" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="M19" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="N19" s="5" t="str">
-        <v>B</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
@@ -783,20 +853,20 @@
       <c r="G20" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="J20" s="5" t="str">
+        <v>A</v>
+      </c>
       <c r="K20" s="5" t="str">
         <v>A</v>
       </c>
       <c r="L20" s="5" t="str">
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="M20" s="5" t="str">
         <v>B</v>
       </c>
-      <c r="N20" s="5" t="str">
-        <v>B</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="str">
         <v>A</v>
       </c>
@@ -806,20 +876,23 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="K21" s="5" t="str">
+      <c r="J21" s="5" t="str">
         <v>C</v>
+      </c>
+      <c r="K21" s="5" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L21" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M21" s="5" t="e">
+      <c r="M21" s="5" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J22" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N21" s="5" t="str">
-        <v>D</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
       <c r="K22" s="5" t="e">
         <v>#N/A</v>
       </c>
@@ -829,53 +902,53 @@
       <c r="M22" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N22" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="O24" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="4" t="str">
-        <f t="array" ref="K26:N29">_xll.xloBlock(C26,C27:D28,_xll.xloFill(E27,2,2),F27,G27)</f>
+      <c r="J26" s="4" t="str">
+        <f t="array" ref="J26:M29">_xll.xloBlock(C26,C27:D28,_xll.xloFill(E27,2,2),F27,G27)</f>
         <v>A</v>
       </c>
-      <c r="L26" s="5" t="str">
+      <c r="K26" s="5" t="str">
         <v>A</v>
+      </c>
+      <c r="L26" s="5" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="M26" s="5" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N26" s="5" t="e">
+      <c r="O26" s="5" t="str">
+        <f t="array" ref="O26:R29">_xll.xloFillNA(".",J26:M29,FALSE)</f>
+        <v>A</v>
+      </c>
+      <c r="P26" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="Q26" s="5" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P26" t="str">
-        <f t="array" ref="P26:S29">_xll.xloFillNA(".",K26:N29,FALSE)</f>
-        <v>A</v>
-      </c>
-      <c r="Q26" t="str">
-        <v>A</v>
-      </c>
-      <c r="R26" t="e">
+      <c r="R26" s="5" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="S26" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>9</v>
       </c>
@@ -896,32 +969,32 @@
       <c r="G27" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="J27" s="5" t="str">
+        <v>A</v>
+      </c>
       <c r="K27" s="5" t="str">
         <v>A</v>
       </c>
-      <c r="L27" s="5" t="str">
-        <v>A</v>
+      <c r="L27" s="5" t="e">
+        <v>#DIV/0!</v>
       </c>
       <c r="M27" s="5" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="N27" s="5" t="e">
+      <c r="O27" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="P27" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="Q27" s="5" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="P27" t="str">
-        <v>A</v>
-      </c>
-      <c r="Q27" t="str">
-        <v>A</v>
-      </c>
-      <c r="R27" t="e">
+      <c r="R27" s="5" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="S27" t="e">
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C28" s="2" t="str">
         <v>A</v>
       </c>
@@ -931,8 +1004,11 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="K28" s="5" t="str">
+      <c r="J28" s="5" t="str">
         <v>Left</v>
+      </c>
+      <c r="K28" s="5" t="e">
+        <v>#N/A</v>
       </c>
       <c r="L28" s="5" t="e">
         <v>#N/A</v>
@@ -940,163 +1016,1896 @@
       <c r="M28" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="N28" s="5" t="e">
+      <c r="O28" s="5" t="str">
+        <v>Left</v>
+      </c>
+      <c r="P28" s="5" t="str">
+        <v>.</v>
+      </c>
+      <c r="Q28" s="5" t="str">
+        <v>.</v>
+      </c>
+      <c r="R28" s="5" t="str">
+        <v>.</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="J29" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P28" t="str">
-        <v>Left</v>
-      </c>
-      <c r="Q28" t="str">
-        <v>.</v>
-      </c>
-      <c r="R28" t="str">
-        <v>.</v>
-      </c>
-      <c r="S28" t="str">
-        <v>.</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
       <c r="K29" s="5" t="e">
         <v>#N/A</v>
       </c>
       <c r="L29" s="5" t="e">
         <v>#N/A</v>
       </c>
-      <c r="M29" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N29" s="5" t="str">
+      <c r="M29" s="5" t="str">
         <v>Right</v>
       </c>
-      <c r="P29" t="str">
+      <c r="O29" s="5" t="str">
         <v>.</v>
       </c>
-      <c r="Q29" t="str">
+      <c r="P29" s="5" t="str">
         <v>.</v>
       </c>
-      <c r="R29" t="str">
+      <c r="Q29" s="5" t="str">
         <v>.</v>
       </c>
-      <c r="S29" t="str">
+      <c r="R29" s="5" t="str">
         <v>Right</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE722B9-50C3-4C00-BF1B-32FF825F8CB4}">
-  <dimension ref="B1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I2" s="1" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="str">
+        <f>_xll.xloConcat(,I5,J5,K5)</f>
+        <v>FooBarBaz</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="I5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="str">
-        <f>_xll.xloConcat(,I4,J4,K4)</f>
-        <v>FooBarBaz</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="I4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="7" t="s">
+      <c r="I7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="str">
+        <f>_xll.xloConcat(",",I5:K5)</f>
+        <v>Foo,Bar,Baz</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="I8" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I5" s="7" t="s">
+      <c r="J8" s="7">
+        <v>3</v>
+      </c>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="str">
+        <f>_xll.xloConcat("…",I5:I8,J5,K5)</f>
+        <v>Foo…Green…Eggs…Ham…Bar…Baz</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="str">
+        <f>_xll.xloConcat("---", I5:I8, _xll.xloConcat(",",J6:J8),J5:K5)</f>
+        <v>Foo---Green---Eggs---Ham---1.000000,2.000000,3.000000---Bar---Baz</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:V105"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="12" max="12" width="4.44140625" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" customWidth="1"/>
+    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="T1" s="11"/>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="10"/>
+      <c r="V3" s="12"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="array" ref="I5:J12">_xll.xloSort(B5:C12,"a","Words")</f>
+        <v>Words</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Numbers</v>
+      </c>
+      <c r="R5" s="7">
+        <f ca="1">RAND()</f>
+        <v>0.70995829035055502</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="array" aca="1" ref="S5:S104" ca="1">_xll.xloSort(R5:R104,"a")</f>
+        <v>4.4892519097212702E-3</v>
+      </c>
+      <c r="T5">
+        <f t="array" aca="1" ref="T5:T104" ca="1">_xll.xloBenchmarkSort(R5:R104)</f>
+        <v>4.4892519097212702E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <f t="array" ref="E6:F12">_xll.xloSort(B6:C12,"a",1)</f>
+        <v>Box</v>
+      </c>
+      <c r="F6" s="5">
+        <v>7</v>
+      </c>
+      <c r="I6" s="5" t="str">
+        <v>Box</v>
+      </c>
+      <c r="J6" s="5">
+        <v>7</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="array" ref="O6:O18">_xll.xloSort(M6:M18,"a",1)</f>
+        <v>4</v>
+      </c>
+      <c r="P6" s="5">
+        <f t="array" ref="P6:P18">_xll.xloSort(M6:M18,"A",1)</f>
+        <v>4</v>
+      </c>
+      <c r="R6" s="7">
+        <v>1.4241351279182801E-2</v>
+      </c>
+      <c r="S6" s="4">
+        <f ca="1"/>
+        <v>8.9705088996498983E-3</v>
+      </c>
+      <c r="T6" s="9">
+        <f ca="1"/>
+        <v>1.4241351279182801E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <v>BOX</v>
+      </c>
+      <c r="F7" s="5">
+        <v>8</v>
+      </c>
+      <c r="I7" s="5" t="str">
+        <v>BOX</v>
+      </c>
+      <c r="J7" s="5">
+        <v>8</v>
+      </c>
+      <c r="M7" s="7">
+        <v>7</v>
+      </c>
+      <c r="O7" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="P7" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="R7" s="7">
+        <v>0.11987234330114915</v>
+      </c>
+      <c r="S7" s="4">
+        <f ca="1"/>
+        <v>1.0142003022623358E-2</v>
+      </c>
+      <c r="T7" s="9">
+        <f ca="1"/>
+        <v>0.11987234330114915</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="7">
+      <c r="C8" s="7">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="I8" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="J8" s="5">
+        <v>3</v>
+      </c>
+      <c r="M8" s="7">
+        <v>4</v>
+      </c>
+      <c r="O8" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="P8" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="R8" s="7">
+        <v>0.43199912726020961</v>
+      </c>
+      <c r="S8" s="4">
+        <f ca="1"/>
+        <v>1.4241351279182801E-2</v>
+      </c>
+      <c r="T8" s="9">
+        <f ca="1"/>
+        <v>0.43199912726020961</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="J9" s="5">
+        <v>3</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="5">
+        <v>7</v>
+      </c>
+      <c r="P9" s="5">
+        <v>7</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0.44362993322818001</v>
+      </c>
+      <c r="S9" s="4">
+        <f ca="1"/>
+        <v>1.7278225187227991E-2</v>
+      </c>
+      <c r="T9" s="9">
+        <f ca="1"/>
+        <v>0.44362993322818001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="7">
-        <v>2</v>
-      </c>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="str">
-        <f>_xll.xloConcat(",",I4:K4)</f>
-        <v>Foo,Bar,Baz</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="I7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="7">
+      <c r="I10" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1</v>
+      </c>
+      <c r="M10" s="7" t="e">
+        <f>NameError</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O10" s="5" t="str">
+        <v>Foo</v>
+      </c>
+      <c r="P10" s="5" t="str">
+        <v>FOO</v>
+      </c>
+      <c r="R10" s="7">
+        <v>0.70719203131190667</v>
+      </c>
+      <c r="S10" s="4">
+        <f ca="1"/>
+        <v>4.2989156379268589E-2</v>
+      </c>
+      <c r="T10" s="9">
+        <f ca="1"/>
+        <v>0.70719203131190667</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="F11" s="5">
         <v>3</v>
       </c>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="str">
-        <f>_xll.xloConcat("…",I4:I7,J4,K4)</f>
-        <v>Foo…Green…Eggs…Ham…Bar…Baz</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="str">
-        <f>_xll.xloConcat("---", I4:I7, _xll.xloConcat(",",J5:J7),J4:K4)</f>
-        <v>Foo---Green---Eggs---Ham---1.000000,2.000000,3.000000---Bar---Baz</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="I11" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3</v>
+      </c>
+      <c r="M11" s="7" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O11" s="5" t="str">
+        <v>FOO</v>
+      </c>
+      <c r="P11" s="5" t="str">
+        <v>FOOD</v>
+      </c>
+      <c r="R11" s="7">
+        <v>0.28303369927876221</v>
+      </c>
+      <c r="S11" s="4">
+        <f ca="1"/>
+        <v>4.8199686141203735E-2</v>
+      </c>
+      <c r="T11" s="9">
+        <f ca="1"/>
+        <v>0.28303369927876221</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="7">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="F12" s="5">
+        <v>4</v>
+      </c>
+      <c r="I12" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="J12" s="5">
+        <v>4</v>
+      </c>
+      <c r="M12" s="7">
+        <v>6.3</v>
+      </c>
+      <c r="O12" s="5" t="str">
+        <v>Food</v>
+      </c>
+      <c r="P12" s="5" t="str">
+        <v>Foo</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0.18684151297687135</v>
+      </c>
+      <c r="S12" s="4">
+        <f ca="1"/>
+        <v>5.2437735118262885E-2</v>
+      </c>
+      <c r="T12" s="9">
+        <f ca="1"/>
+        <v>0.18684151297687135</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="M13" s="7">
+        <v>6.2</v>
+      </c>
+      <c r="O13" s="5" t="str">
+        <v>FOOD</v>
+      </c>
+      <c r="P13" s="5" t="str">
+        <v>FooDs</v>
+      </c>
+      <c r="R13" s="7">
+        <v>7.6545233242765964E-2</v>
+      </c>
+      <c r="S13" s="4">
+        <f ca="1"/>
+        <v>6.063738431260568E-2</v>
+      </c>
+      <c r="T13" s="9">
+        <f ca="1"/>
+        <v>7.6545233242765964E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="I14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="5" t="str">
+        <v>FooDs</v>
+      </c>
+      <c r="P14" s="5" t="str">
+        <v>Food</v>
+      </c>
+      <c r="R14" s="7">
+        <v>0.78402600397426425</v>
+      </c>
+      <c r="S14" s="4">
+        <f ca="1"/>
+        <v>7.6545233242765964E-2</v>
+      </c>
+      <c r="T14" s="9">
+        <f ca="1"/>
+        <v>0.78402600397426425</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="E15" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="M15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="P15" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="R15" s="7">
+        <v>0.5992299667126384</v>
+      </c>
+      <c r="S15" s="4">
+        <f ca="1"/>
+        <v>9.6043732044653662E-2</v>
+      </c>
+      <c r="T15" s="9">
+        <f ca="1"/>
+        <v>0.5992299667126384</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="I16" t="str">
+        <f t="array" ref="I16:J23">_xll.xloSort(B5:C12,"d a","Numbers","Words")</f>
+        <v>Words</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Numbers</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="P16" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="R16" s="7">
+        <v>0.21129177216442607</v>
+      </c>
+      <c r="S16" s="4">
+        <f ca="1"/>
+        <v>0.10466409270245647</v>
+      </c>
+      <c r="T16" s="9">
+        <f ca="1"/>
+        <v>0.21129177216442607</v>
+      </c>
+    </row>
+    <row r="17" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="E17" s="5" t="str">
+        <f t="array" ref="E17:F23">_xll.xloSort(B6:C12,"d a",2,1)</f>
+        <v>BOX</v>
+      </c>
+      <c r="F17" s="5">
+        <v>8</v>
+      </c>
+      <c r="I17" s="5" t="str">
+        <v>BOX</v>
+      </c>
+      <c r="J17" s="5">
+        <v>8</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="5" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="P17" s="5" t="e">
+        <v>#NAME?</v>
+      </c>
+      <c r="R17" s="7">
+        <v>0.56907031356613658</v>
+      </c>
+      <c r="S17" s="4">
+        <f ca="1"/>
+        <v>0.11099657306935851</v>
+      </c>
+      <c r="T17" s="9">
+        <f ca="1"/>
+        <v>0.56907031356613658</v>
+      </c>
+    </row>
+    <row r="18" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="E18" s="5" t="str">
+        <v>Box</v>
+      </c>
+      <c r="F18" s="5">
+        <v>7</v>
+      </c>
+      <c r="I18" s="5" t="str">
+        <v>Box</v>
+      </c>
+      <c r="J18" s="5">
+        <v>7</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P18" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="R18" s="7">
+        <v>0.70052257146975117</v>
+      </c>
+      <c r="S18" s="4">
+        <f ca="1"/>
+        <v>0.11987234330114915</v>
+      </c>
+      <c r="T18" s="9">
+        <f ca="1"/>
+        <v>0.70052257146975117</v>
+      </c>
+    </row>
+    <row r="19" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="E19" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="F19" s="5">
+        <v>4</v>
+      </c>
+      <c r="I19" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="J19" s="5">
+        <v>4</v>
+      </c>
+      <c r="R19" s="7">
+        <v>0.96985704312068066</v>
+      </c>
+      <c r="S19" s="4">
+        <f ca="1"/>
+        <v>0.15138392223952224</v>
+      </c>
+      <c r="T19" s="9">
+        <f ca="1"/>
+        <v>0.96985704312068066</v>
+      </c>
+    </row>
+    <row r="20" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="E20" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="F20" s="5">
+        <v>3</v>
+      </c>
+      <c r="I20" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="J20" s="5">
+        <v>3</v>
+      </c>
+      <c r="R20" s="7">
+        <v>0.55553726039846762</v>
+      </c>
+      <c r="S20" s="4">
+        <f ca="1"/>
+        <v>0.15285256271102787</v>
+      </c>
+      <c r="T20" s="9">
+        <f ca="1"/>
+        <v>0.55553726039846762</v>
+      </c>
+    </row>
+    <row r="21" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="E21" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3</v>
+      </c>
+      <c r="I21" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="J21" s="5">
+        <v>3</v>
+      </c>
+      <c r="R21" s="7">
+        <v>0.346644941363903</v>
+      </c>
+      <c r="S21" s="4">
+        <f ca="1"/>
+        <v>0.15935651729819933</v>
+      </c>
+      <c r="T21" s="9">
+        <f ca="1"/>
+        <v>0.346644941363903</v>
+      </c>
+    </row>
+    <row r="22" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="E22" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="I22" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="J22" s="5">
+        <v>3</v>
+      </c>
+      <c r="R22" s="7">
+        <v>0.86284631971635639</v>
+      </c>
+      <c r="S22" s="4">
+        <f ca="1"/>
+        <v>0.16534127039316493</v>
+      </c>
+      <c r="T22" s="9">
+        <f ca="1"/>
+        <v>0.86284631971635639</v>
+      </c>
+    </row>
+    <row r="23" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="E23" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1</v>
+      </c>
+      <c r="R23" s="7">
+        <v>0.25958386357364216</v>
+      </c>
+      <c r="S23" s="4">
+        <f ca="1"/>
+        <v>0.18684151297687135</v>
+      </c>
+      <c r="T23" s="9">
+        <f ca="1"/>
+        <v>0.25958386357364216</v>
+      </c>
+    </row>
+    <row r="24" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R24" s="7">
+        <v>0.44578595954200495</v>
+      </c>
+      <c r="S24" s="4">
+        <f ca="1"/>
+        <v>0.19150797219437865</v>
+      </c>
+      <c r="T24" s="9">
+        <f ca="1"/>
+        <v>0.44578595954200495</v>
+      </c>
+    </row>
+    <row r="25" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R25" s="7">
+        <v>0.35070608842246354</v>
+      </c>
+      <c r="S25" s="4">
+        <f ca="1"/>
+        <v>0.19332448079141096</v>
+      </c>
+      <c r="T25" s="9">
+        <f ca="1"/>
+        <v>0.35070608842246354</v>
+      </c>
+    </row>
+    <row r="26" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R26" s="7">
+        <v>0.97062641299883634</v>
+      </c>
+      <c r="S26" s="4">
+        <f ca="1"/>
+        <v>0.20455886903305909</v>
+      </c>
+      <c r="T26" s="9">
+        <f ca="1"/>
+        <v>0.97062641299883634</v>
+      </c>
+    </row>
+    <row r="27" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R27" s="7">
+        <v>0.36303952239766712</v>
+      </c>
+      <c r="S27" s="4">
+        <f ca="1"/>
+        <v>0.21129177216442607</v>
+      </c>
+      <c r="T27" s="9">
+        <f ca="1"/>
+        <v>0.36303952239766712</v>
+      </c>
+    </row>
+    <row r="28" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R28" s="7">
+        <v>0.35500379302962237</v>
+      </c>
+      <c r="S28" s="4">
+        <f ca="1"/>
+        <v>0.21289020404938441</v>
+      </c>
+      <c r="T28" s="9">
+        <f ca="1"/>
+        <v>0.35500379302962237</v>
+      </c>
+    </row>
+    <row r="29" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R29" s="7">
+        <v>0.30991009987247375</v>
+      </c>
+      <c r="S29" s="4">
+        <f ca="1"/>
+        <v>0.24005046089105242</v>
+      </c>
+      <c r="T29" s="9">
+        <f ca="1"/>
+        <v>0.30991009987247375</v>
+      </c>
+    </row>
+    <row r="30" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R30" s="7">
+        <v>0.50309865693105404</v>
+      </c>
+      <c r="S30" s="4">
+        <f ca="1"/>
+        <v>0.24683784713265966</v>
+      </c>
+      <c r="T30" s="9">
+        <f ca="1"/>
+        <v>0.50309865693105404</v>
+      </c>
+    </row>
+    <row r="31" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R31" s="7">
+        <v>0.24683784713265966</v>
+      </c>
+      <c r="S31" s="4">
+        <f ca="1"/>
+        <v>0.25090708805825079</v>
+      </c>
+      <c r="T31" s="9">
+        <f ca="1"/>
+        <v>0.24683784713265966</v>
+      </c>
+    </row>
+    <row r="32" spans="5:20" x14ac:dyDescent="0.3">
+      <c r="R32" s="7">
+        <v>0.21289020404938441</v>
+      </c>
+      <c r="S32" s="4">
+        <f ca="1"/>
+        <v>0.25958386357364216</v>
+      </c>
+      <c r="T32" s="9">
+        <f ca="1"/>
+        <v>0.21289020404938441</v>
+      </c>
+    </row>
+    <row r="33" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R33" s="7">
+        <v>0.57712158377157863</v>
+      </c>
+      <c r="S33" s="4">
+        <f ca="1"/>
+        <v>0.26026766796149603</v>
+      </c>
+      <c r="T33" s="9">
+        <f ca="1"/>
+        <v>0.57712158377157863</v>
+      </c>
+    </row>
+    <row r="34" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R34" s="7">
+        <v>6.063738431260568E-2</v>
+      </c>
+      <c r="S34" s="4">
+        <f ca="1"/>
+        <v>0.2819709570143808</v>
+      </c>
+      <c r="T34" s="9">
+        <f ca="1"/>
+        <v>6.063738431260568E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R35" s="7">
+        <v>0.37822251634842252</v>
+      </c>
+      <c r="S35" s="4">
+        <f ca="1"/>
+        <v>0.28303369927876221</v>
+      </c>
+      <c r="T35" s="9">
+        <f ca="1"/>
+        <v>0.37822251634842252</v>
+      </c>
+    </row>
+    <row r="36" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R36" s="7">
+        <v>0.60977631212733274</v>
+      </c>
+      <c r="S36" s="4">
+        <f ca="1"/>
+        <v>0.29579294051174709</v>
+      </c>
+      <c r="T36" s="9">
+        <f ca="1"/>
+        <v>0.60977631212733274</v>
+      </c>
+    </row>
+    <row r="37" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R37" s="7">
+        <v>0.20455886903305909</v>
+      </c>
+      <c r="S37" s="4">
+        <f ca="1"/>
+        <v>0.30621594261281582</v>
+      </c>
+      <c r="T37" s="9">
+        <f ca="1"/>
+        <v>0.20455886903305909</v>
+      </c>
+    </row>
+    <row r="38" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R38" s="7">
+        <v>0.947318592329083</v>
+      </c>
+      <c r="S38" s="4">
+        <f ca="1"/>
+        <v>0.30699880764121135</v>
+      </c>
+      <c r="T38" s="9">
+        <f ca="1"/>
+        <v>0.947318592329083</v>
+      </c>
+    </row>
+    <row r="39" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R39" s="7">
+        <v>0.68147699048550281</v>
+      </c>
+      <c r="S39" s="4">
+        <f ca="1"/>
+        <v>0.30746381468864881</v>
+      </c>
+      <c r="T39" s="9">
+        <f ca="1"/>
+        <v>0.68147699048550281</v>
+      </c>
+    </row>
+    <row r="40" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R40" s="7">
+        <v>0.90600850571232516</v>
+      </c>
+      <c r="S40" s="4">
+        <f ca="1"/>
+        <v>0.30991009987247375</v>
+      </c>
+      <c r="T40" s="9">
+        <f ca="1"/>
+        <v>0.90600850571232516</v>
+      </c>
+    </row>
+    <row r="41" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R41" s="7">
+        <v>0.85960749899325406</v>
+      </c>
+      <c r="S41" s="4">
+        <f ca="1"/>
+        <v>0.34322350221251363</v>
+      </c>
+      <c r="T41" s="9">
+        <f ca="1"/>
+        <v>0.85960749899325406</v>
+      </c>
+    </row>
+    <row r="42" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R42" s="7">
+        <v>4.2989156379268589E-2</v>
+      </c>
+      <c r="S42" s="4">
+        <f ca="1"/>
+        <v>0.346644941363903</v>
+      </c>
+      <c r="T42" s="9">
+        <f ca="1"/>
+        <v>4.2989156379268589E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R43" s="7">
+        <v>0.15285256271102787</v>
+      </c>
+      <c r="S43" s="4">
+        <f ca="1"/>
+        <v>0.35070608842246354</v>
+      </c>
+      <c r="T43" s="9">
+        <f ca="1"/>
+        <v>0.15285256271102787</v>
+      </c>
+    </row>
+    <row r="44" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R44" s="7">
+        <v>4.4892519097212702E-3</v>
+      </c>
+      <c r="S44" s="4">
+        <f ca="1"/>
+        <v>0.35500379302962237</v>
+      </c>
+      <c r="T44" s="9">
+        <f ca="1"/>
+        <v>4.4892519097212702E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R45" s="7">
+        <v>9.6043732044653662E-2</v>
+      </c>
+      <c r="S45" s="4">
+        <f ca="1"/>
+        <v>0.36303952239766712</v>
+      </c>
+      <c r="T45" s="9">
+        <f ca="1"/>
+        <v>9.6043732044653662E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R46" s="7">
+        <v>0.30746381468864881</v>
+      </c>
+      <c r="S46" s="4">
+        <f ca="1"/>
+        <v>0.37590154211670712</v>
+      </c>
+      <c r="T46" s="9">
+        <f ca="1"/>
+        <v>0.30746381468864881</v>
+      </c>
+    </row>
+    <row r="47" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R47" s="7">
+        <v>0.15935651729819933</v>
+      </c>
+      <c r="S47" s="4">
+        <f ca="1"/>
+        <v>0.37822251634842252</v>
+      </c>
+      <c r="T47" s="9">
+        <f ca="1"/>
+        <v>0.15935651729819933</v>
+      </c>
+    </row>
+    <row r="48" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R48" s="7">
+        <v>0.73492497530386436</v>
+      </c>
+      <c r="S48" s="4">
+        <f ca="1"/>
+        <v>0.38122419173045929</v>
+      </c>
+      <c r="T48" s="9">
+        <f ca="1"/>
+        <v>0.73492497530386436</v>
+      </c>
+    </row>
+    <row r="49" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R49" s="7">
+        <v>0.93045439034459587</v>
+      </c>
+      <c r="S49" s="4">
+        <f ca="1"/>
+        <v>0.38693032613344891</v>
+      </c>
+      <c r="T49" s="9">
+        <f ca="1"/>
+        <v>0.93045439034459587</v>
+      </c>
+    </row>
+    <row r="50" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R50" s="7">
+        <v>0.70064205520622802</v>
+      </c>
+      <c r="S50" s="4">
+        <f ca="1"/>
+        <v>0.38924117354343202</v>
+      </c>
+      <c r="T50" s="9">
+        <f ca="1"/>
+        <v>0.70064205520622802</v>
+      </c>
+    </row>
+    <row r="51" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R51" s="7">
+        <v>0.34322350221251363</v>
+      </c>
+      <c r="S51" s="4">
+        <f ca="1"/>
+        <v>0.41032128248045219</v>
+      </c>
+      <c r="T51" s="9">
+        <f ca="1"/>
+        <v>0.34322350221251363</v>
+      </c>
+    </row>
+    <row r="52" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R52" s="7">
+        <v>0.30699880764121135</v>
+      </c>
+      <c r="S52" s="4">
+        <f ca="1"/>
+        <v>0.43199912726020961</v>
+      </c>
+      <c r="T52" s="9">
+        <f ca="1"/>
+        <v>0.30699880764121135</v>
+      </c>
+    </row>
+    <row r="53" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R53" s="7">
+        <v>0.56072877256876819</v>
+      </c>
+      <c r="S53" s="4">
+        <f ca="1"/>
+        <v>0.44362993322818001</v>
+      </c>
+      <c r="T53" s="9">
+        <f ca="1"/>
+        <v>0.56072877256876819</v>
+      </c>
+    </row>
+    <row r="54" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R54" s="7">
+        <v>1.0142003022623358E-2</v>
+      </c>
+      <c r="S54" s="4">
+        <f ca="1"/>
+        <v>0.44578595954200495</v>
+      </c>
+      <c r="T54" s="9">
+        <f ca="1"/>
+        <v>1.0142003022623358E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R55" s="7">
+        <v>0.38122419173045929</v>
+      </c>
+      <c r="S55" s="4">
+        <f ca="1"/>
+        <v>0.50309865693105404</v>
+      </c>
+      <c r="T55" s="9">
+        <f ca="1"/>
+        <v>0.38122419173045929</v>
+      </c>
+    </row>
+    <row r="56" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R56" s="7">
+        <v>0.60411978716231773</v>
+      </c>
+      <c r="S56" s="4">
+        <f ca="1"/>
+        <v>0.55553726039846762</v>
+      </c>
+      <c r="T56" s="9">
+        <f ca="1"/>
+        <v>0.60411978716231773</v>
+      </c>
+    </row>
+    <row r="57" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R57" s="7">
+        <v>0.2819709570143808</v>
+      </c>
+      <c r="S57" s="4">
+        <f ca="1"/>
+        <v>0.56072877256876819</v>
+      </c>
+      <c r="T57" s="9">
+        <f ca="1"/>
+        <v>0.2819709570143808</v>
+      </c>
+    </row>
+    <row r="58" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R58" s="7">
+        <v>0.58507289523339523</v>
+      </c>
+      <c r="S58" s="4">
+        <f ca="1"/>
+        <v>0.56613202852270661</v>
+      </c>
+      <c r="T58" s="9">
+        <f ca="1"/>
+        <v>0.58507289523339523</v>
+      </c>
+    </row>
+    <row r="59" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R59" s="7">
+        <v>0.38693032613344891</v>
+      </c>
+      <c r="S59" s="4">
+        <f ca="1"/>
+        <v>0.56907031356613658</v>
+      </c>
+      <c r="T59" s="9">
+        <f ca="1"/>
+        <v>0.38693032613344891</v>
+      </c>
+    </row>
+    <row r="60" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R60" s="7">
+        <v>0.38924117354343202</v>
+      </c>
+      <c r="S60" s="4">
+        <f ca="1"/>
+        <v>0.57665750527755044</v>
+      </c>
+      <c r="T60" s="9">
+        <f ca="1"/>
+        <v>0.38924117354343202</v>
+      </c>
+    </row>
+    <row r="61" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R61" s="7">
+        <v>0.25090708805825079</v>
+      </c>
+      <c r="S61" s="4">
+        <f ca="1"/>
+        <v>0.57712158377157863</v>
+      </c>
+      <c r="T61" s="9">
+        <f ca="1"/>
+        <v>0.25090708805825079</v>
+      </c>
+    </row>
+    <row r="62" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R62" s="7">
+        <v>0.99561513362173215</v>
+      </c>
+      <c r="S62" s="4">
+        <f ca="1"/>
+        <v>0.58507289523339523</v>
+      </c>
+      <c r="T62" s="9">
+        <f ca="1"/>
+        <v>0.99561513362173215</v>
+      </c>
+    </row>
+    <row r="63" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R63" s="7">
+        <v>0.41032128248045219</v>
+      </c>
+      <c r="S63" s="4">
+        <f ca="1"/>
+        <v>0.5992299667126384</v>
+      </c>
+      <c r="T63" s="9">
+        <f ca="1"/>
+        <v>0.41032128248045219</v>
+      </c>
+    </row>
+    <row r="64" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R64" s="7">
+        <v>0.10466409270245647</v>
+      </c>
+      <c r="S64" s="4">
+        <f ca="1"/>
+        <v>0.60411978716231773</v>
+      </c>
+      <c r="T64" s="9">
+        <f ca="1"/>
+        <v>0.10466409270245647</v>
+      </c>
+    </row>
+    <row r="65" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R65" s="7">
+        <v>0.96328079049455895</v>
+      </c>
+      <c r="S65" s="4">
+        <f ca="1"/>
+        <v>0.60977631212733274</v>
+      </c>
+      <c r="T65" s="9">
+        <f ca="1"/>
+        <v>0.96328079049455895</v>
+      </c>
+    </row>
+    <row r="66" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R66" s="7">
+        <v>0.99946735978378209</v>
+      </c>
+      <c r="S66" s="4">
+        <f ca="1"/>
+        <v>0.61835596776400625</v>
+      </c>
+      <c r="T66" s="9">
+        <f ca="1"/>
+        <v>0.99946735978378209</v>
+      </c>
+    </row>
+    <row r="67" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R67" s="7">
+        <v>0.82935893028115659</v>
+      </c>
+      <c r="S67" s="4">
+        <f ca="1"/>
+        <v>0.64226730514312624</v>
+      </c>
+      <c r="T67" s="9">
+        <f ca="1"/>
+        <v>0.82935893028115659</v>
+      </c>
+    </row>
+    <row r="68" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R68" s="7">
+        <v>0.15138392223952224</v>
+      </c>
+      <c r="S68" s="4">
+        <f ca="1"/>
+        <v>0.64904570666639028</v>
+      </c>
+      <c r="T68" s="9">
+        <f ca="1"/>
+        <v>0.15138392223952224</v>
+      </c>
+    </row>
+    <row r="69" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R69" s="7">
+        <v>0.26026766796149603</v>
+      </c>
+      <c r="S69" s="4">
+        <f ca="1"/>
+        <v>0.67056525021684998</v>
+      </c>
+      <c r="T69" s="9">
+        <f ca="1"/>
+        <v>0.26026766796149603</v>
+      </c>
+    </row>
+    <row r="70" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R70" s="7">
+        <v>0.56613202852270661</v>
+      </c>
+      <c r="S70" s="4">
+        <f ca="1"/>
+        <v>0.68147699048550281</v>
+      </c>
+      <c r="T70" s="9">
+        <f ca="1"/>
+        <v>0.56613202852270661</v>
+      </c>
+    </row>
+    <row r="71" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R71" s="7">
+        <v>0.57665750527755044</v>
+      </c>
+      <c r="S71" s="4">
+        <f ca="1"/>
+        <v>0.70052257146975117</v>
+      </c>
+      <c r="T71" s="9">
+        <f ca="1"/>
+        <v>0.57665750527755044</v>
+      </c>
+    </row>
+    <row r="72" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R72" s="7">
+        <v>0.83938605783476394</v>
+      </c>
+      <c r="S72" s="4">
+        <f ca="1"/>
+        <v>0.70064205520622802</v>
+      </c>
+      <c r="T72" s="9">
+        <f ca="1"/>
+        <v>0.83938605783476394</v>
+      </c>
+    </row>
+    <row r="73" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R73" s="7">
+        <v>0.37590154211670712</v>
+      </c>
+      <c r="S73" s="4">
+        <f ca="1"/>
+        <v>0.70719203131190667</v>
+      </c>
+      <c r="T73" s="9">
+        <f ca="1"/>
+        <v>0.37590154211670712</v>
+      </c>
+    </row>
+    <row r="74" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R74" s="7">
+        <v>0.95887267917531893</v>
+      </c>
+      <c r="S74" s="4">
+        <f ca="1"/>
+        <v>0.70995829035055502</v>
+      </c>
+      <c r="T74" s="9">
+        <f ca="1"/>
+        <v>0.95887267917531893</v>
+      </c>
+    </row>
+    <row r="75" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R75" s="7">
+        <v>0.11099657306935851</v>
+      </c>
+      <c r="S75" s="4">
+        <f ca="1"/>
+        <v>0.71755405184921206</v>
+      </c>
+      <c r="T75" s="9">
+        <f ca="1"/>
+        <v>0.11099657306935851</v>
+      </c>
+    </row>
+    <row r="76" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R76" s="7">
+        <v>0.67056525021684998</v>
+      </c>
+      <c r="S76" s="4">
+        <f ca="1"/>
+        <v>0.73492497530386436</v>
+      </c>
+      <c r="T76" s="9">
+        <f ca="1"/>
+        <v>0.67056525021684998</v>
+      </c>
+    </row>
+    <row r="77" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R77" s="7">
+        <v>0.82167610222353549</v>
+      </c>
+      <c r="S77" s="4">
+        <f ca="1"/>
+        <v>0.78402600397426425</v>
+      </c>
+      <c r="T77" s="9">
+        <f ca="1"/>
+        <v>0.82167610222353549</v>
+      </c>
+    </row>
+    <row r="78" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R78" s="7">
+        <v>0.79626472404113779</v>
+      </c>
+      <c r="S78" s="4">
+        <f ca="1"/>
+        <v>0.79404440245310404</v>
+      </c>
+      <c r="T78" s="9">
+        <f ca="1"/>
+        <v>0.79626472404113779</v>
+      </c>
+    </row>
+    <row r="79" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R79" s="7">
+        <v>0.79404440245310404</v>
+      </c>
+      <c r="S79" s="4">
+        <f ca="1"/>
+        <v>0.79626472404113779</v>
+      </c>
+      <c r="T79" s="9">
+        <f ca="1"/>
+        <v>0.79404440245310404</v>
+      </c>
+    </row>
+    <row r="80" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R80" s="7">
+        <v>0.24005046089105242</v>
+      </c>
+      <c r="S80" s="4">
+        <f ca="1"/>
+        <v>0.79852373727417758</v>
+      </c>
+      <c r="T80" s="9">
+        <f ca="1"/>
+        <v>0.24005046089105242</v>
+      </c>
+    </row>
+    <row r="81" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R81" s="7">
+        <v>1.7278225187227991E-2</v>
+      </c>
+      <c r="S81" s="4">
+        <f ca="1"/>
+        <v>0.82167610222353549</v>
+      </c>
+      <c r="T81" s="9">
+        <f ca="1"/>
+        <v>1.7278225187227991E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R82" s="7">
+        <v>0.83233289115523368</v>
+      </c>
+      <c r="S82" s="4">
+        <f ca="1"/>
+        <v>0.82935893028115659</v>
+      </c>
+      <c r="T82" s="9">
+        <f ca="1"/>
+        <v>0.83233289115523368</v>
+      </c>
+    </row>
+    <row r="83" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R83" s="7">
+        <v>5.2437735118262885E-2</v>
+      </c>
+      <c r="S83" s="4">
+        <f ca="1"/>
+        <v>0.83233289115523368</v>
+      </c>
+      <c r="T83" s="9">
+        <f ca="1"/>
+        <v>5.2437735118262885E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R84" s="7">
+        <v>0.79852373727417758</v>
+      </c>
+      <c r="S84" s="4">
+        <f ca="1"/>
+        <v>0.83938605783476394</v>
+      </c>
+      <c r="T84" s="9">
+        <f ca="1"/>
+        <v>0.79852373727417758</v>
+      </c>
+    </row>
+    <row r="85" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R85" s="7">
+        <v>0.88056162198032462</v>
+      </c>
+      <c r="S85" s="4">
+        <f ca="1"/>
+        <v>0.85960749899325406</v>
+      </c>
+      <c r="T85" s="9">
+        <f ca="1"/>
+        <v>0.88056162198032462</v>
+      </c>
+    </row>
+    <row r="86" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R86" s="7">
+        <v>0.29579294051174709</v>
+      </c>
+      <c r="S86" s="4">
+        <f ca="1"/>
+        <v>0.86081826465673084</v>
+      </c>
+      <c r="T86" s="9">
+        <f ca="1"/>
+        <v>0.29579294051174709</v>
+      </c>
+    </row>
+    <row r="87" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R87" s="7">
+        <v>0.71755405184921206</v>
+      </c>
+      <c r="S87" s="4">
+        <f ca="1"/>
+        <v>0.86284631971635639</v>
+      </c>
+      <c r="T87" s="9">
+        <f ca="1"/>
+        <v>0.71755405184921206</v>
+      </c>
+    </row>
+    <row r="88" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R88" s="7">
+        <v>0.97078869366691067</v>
+      </c>
+      <c r="S88" s="4">
+        <f ca="1"/>
+        <v>0.88056162198032462</v>
+      </c>
+      <c r="T88" s="9">
+        <f ca="1"/>
+        <v>0.97078869366691067</v>
+      </c>
+    </row>
+    <row r="89" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R89" s="7">
+        <v>4.8199686141203735E-2</v>
+      </c>
+      <c r="S89" s="4">
+        <f ca="1"/>
+        <v>0.89299919543294648</v>
+      </c>
+      <c r="T89" s="9">
+        <f ca="1"/>
+        <v>4.8199686141203735E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R90" s="7">
+        <v>0.19150797219437865</v>
+      </c>
+      <c r="S90" s="4">
+        <f ca="1"/>
+        <v>0.90600850571232516</v>
+      </c>
+      <c r="T90" s="9">
+        <f ca="1"/>
+        <v>0.19150797219437865</v>
+      </c>
+    </row>
+    <row r="91" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R91" s="7">
+        <v>0.19332448079141096</v>
+      </c>
+      <c r="S91" s="4">
+        <f ca="1"/>
+        <v>0.9287334580292661</v>
+      </c>
+      <c r="T91" s="9">
+        <f ca="1"/>
+        <v>0.19332448079141096</v>
+      </c>
+    </row>
+    <row r="92" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R92" s="7">
+        <v>0.64904570666639028</v>
+      </c>
+      <c r="S92" s="4">
+        <f ca="1"/>
+        <v>0.93045439034459587</v>
+      </c>
+      <c r="T92" s="9">
+        <f ca="1"/>
+        <v>0.64904570666639028</v>
+      </c>
+    </row>
+    <row r="93" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R93" s="7">
+        <v>0.89299919543294648</v>
+      </c>
+      <c r="S93" s="4">
+        <f ca="1"/>
+        <v>0.947318592329083</v>
+      </c>
+      <c r="T93" s="9">
+        <f ca="1"/>
+        <v>0.89299919543294648</v>
+      </c>
+    </row>
+    <row r="94" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R94" s="7">
+        <v>0.98357223163047991</v>
+      </c>
+      <c r="S94" s="4">
+        <f ca="1"/>
+        <v>0.94876869372932582</v>
+      </c>
+      <c r="T94" s="9">
+        <f ca="1"/>
+        <v>0.98357223163047991</v>
+      </c>
+    </row>
+    <row r="95" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R95" s="7">
+        <v>0.95613469316823751</v>
+      </c>
+      <c r="S95" s="4">
+        <f ca="1"/>
+        <v>0.95613469316823751</v>
+      </c>
+      <c r="T95" s="9">
+        <f ca="1"/>
+        <v>0.95613469316823751</v>
+      </c>
+    </row>
+    <row r="96" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R96" s="7">
+        <v>0.97356891451331928</v>
+      </c>
+      <c r="S96" s="4">
+        <f ca="1"/>
+        <v>0.95887267917531893</v>
+      </c>
+      <c r="T96" s="9">
+        <f ca="1"/>
+        <v>0.97356891451331928</v>
+      </c>
+    </row>
+    <row r="97" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R97" s="7">
+        <v>0.64226730514312624</v>
+      </c>
+      <c r="S97" s="4">
+        <f ca="1"/>
+        <v>0.96328079049455895</v>
+      </c>
+      <c r="T97" s="9">
+        <f ca="1"/>
+        <v>0.64226730514312624</v>
+      </c>
+    </row>
+    <row r="98" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R98" s="7">
+        <v>0.61835596776400625</v>
+      </c>
+      <c r="S98" s="4">
+        <f ca="1"/>
+        <v>0.96985704312068066</v>
+      </c>
+      <c r="T98" s="9">
+        <f ca="1"/>
+        <v>0.61835596776400625</v>
+      </c>
+    </row>
+    <row r="99" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R99" s="7">
+        <v>0.86081826465673084</v>
+      </c>
+      <c r="S99" s="4">
+        <f ca="1"/>
+        <v>0.97062641299883634</v>
+      </c>
+      <c r="T99" s="9">
+        <f ca="1"/>
+        <v>0.86081826465673084</v>
+      </c>
+    </row>
+    <row r="100" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R100" s="7">
+        <v>0.16534127039316493</v>
+      </c>
+      <c r="S100" s="4">
+        <f ca="1"/>
+        <v>0.97078869366691067</v>
+      </c>
+      <c r="T100" s="9">
+        <f ca="1"/>
+        <v>0.16534127039316493</v>
+      </c>
+    </row>
+    <row r="101" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R101" s="7">
+        <v>0.9287334580292661</v>
+      </c>
+      <c r="S101" s="4">
+        <f ca="1"/>
+        <v>0.97356891451331928</v>
+      </c>
+      <c r="T101" s="9">
+        <f ca="1"/>
+        <v>0.9287334580292661</v>
+      </c>
+    </row>
+    <row r="102" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R102" s="7">
+        <v>8.9705088996498983E-3</v>
+      </c>
+      <c r="S102" s="4">
+        <f ca="1"/>
+        <v>0.98357223163047991</v>
+      </c>
+      <c r="T102" s="9">
+        <f ca="1"/>
+        <v>8.9705088996498983E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R103" s="7">
+        <v>0.30621594261281582</v>
+      </c>
+      <c r="S103" s="4">
+        <f ca="1"/>
+        <v>0.99561513362173215</v>
+      </c>
+      <c r="T103" s="9">
+        <f ca="1"/>
+        <v>0.30621594261281582</v>
+      </c>
+    </row>
+    <row r="104" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="R104" s="7">
+        <v>0.94876869372932582</v>
+      </c>
+      <c r="S104" s="4">
+        <f ca="1"/>
+        <v>0.99946735978378209</v>
+      </c>
+      <c r="T104" s="9">
+        <f ca="1"/>
+        <v>0.94876869372932582</v>
+      </c>
+    </row>
+    <row r="105" spans="18:20" x14ac:dyDescent="0.3">
+      <c r="S105" s="9"/>
+      <c r="T105" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* Add xloSplit function which reverses xloConcat. * In ExcelObj toX functions add support for default arguments * Add test for xloSplit
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CC06AF-02B6-44C8-92DC-395F95739B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C7FAC7-5305-4EDC-9E66-D6E464739DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="-108" windowWidth="22260" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
-    <sheet name="Concat" sheetId="2" r:id="rId2"/>
+    <sheet name="Concat-Split" sheetId="2" r:id="rId2"/>
     <sheet name="Sort" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>1, 2; 3, 4;</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>xloFillNA applied</t>
+  </si>
+  <si>
+    <t>xloSplit</t>
+  </si>
+  <si>
+    <t>Split string above on '-'</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +251,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -258,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -275,6 +287,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K14"/>
+  <dimension ref="B2:K23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1173,6 +1186,93 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="str">
+        <f t="array" ref="B21:H21">_xll.xloSplit(B14,"-")</f>
+        <v>Foo</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="F21" s="5" t="str">
+        <v>1.000000,2.000000,3.000000</v>
+      </c>
+      <c r="G21" s="5" t="str">
+        <v>Bar</v>
+      </c>
+      <c r="H21" s="5" t="str">
+        <v>Baz</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <f>I5</f>
+        <v>Foo</v>
+      </c>
+      <c r="C22" t="str">
+        <f>I6</f>
+        <v>Green</v>
+      </c>
+      <c r="D22" t="str">
+        <f>I7</f>
+        <v>Eggs</v>
+      </c>
+      <c r="E22" t="str">
+        <f>I8</f>
+        <v>Ham</v>
+      </c>
+      <c r="G22" t="str">
+        <f>J5</f>
+        <v>Bar</v>
+      </c>
+      <c r="H22" t="str">
+        <f>K5</f>
+        <v>Baz</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="16" t="b">
+        <f>B21=B22</f>
+        <v>1</v>
+      </c>
+      <c r="C23" s="16" t="b">
+        <f t="shared" ref="C23:H23" si="0">C21=C22</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1182,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:V105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1254,15 +1354,15 @@
       </c>
       <c r="R5" s="7">
         <f ca="1">RAND()</f>
-        <v>0.70995829035055502</v>
+        <v>0.1384070008738012</v>
       </c>
       <c r="S5" s="4">
         <f t="array" aca="1" ref="S5:S104" ca="1">_xll.xloSort(R5:R104,"a")</f>
         <v>4.4892519097212702E-3</v>
       </c>
-      <c r="T5">
+      <c r="T5" t="e">
         <f t="array" aca="1" ref="T5:T104" ca="1">_xll.xloBenchmarkSort(R5:R104)</f>
-        <v>4.4892519097212702E-3</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
@@ -1303,9 +1403,9 @@
         <f ca="1"/>
         <v>8.9705088996498983E-3</v>
       </c>
-      <c r="T6" s="9">
-        <f ca="1"/>
-        <v>1.4241351279182801E-2</v>
+      <c r="T6" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.3">
@@ -1343,9 +1443,9 @@
         <f ca="1"/>
         <v>1.0142003022623358E-2</v>
       </c>
-      <c r="T7" s="9">
-        <f ca="1"/>
-        <v>0.11987234330114915</v>
+      <c r="T7" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
@@ -1383,9 +1483,9 @@
         <f ca="1"/>
         <v>1.4241351279182801E-2</v>
       </c>
-      <c r="T8" s="9">
-        <f ca="1"/>
-        <v>0.43199912726020961</v>
+      <c r="T8" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
@@ -1423,9 +1523,9 @@
         <f ca="1"/>
         <v>1.7278225187227991E-2</v>
       </c>
-      <c r="T9" s="9">
-        <f ca="1"/>
-        <v>0.44362993322818001</v>
+      <c r="T9" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
@@ -1464,9 +1564,9 @@
         <f ca="1"/>
         <v>4.2989156379268589E-2</v>
       </c>
-      <c r="T10" s="9">
-        <f ca="1"/>
-        <v>0.70719203131190667</v>
+      <c r="T10" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
@@ -1505,9 +1605,9 @@
         <f ca="1"/>
         <v>4.8199686141203735E-2</v>
       </c>
-      <c r="T11" s="9">
-        <f ca="1"/>
-        <v>0.28303369927876221</v>
+      <c r="T11" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
@@ -1545,9 +1645,9 @@
         <f ca="1"/>
         <v>5.2437735118262885E-2</v>
       </c>
-      <c r="T12" s="9">
-        <f ca="1"/>
-        <v>0.18684151297687135</v>
+      <c r="T12" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
@@ -1567,9 +1667,9 @@
         <f ca="1"/>
         <v>6.063738431260568E-2</v>
       </c>
-      <c r="T13" s="9">
-        <f ca="1"/>
-        <v>7.6545233242765964E-2</v>
+      <c r="T13" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="14" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1596,9 +1696,9 @@
         <f ca="1"/>
         <v>7.6545233242765964E-2</v>
       </c>
-      <c r="T14" s="9">
-        <f ca="1"/>
-        <v>0.78402600397426425</v>
+      <c r="T14" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
@@ -1622,9 +1722,9 @@
         <f ca="1"/>
         <v>9.6043732044653662E-2</v>
       </c>
-      <c r="T15" s="9">
-        <f ca="1"/>
-        <v>0.5992299667126384</v>
+      <c r="T15" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.3">
@@ -1651,9 +1751,9 @@
         <f ca="1"/>
         <v>0.10466409270245647</v>
       </c>
-      <c r="T16" s="9">
-        <f ca="1"/>
-        <v>0.21129177216442607</v>
+      <c r="T16" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="17" spans="5:20" x14ac:dyDescent="0.3">
@@ -1686,9 +1786,9 @@
         <f ca="1"/>
         <v>0.11099657306935851</v>
       </c>
-      <c r="T17" s="9">
-        <f ca="1"/>
-        <v>0.56907031356613658</v>
+      <c r="T17" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="18" spans="5:20" x14ac:dyDescent="0.3">
@@ -1720,9 +1820,9 @@
         <f ca="1"/>
         <v>0.11987234330114915</v>
       </c>
-      <c r="T18" s="9">
-        <f ca="1"/>
-        <v>0.70052257146975117</v>
+      <c r="T18" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="19" spans="5:20" x14ac:dyDescent="0.3">
@@ -1743,11 +1843,11 @@
       </c>
       <c r="S19" s="4">
         <f ca="1"/>
-        <v>0.15138392223952224</v>
-      </c>
-      <c r="T19" s="9">
-        <f ca="1"/>
-        <v>0.96985704312068066</v>
+        <v>0.1384070008738012</v>
+      </c>
+      <c r="T19" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="20" spans="5:20" x14ac:dyDescent="0.3">
@@ -1768,11 +1868,11 @@
       </c>
       <c r="S20" s="4">
         <f ca="1"/>
-        <v>0.15285256271102787</v>
-      </c>
-      <c r="T20" s="9">
-        <f ca="1"/>
-        <v>0.55553726039846762</v>
+        <v>0.15138392223952224</v>
+      </c>
+      <c r="T20" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="21" spans="5:20" x14ac:dyDescent="0.3">
@@ -1793,11 +1893,11 @@
       </c>
       <c r="S21" s="4">
         <f ca="1"/>
-        <v>0.15935651729819933</v>
-      </c>
-      <c r="T21" s="9">
-        <f ca="1"/>
-        <v>0.346644941363903</v>
+        <v>0.15285256271102787</v>
+      </c>
+      <c r="T21" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="22" spans="5:20" x14ac:dyDescent="0.3">
@@ -1818,11 +1918,11 @@
       </c>
       <c r="S22" s="4">
         <f ca="1"/>
-        <v>0.16534127039316493</v>
-      </c>
-      <c r="T22" s="9">
-        <f ca="1"/>
-        <v>0.86284631971635639</v>
+        <v>0.15935651729819933</v>
+      </c>
+      <c r="T22" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="23" spans="5:20" x14ac:dyDescent="0.3">
@@ -1843,11 +1943,11 @@
       </c>
       <c r="S23" s="4">
         <f ca="1"/>
-        <v>0.18684151297687135</v>
-      </c>
-      <c r="T23" s="9">
-        <f ca="1"/>
-        <v>0.25958386357364216</v>
+        <v>0.16534127039316493</v>
+      </c>
+      <c r="T23" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="24" spans="5:20" x14ac:dyDescent="0.3">
@@ -1856,11 +1956,11 @@
       </c>
       <c r="S24" s="4">
         <f ca="1"/>
-        <v>0.19150797219437865</v>
-      </c>
-      <c r="T24" s="9">
-        <f ca="1"/>
-        <v>0.44578595954200495</v>
+        <v>0.18684151297687135</v>
+      </c>
+      <c r="T24" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="25" spans="5:20" x14ac:dyDescent="0.3">
@@ -1869,11 +1969,11 @@
       </c>
       <c r="S25" s="4">
         <f ca="1"/>
-        <v>0.19332448079141096</v>
-      </c>
-      <c r="T25" s="9">
-        <f ca="1"/>
-        <v>0.35070608842246354</v>
+        <v>0.19150797219437865</v>
+      </c>
+      <c r="T25" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="26" spans="5:20" x14ac:dyDescent="0.3">
@@ -1882,11 +1982,11 @@
       </c>
       <c r="S26" s="4">
         <f ca="1"/>
-        <v>0.20455886903305909</v>
-      </c>
-      <c r="T26" s="9">
-        <f ca="1"/>
-        <v>0.97062641299883634</v>
+        <v>0.19332448079141096</v>
+      </c>
+      <c r="T26" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="27" spans="5:20" x14ac:dyDescent="0.3">
@@ -1895,11 +1995,11 @@
       </c>
       <c r="S27" s="4">
         <f ca="1"/>
-        <v>0.21129177216442607</v>
-      </c>
-      <c r="T27" s="9">
-        <f ca="1"/>
-        <v>0.36303952239766712</v>
+        <v>0.20455886903305909</v>
+      </c>
+      <c r="T27" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="28" spans="5:20" x14ac:dyDescent="0.3">
@@ -1908,11 +2008,11 @@
       </c>
       <c r="S28" s="4">
         <f ca="1"/>
-        <v>0.21289020404938441</v>
-      </c>
-      <c r="T28" s="9">
-        <f ca="1"/>
-        <v>0.35500379302962237</v>
+        <v>0.21129177216442607</v>
+      </c>
+      <c r="T28" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="29" spans="5:20" x14ac:dyDescent="0.3">
@@ -1921,11 +2021,11 @@
       </c>
       <c r="S29" s="4">
         <f ca="1"/>
-        <v>0.24005046089105242</v>
-      </c>
-      <c r="T29" s="9">
-        <f ca="1"/>
-        <v>0.30991009987247375</v>
+        <v>0.21289020404938441</v>
+      </c>
+      <c r="T29" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="30" spans="5:20" x14ac:dyDescent="0.3">
@@ -1934,11 +2034,11 @@
       </c>
       <c r="S30" s="4">
         <f ca="1"/>
-        <v>0.24683784713265966</v>
-      </c>
-      <c r="T30" s="9">
-        <f ca="1"/>
-        <v>0.50309865693105404</v>
+        <v>0.24005046089105242</v>
+      </c>
+      <c r="T30" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="31" spans="5:20" x14ac:dyDescent="0.3">
@@ -1947,11 +2047,11 @@
       </c>
       <c r="S31" s="4">
         <f ca="1"/>
-        <v>0.25090708805825079</v>
-      </c>
-      <c r="T31" s="9">
-        <f ca="1"/>
         <v>0.24683784713265966</v>
+      </c>
+      <c r="T31" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="32" spans="5:20" x14ac:dyDescent="0.3">
@@ -1960,11 +2060,11 @@
       </c>
       <c r="S32" s="4">
         <f ca="1"/>
-        <v>0.25958386357364216</v>
-      </c>
-      <c r="T32" s="9">
-        <f ca="1"/>
-        <v>0.21289020404938441</v>
+        <v>0.25090708805825079</v>
+      </c>
+      <c r="T32" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="33" spans="18:20" x14ac:dyDescent="0.3">
@@ -1973,11 +2073,11 @@
       </c>
       <c r="S33" s="4">
         <f ca="1"/>
-        <v>0.26026766796149603</v>
-      </c>
-      <c r="T33" s="9">
-        <f ca="1"/>
-        <v>0.57712158377157863</v>
+        <v>0.25958386357364216</v>
+      </c>
+      <c r="T33" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="34" spans="18:20" x14ac:dyDescent="0.3">
@@ -1986,11 +2086,11 @@
       </c>
       <c r="S34" s="4">
         <f ca="1"/>
-        <v>0.2819709570143808</v>
-      </c>
-      <c r="T34" s="9">
-        <f ca="1"/>
-        <v>6.063738431260568E-2</v>
+        <v>0.26026766796149603</v>
+      </c>
+      <c r="T34" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="35" spans="18:20" x14ac:dyDescent="0.3">
@@ -1999,11 +2099,11 @@
       </c>
       <c r="S35" s="4">
         <f ca="1"/>
-        <v>0.28303369927876221</v>
-      </c>
-      <c r="T35" s="9">
-        <f ca="1"/>
-        <v>0.37822251634842252</v>
+        <v>0.2819709570143808</v>
+      </c>
+      <c r="T35" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="36" spans="18:20" x14ac:dyDescent="0.3">
@@ -2012,11 +2112,11 @@
       </c>
       <c r="S36" s="4">
         <f ca="1"/>
-        <v>0.29579294051174709</v>
-      </c>
-      <c r="T36" s="9">
-        <f ca="1"/>
-        <v>0.60977631212733274</v>
+        <v>0.28303369927876221</v>
+      </c>
+      <c r="T36" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="37" spans="18:20" x14ac:dyDescent="0.3">
@@ -2025,11 +2125,11 @@
       </c>
       <c r="S37" s="4">
         <f ca="1"/>
-        <v>0.30621594261281582</v>
-      </c>
-      <c r="T37" s="9">
-        <f ca="1"/>
-        <v>0.20455886903305909</v>
+        <v>0.29579294051174709</v>
+      </c>
+      <c r="T37" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="38" spans="18:20" x14ac:dyDescent="0.3">
@@ -2038,11 +2138,11 @@
       </c>
       <c r="S38" s="4">
         <f ca="1"/>
-        <v>0.30699880764121135</v>
-      </c>
-      <c r="T38" s="9">
-        <f ca="1"/>
-        <v>0.947318592329083</v>
+        <v>0.30621594261281582</v>
+      </c>
+      <c r="T38" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="39" spans="18:20" x14ac:dyDescent="0.3">
@@ -2051,11 +2151,11 @@
       </c>
       <c r="S39" s="4">
         <f ca="1"/>
-        <v>0.30746381468864881</v>
-      </c>
-      <c r="T39" s="9">
-        <f ca="1"/>
-        <v>0.68147699048550281</v>
+        <v>0.30699880764121135</v>
+      </c>
+      <c r="T39" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="40" spans="18:20" x14ac:dyDescent="0.3">
@@ -2064,11 +2164,11 @@
       </c>
       <c r="S40" s="4">
         <f ca="1"/>
-        <v>0.30991009987247375</v>
-      </c>
-      <c r="T40" s="9">
-        <f ca="1"/>
-        <v>0.90600850571232516</v>
+        <v>0.30746381468864881</v>
+      </c>
+      <c r="T40" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="41" spans="18:20" x14ac:dyDescent="0.3">
@@ -2077,11 +2177,11 @@
       </c>
       <c r="S41" s="4">
         <f ca="1"/>
-        <v>0.34322350221251363</v>
-      </c>
-      <c r="T41" s="9">
-        <f ca="1"/>
-        <v>0.85960749899325406</v>
+        <v>0.30991009987247375</v>
+      </c>
+      <c r="T41" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="42" spans="18:20" x14ac:dyDescent="0.3">
@@ -2090,11 +2190,11 @@
       </c>
       <c r="S42" s="4">
         <f ca="1"/>
-        <v>0.346644941363903</v>
-      </c>
-      <c r="T42" s="9">
-        <f ca="1"/>
-        <v>4.2989156379268589E-2</v>
+        <v>0.34322350221251363</v>
+      </c>
+      <c r="T42" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="43" spans="18:20" x14ac:dyDescent="0.3">
@@ -2103,11 +2203,11 @@
       </c>
       <c r="S43" s="4">
         <f ca="1"/>
-        <v>0.35070608842246354</v>
-      </c>
-      <c r="T43" s="9">
-        <f ca="1"/>
-        <v>0.15285256271102787</v>
+        <v>0.346644941363903</v>
+      </c>
+      <c r="T43" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="44" spans="18:20" x14ac:dyDescent="0.3">
@@ -2116,11 +2216,11 @@
       </c>
       <c r="S44" s="4">
         <f ca="1"/>
-        <v>0.35500379302962237</v>
-      </c>
-      <c r="T44" s="9">
-        <f ca="1"/>
-        <v>4.4892519097212702E-3</v>
+        <v>0.35070608842246354</v>
+      </c>
+      <c r="T44" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="45" spans="18:20" x14ac:dyDescent="0.3">
@@ -2129,11 +2229,11 @@
       </c>
       <c r="S45" s="4">
         <f ca="1"/>
-        <v>0.36303952239766712</v>
-      </c>
-      <c r="T45" s="9">
-        <f ca="1"/>
-        <v>9.6043732044653662E-2</v>
+        <v>0.35500379302962237</v>
+      </c>
+      <c r="T45" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="46" spans="18:20" x14ac:dyDescent="0.3">
@@ -2142,11 +2242,11 @@
       </c>
       <c r="S46" s="4">
         <f ca="1"/>
-        <v>0.37590154211670712</v>
-      </c>
-      <c r="T46" s="9">
-        <f ca="1"/>
-        <v>0.30746381468864881</v>
+        <v>0.36303952239766712</v>
+      </c>
+      <c r="T46" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="47" spans="18:20" x14ac:dyDescent="0.3">
@@ -2155,11 +2255,11 @@
       </c>
       <c r="S47" s="4">
         <f ca="1"/>
-        <v>0.37822251634842252</v>
-      </c>
-      <c r="T47" s="9">
-        <f ca="1"/>
-        <v>0.15935651729819933</v>
+        <v>0.37590154211670712</v>
+      </c>
+      <c r="T47" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="48" spans="18:20" x14ac:dyDescent="0.3">
@@ -2168,11 +2268,11 @@
       </c>
       <c r="S48" s="4">
         <f ca="1"/>
-        <v>0.38122419173045929</v>
-      </c>
-      <c r="T48" s="9">
-        <f ca="1"/>
-        <v>0.73492497530386436</v>
+        <v>0.37822251634842252</v>
+      </c>
+      <c r="T48" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="49" spans="18:20" x14ac:dyDescent="0.3">
@@ -2181,11 +2281,11 @@
       </c>
       <c r="S49" s="4">
         <f ca="1"/>
-        <v>0.38693032613344891</v>
-      </c>
-      <c r="T49" s="9">
-        <f ca="1"/>
-        <v>0.93045439034459587</v>
+        <v>0.38122419173045929</v>
+      </c>
+      <c r="T49" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="50" spans="18:20" x14ac:dyDescent="0.3">
@@ -2194,11 +2294,11 @@
       </c>
       <c r="S50" s="4">
         <f ca="1"/>
-        <v>0.38924117354343202</v>
-      </c>
-      <c r="T50" s="9">
-        <f ca="1"/>
-        <v>0.70064205520622802</v>
+        <v>0.38693032613344891</v>
+      </c>
+      <c r="T50" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="51" spans="18:20" x14ac:dyDescent="0.3">
@@ -2207,11 +2307,11 @@
       </c>
       <c r="S51" s="4">
         <f ca="1"/>
-        <v>0.41032128248045219</v>
-      </c>
-      <c r="T51" s="9">
-        <f ca="1"/>
-        <v>0.34322350221251363</v>
+        <v>0.38924117354343202</v>
+      </c>
+      <c r="T51" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="52" spans="18:20" x14ac:dyDescent="0.3">
@@ -2220,11 +2320,11 @@
       </c>
       <c r="S52" s="4">
         <f ca="1"/>
-        <v>0.43199912726020961</v>
-      </c>
-      <c r="T52" s="9">
-        <f ca="1"/>
-        <v>0.30699880764121135</v>
+        <v>0.41032128248045219</v>
+      </c>
+      <c r="T52" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="53" spans="18:20" x14ac:dyDescent="0.3">
@@ -2233,11 +2333,11 @@
       </c>
       <c r="S53" s="4">
         <f ca="1"/>
-        <v>0.44362993322818001</v>
-      </c>
-      <c r="T53" s="9">
-        <f ca="1"/>
-        <v>0.56072877256876819</v>
+        <v>0.43199912726020961</v>
+      </c>
+      <c r="T53" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="54" spans="18:20" x14ac:dyDescent="0.3">
@@ -2246,11 +2346,11 @@
       </c>
       <c r="S54" s="4">
         <f ca="1"/>
-        <v>0.44578595954200495</v>
-      </c>
-      <c r="T54" s="9">
-        <f ca="1"/>
-        <v>1.0142003022623358E-2</v>
+        <v>0.44362993322818001</v>
+      </c>
+      <c r="T54" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="55" spans="18:20" x14ac:dyDescent="0.3">
@@ -2259,11 +2359,11 @@
       </c>
       <c r="S55" s="4">
         <f ca="1"/>
-        <v>0.50309865693105404</v>
-      </c>
-      <c r="T55" s="9">
-        <f ca="1"/>
-        <v>0.38122419173045929</v>
+        <v>0.44578595954200495</v>
+      </c>
+      <c r="T55" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="56" spans="18:20" x14ac:dyDescent="0.3">
@@ -2272,11 +2372,11 @@
       </c>
       <c r="S56" s="4">
         <f ca="1"/>
-        <v>0.55553726039846762</v>
-      </c>
-      <c r="T56" s="9">
-        <f ca="1"/>
-        <v>0.60411978716231773</v>
+        <v>0.50309865693105404</v>
+      </c>
+      <c r="T56" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="57" spans="18:20" x14ac:dyDescent="0.3">
@@ -2285,11 +2385,11 @@
       </c>
       <c r="S57" s="4">
         <f ca="1"/>
-        <v>0.56072877256876819</v>
-      </c>
-      <c r="T57" s="9">
-        <f ca="1"/>
-        <v>0.2819709570143808</v>
+        <v>0.55553726039846762</v>
+      </c>
+      <c r="T57" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="58" spans="18:20" x14ac:dyDescent="0.3">
@@ -2298,11 +2398,11 @@
       </c>
       <c r="S58" s="4">
         <f ca="1"/>
-        <v>0.56613202852270661</v>
-      </c>
-      <c r="T58" s="9">
-        <f ca="1"/>
-        <v>0.58507289523339523</v>
+        <v>0.56072877256876819</v>
+      </c>
+      <c r="T58" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="59" spans="18:20" x14ac:dyDescent="0.3">
@@ -2311,11 +2411,11 @@
       </c>
       <c r="S59" s="4">
         <f ca="1"/>
-        <v>0.56907031356613658</v>
-      </c>
-      <c r="T59" s="9">
-        <f ca="1"/>
-        <v>0.38693032613344891</v>
+        <v>0.56613202852270661</v>
+      </c>
+      <c r="T59" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="60" spans="18:20" x14ac:dyDescent="0.3">
@@ -2324,11 +2424,11 @@
       </c>
       <c r="S60" s="4">
         <f ca="1"/>
-        <v>0.57665750527755044</v>
-      </c>
-      <c r="T60" s="9">
-        <f ca="1"/>
-        <v>0.38924117354343202</v>
+        <v>0.56907031356613658</v>
+      </c>
+      <c r="T60" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="61" spans="18:20" x14ac:dyDescent="0.3">
@@ -2337,11 +2437,11 @@
       </c>
       <c r="S61" s="4">
         <f ca="1"/>
-        <v>0.57712158377157863</v>
-      </c>
-      <c r="T61" s="9">
-        <f ca="1"/>
-        <v>0.25090708805825079</v>
+        <v>0.57665750527755044</v>
+      </c>
+      <c r="T61" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="62" spans="18:20" x14ac:dyDescent="0.3">
@@ -2350,11 +2450,11 @@
       </c>
       <c r="S62" s="4">
         <f ca="1"/>
-        <v>0.58507289523339523</v>
-      </c>
-      <c r="T62" s="9">
-        <f ca="1"/>
-        <v>0.99561513362173215</v>
+        <v>0.57712158377157863</v>
+      </c>
+      <c r="T62" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="63" spans="18:20" x14ac:dyDescent="0.3">
@@ -2363,11 +2463,11 @@
       </c>
       <c r="S63" s="4">
         <f ca="1"/>
-        <v>0.5992299667126384</v>
-      </c>
-      <c r="T63" s="9">
-        <f ca="1"/>
-        <v>0.41032128248045219</v>
+        <v>0.58507289523339523</v>
+      </c>
+      <c r="T63" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="64" spans="18:20" x14ac:dyDescent="0.3">
@@ -2376,11 +2476,11 @@
       </c>
       <c r="S64" s="4">
         <f ca="1"/>
-        <v>0.60411978716231773</v>
-      </c>
-      <c r="T64" s="9">
-        <f ca="1"/>
-        <v>0.10466409270245647</v>
+        <v>0.5992299667126384</v>
+      </c>
+      <c r="T64" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="65" spans="18:20" x14ac:dyDescent="0.3">
@@ -2389,11 +2489,11 @@
       </c>
       <c r="S65" s="4">
         <f ca="1"/>
-        <v>0.60977631212733274</v>
-      </c>
-      <c r="T65" s="9">
-        <f ca="1"/>
-        <v>0.96328079049455895</v>
+        <v>0.60411978716231773</v>
+      </c>
+      <c r="T65" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="66" spans="18:20" x14ac:dyDescent="0.3">
@@ -2402,11 +2502,11 @@
       </c>
       <c r="S66" s="4">
         <f ca="1"/>
-        <v>0.61835596776400625</v>
-      </c>
-      <c r="T66" s="9">
-        <f ca="1"/>
-        <v>0.99946735978378209</v>
+        <v>0.60977631212733274</v>
+      </c>
+      <c r="T66" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="67" spans="18:20" x14ac:dyDescent="0.3">
@@ -2415,11 +2515,11 @@
       </c>
       <c r="S67" s="4">
         <f ca="1"/>
-        <v>0.64226730514312624</v>
-      </c>
-      <c r="T67" s="9">
-        <f ca="1"/>
-        <v>0.82935893028115659</v>
+        <v>0.61835596776400625</v>
+      </c>
+      <c r="T67" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="68" spans="18:20" x14ac:dyDescent="0.3">
@@ -2428,11 +2528,11 @@
       </c>
       <c r="S68" s="4">
         <f ca="1"/>
-        <v>0.64904570666639028</v>
-      </c>
-      <c r="T68" s="9">
-        <f ca="1"/>
-        <v>0.15138392223952224</v>
+        <v>0.64226730514312624</v>
+      </c>
+      <c r="T68" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="69" spans="18:20" x14ac:dyDescent="0.3">
@@ -2441,11 +2541,11 @@
       </c>
       <c r="S69" s="4">
         <f ca="1"/>
-        <v>0.67056525021684998</v>
-      </c>
-      <c r="T69" s="9">
-        <f ca="1"/>
-        <v>0.26026766796149603</v>
+        <v>0.64904570666639028</v>
+      </c>
+      <c r="T69" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="70" spans="18:20" x14ac:dyDescent="0.3">
@@ -2454,11 +2554,11 @@
       </c>
       <c r="S70" s="4">
         <f ca="1"/>
-        <v>0.68147699048550281</v>
-      </c>
-      <c r="T70" s="9">
-        <f ca="1"/>
-        <v>0.56613202852270661</v>
+        <v>0.67056525021684998</v>
+      </c>
+      <c r="T70" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="71" spans="18:20" x14ac:dyDescent="0.3">
@@ -2467,11 +2567,11 @@
       </c>
       <c r="S71" s="4">
         <f ca="1"/>
-        <v>0.70052257146975117</v>
-      </c>
-      <c r="T71" s="9">
-        <f ca="1"/>
-        <v>0.57665750527755044</v>
+        <v>0.68147699048550281</v>
+      </c>
+      <c r="T71" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="72" spans="18:20" x14ac:dyDescent="0.3">
@@ -2480,11 +2580,11 @@
       </c>
       <c r="S72" s="4">
         <f ca="1"/>
-        <v>0.70064205520622802</v>
-      </c>
-      <c r="T72" s="9">
-        <f ca="1"/>
-        <v>0.83938605783476394</v>
+        <v>0.70052257146975117</v>
+      </c>
+      <c r="T72" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="73" spans="18:20" x14ac:dyDescent="0.3">
@@ -2493,11 +2593,11 @@
       </c>
       <c r="S73" s="4">
         <f ca="1"/>
-        <v>0.70719203131190667</v>
-      </c>
-      <c r="T73" s="9">
-        <f ca="1"/>
-        <v>0.37590154211670712</v>
+        <v>0.70064205520622802</v>
+      </c>
+      <c r="T73" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="74" spans="18:20" x14ac:dyDescent="0.3">
@@ -2506,11 +2606,11 @@
       </c>
       <c r="S74" s="4">
         <f ca="1"/>
-        <v>0.70995829035055502</v>
-      </c>
-      <c r="T74" s="9">
-        <f ca="1"/>
-        <v>0.95887267917531893</v>
+        <v>0.70719203131190667</v>
+      </c>
+      <c r="T74" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="75" spans="18:20" x14ac:dyDescent="0.3">
@@ -2521,9 +2621,9 @@
         <f ca="1"/>
         <v>0.71755405184921206</v>
       </c>
-      <c r="T75" s="9">
-        <f ca="1"/>
-        <v>0.11099657306935851</v>
+      <c r="T75" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="76" spans="18:20" x14ac:dyDescent="0.3">
@@ -2534,9 +2634,9 @@
         <f ca="1"/>
         <v>0.73492497530386436</v>
       </c>
-      <c r="T76" s="9">
-        <f ca="1"/>
-        <v>0.67056525021684998</v>
+      <c r="T76" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="77" spans="18:20" x14ac:dyDescent="0.3">
@@ -2547,9 +2647,9 @@
         <f ca="1"/>
         <v>0.78402600397426425</v>
       </c>
-      <c r="T77" s="9">
-        <f ca="1"/>
-        <v>0.82167610222353549</v>
+      <c r="T77" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="78" spans="18:20" x14ac:dyDescent="0.3">
@@ -2560,9 +2660,9 @@
         <f ca="1"/>
         <v>0.79404440245310404</v>
       </c>
-      <c r="T78" s="9">
-        <f ca="1"/>
-        <v>0.79626472404113779</v>
+      <c r="T78" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="79" spans="18:20" x14ac:dyDescent="0.3">
@@ -2573,9 +2673,9 @@
         <f ca="1"/>
         <v>0.79626472404113779</v>
       </c>
-      <c r="T79" s="9">
-        <f ca="1"/>
-        <v>0.79404440245310404</v>
+      <c r="T79" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="80" spans="18:20" x14ac:dyDescent="0.3">
@@ -2586,9 +2686,9 @@
         <f ca="1"/>
         <v>0.79852373727417758</v>
       </c>
-      <c r="T80" s="9">
-        <f ca="1"/>
-        <v>0.24005046089105242</v>
+      <c r="T80" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="81" spans="18:20" x14ac:dyDescent="0.3">
@@ -2599,9 +2699,9 @@
         <f ca="1"/>
         <v>0.82167610222353549</v>
       </c>
-      <c r="T81" s="9">
-        <f ca="1"/>
-        <v>1.7278225187227991E-2</v>
+      <c r="T81" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="82" spans="18:20" x14ac:dyDescent="0.3">
@@ -2612,9 +2712,9 @@
         <f ca="1"/>
         <v>0.82935893028115659</v>
       </c>
-      <c r="T82" s="9">
-        <f ca="1"/>
-        <v>0.83233289115523368</v>
+      <c r="T82" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="83" spans="18:20" x14ac:dyDescent="0.3">
@@ -2625,9 +2725,9 @@
         <f ca="1"/>
         <v>0.83233289115523368</v>
       </c>
-      <c r="T83" s="9">
-        <f ca="1"/>
-        <v>5.2437735118262885E-2</v>
+      <c r="T83" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="84" spans="18:20" x14ac:dyDescent="0.3">
@@ -2638,9 +2738,9 @@
         <f ca="1"/>
         <v>0.83938605783476394</v>
       </c>
-      <c r="T84" s="9">
-        <f ca="1"/>
-        <v>0.79852373727417758</v>
+      <c r="T84" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="85" spans="18:20" x14ac:dyDescent="0.3">
@@ -2651,9 +2751,9 @@
         <f ca="1"/>
         <v>0.85960749899325406</v>
       </c>
-      <c r="T85" s="9">
-        <f ca="1"/>
-        <v>0.88056162198032462</v>
+      <c r="T85" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="86" spans="18:20" x14ac:dyDescent="0.3">
@@ -2664,9 +2764,9 @@
         <f ca="1"/>
         <v>0.86081826465673084</v>
       </c>
-      <c r="T86" s="9">
-        <f ca="1"/>
-        <v>0.29579294051174709</v>
+      <c r="T86" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="87" spans="18:20" x14ac:dyDescent="0.3">
@@ -2677,9 +2777,9 @@
         <f ca="1"/>
         <v>0.86284631971635639</v>
       </c>
-      <c r="T87" s="9">
-        <f ca="1"/>
-        <v>0.71755405184921206</v>
+      <c r="T87" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="88" spans="18:20" x14ac:dyDescent="0.3">
@@ -2690,9 +2790,9 @@
         <f ca="1"/>
         <v>0.88056162198032462</v>
       </c>
-      <c r="T88" s="9">
-        <f ca="1"/>
-        <v>0.97078869366691067</v>
+      <c r="T88" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="89" spans="18:20" x14ac:dyDescent="0.3">
@@ -2703,9 +2803,9 @@
         <f ca="1"/>
         <v>0.89299919543294648</v>
       </c>
-      <c r="T89" s="9">
-        <f ca="1"/>
-        <v>4.8199686141203735E-2</v>
+      <c r="T89" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="90" spans="18:20" x14ac:dyDescent="0.3">
@@ -2716,9 +2816,9 @@
         <f ca="1"/>
         <v>0.90600850571232516</v>
       </c>
-      <c r="T90" s="9">
-        <f ca="1"/>
-        <v>0.19150797219437865</v>
+      <c r="T90" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="91" spans="18:20" x14ac:dyDescent="0.3">
@@ -2729,9 +2829,9 @@
         <f ca="1"/>
         <v>0.9287334580292661</v>
       </c>
-      <c r="T91" s="9">
-        <f ca="1"/>
-        <v>0.19332448079141096</v>
+      <c r="T91" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="92" spans="18:20" x14ac:dyDescent="0.3">
@@ -2742,9 +2842,9 @@
         <f ca="1"/>
         <v>0.93045439034459587</v>
       </c>
-      <c r="T92" s="9">
-        <f ca="1"/>
-        <v>0.64904570666639028</v>
+      <c r="T92" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="93" spans="18:20" x14ac:dyDescent="0.3">
@@ -2755,9 +2855,9 @@
         <f ca="1"/>
         <v>0.947318592329083</v>
       </c>
-      <c r="T93" s="9">
-        <f ca="1"/>
-        <v>0.89299919543294648</v>
+      <c r="T93" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="94" spans="18:20" x14ac:dyDescent="0.3">
@@ -2768,9 +2868,9 @@
         <f ca="1"/>
         <v>0.94876869372932582</v>
       </c>
-      <c r="T94" s="9">
-        <f ca="1"/>
-        <v>0.98357223163047991</v>
+      <c r="T94" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="95" spans="18:20" x14ac:dyDescent="0.3">
@@ -2781,9 +2881,9 @@
         <f ca="1"/>
         <v>0.95613469316823751</v>
       </c>
-      <c r="T95" s="9">
-        <f ca="1"/>
-        <v>0.95613469316823751</v>
+      <c r="T95" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="96" spans="18:20" x14ac:dyDescent="0.3">
@@ -2794,9 +2894,9 @@
         <f ca="1"/>
         <v>0.95887267917531893</v>
       </c>
-      <c r="T96" s="9">
-        <f ca="1"/>
-        <v>0.97356891451331928</v>
+      <c r="T96" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="97" spans="18:20" x14ac:dyDescent="0.3">
@@ -2807,9 +2907,9 @@
         <f ca="1"/>
         <v>0.96328079049455895</v>
       </c>
-      <c r="T97" s="9">
-        <f ca="1"/>
-        <v>0.64226730514312624</v>
+      <c r="T97" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="98" spans="18:20" x14ac:dyDescent="0.3">
@@ -2820,9 +2920,9 @@
         <f ca="1"/>
         <v>0.96985704312068066</v>
       </c>
-      <c r="T98" s="9">
-        <f ca="1"/>
-        <v>0.61835596776400625</v>
+      <c r="T98" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="99" spans="18:20" x14ac:dyDescent="0.3">
@@ -2833,9 +2933,9 @@
         <f ca="1"/>
         <v>0.97062641299883634</v>
       </c>
-      <c r="T99" s="9">
-        <f ca="1"/>
-        <v>0.86081826465673084</v>
+      <c r="T99" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="100" spans="18:20" x14ac:dyDescent="0.3">
@@ -2846,9 +2946,9 @@
         <f ca="1"/>
         <v>0.97078869366691067</v>
       </c>
-      <c r="T100" s="9">
-        <f ca="1"/>
-        <v>0.16534127039316493</v>
+      <c r="T100" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="101" spans="18:20" x14ac:dyDescent="0.3">
@@ -2859,9 +2959,9 @@
         <f ca="1"/>
         <v>0.97356891451331928</v>
       </c>
-      <c r="T101" s="9">
-        <f ca="1"/>
-        <v>0.9287334580292661</v>
+      <c r="T101" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="102" spans="18:20" x14ac:dyDescent="0.3">
@@ -2872,9 +2972,9 @@
         <f ca="1"/>
         <v>0.98357223163047991</v>
       </c>
-      <c r="T102" s="9">
-        <f ca="1"/>
-        <v>8.9705088996498983E-3</v>
+      <c r="T102" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="103" spans="18:20" x14ac:dyDescent="0.3">
@@ -2885,9 +2985,9 @@
         <f ca="1"/>
         <v>0.99561513362173215</v>
       </c>
-      <c r="T103" s="9">
-        <f ca="1"/>
-        <v>0.30621594261281582</v>
+      <c r="T103" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="104" spans="18:20" x14ac:dyDescent="0.3">
@@ -2898,9 +2998,9 @@
         <f ca="1"/>
         <v>0.99946735978378209</v>
       </c>
-      <c r="T104" s="9">
-        <f ca="1"/>
-        <v>0.94876869372932582</v>
+      <c r="T104" s="9" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="105" spans="18:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
* Much cleaner syntax for writing to ExcelArrayBuilder. I think it should resolve to the same code...! * Sort out some of the type mess in ExcelObj and make c'tors explicit to prevent accidents. * Fix small memory leak in numpy string array handling. * Add xloPad function to ensure arrays are at least 2x2 to stop Excel's fill behaviour. * Add default sort in xloSort * Update tests
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C7FAC7-5305-4EDC-9E66-D6E464739DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D53C4D-33A7-46FF-AC66-13078E028B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Sort" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1077,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,7 +1178,7 @@
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="str">
         <f>_xll.xloConcat("---", I5:I8, _xll.xloConcat(",",J6:J8),J5:K5)</f>
-        <v>Foo---Green---Eggs---Ham---1.000000,2.000000,3.000000---Bar---Baz</v>
+        <v>Foo---Green---Eggs---Ham---1---Bar---Baz</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1198,7 +1199,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="str">
-        <f t="array" ref="B21:H21">_xll.xloSplit(B14,"-")</f>
+        <f t="array" ref="B21:H21">TRANSPOSE(_xll.xloSplit(B14,"-"))</f>
         <v>Foo</v>
       </c>
       <c r="C21" s="5" t="str">
@@ -1211,7 +1212,7 @@
         <v>Ham</v>
       </c>
       <c r="F21" s="5" t="str">
-        <v>1.000000,2.000000,3.000000</v>
+        <v>1</v>
       </c>
       <c r="G21" s="5" t="str">
         <v>Bar</v>
@@ -1354,7 +1355,7 @@
       </c>
       <c r="R5" s="7">
         <f ca="1">RAND()</f>
-        <v>0.1384070008738012</v>
+        <v>0.63120330732006702</v>
       </c>
       <c r="S5" s="4">
         <f t="array" aca="1" ref="S5:S104" ca="1">_xll.xloSort(R5:R104,"a")</f>
@@ -1843,7 +1844,7 @@
       </c>
       <c r="S19" s="4">
         <f ca="1"/>
-        <v>0.1384070008738012</v>
+        <v>0.15138392223952224</v>
       </c>
       <c r="T19" s="9" t="e">
         <f ca="1"/>
@@ -1868,7 +1869,7 @@
       </c>
       <c r="S20" s="4">
         <f ca="1"/>
-        <v>0.15138392223952224</v>
+        <v>0.15285256271102787</v>
       </c>
       <c r="T20" s="9" t="e">
         <f ca="1"/>
@@ -1893,7 +1894,7 @@
       </c>
       <c r="S21" s="4">
         <f ca="1"/>
-        <v>0.15285256271102787</v>
+        <v>0.15935651729819933</v>
       </c>
       <c r="T21" s="9" t="e">
         <f ca="1"/>
@@ -1918,7 +1919,7 @@
       </c>
       <c r="S22" s="4">
         <f ca="1"/>
-        <v>0.15935651729819933</v>
+        <v>0.16534127039316493</v>
       </c>
       <c r="T22" s="9" t="e">
         <f ca="1"/>
@@ -1943,7 +1944,7 @@
       </c>
       <c r="S23" s="4">
         <f ca="1"/>
-        <v>0.16534127039316493</v>
+        <v>0.18684151297687135</v>
       </c>
       <c r="T23" s="9" t="e">
         <f ca="1"/>
@@ -1956,7 +1957,7 @@
       </c>
       <c r="S24" s="4">
         <f ca="1"/>
-        <v>0.18684151297687135</v>
+        <v>0.19150797219437865</v>
       </c>
       <c r="T24" s="9" t="e">
         <f ca="1"/>
@@ -1969,7 +1970,7 @@
       </c>
       <c r="S25" s="4">
         <f ca="1"/>
-        <v>0.19150797219437865</v>
+        <v>0.19332448079141096</v>
       </c>
       <c r="T25" s="9" t="e">
         <f ca="1"/>
@@ -1982,7 +1983,7 @@
       </c>
       <c r="S26" s="4">
         <f ca="1"/>
-        <v>0.19332448079141096</v>
+        <v>0.20455886903305909</v>
       </c>
       <c r="T26" s="9" t="e">
         <f ca="1"/>
@@ -1995,7 +1996,7 @@
       </c>
       <c r="S27" s="4">
         <f ca="1"/>
-        <v>0.20455886903305909</v>
+        <v>0.21129177216442607</v>
       </c>
       <c r="T27" s="9" t="e">
         <f ca="1"/>
@@ -2008,7 +2009,7 @@
       </c>
       <c r="S28" s="4">
         <f ca="1"/>
-        <v>0.21129177216442607</v>
+        <v>0.21289020404938441</v>
       </c>
       <c r="T28" s="9" t="e">
         <f ca="1"/>
@@ -2021,7 +2022,7 @@
       </c>
       <c r="S29" s="4">
         <f ca="1"/>
-        <v>0.21289020404938441</v>
+        <v>0.24005046089105242</v>
       </c>
       <c r="T29" s="9" t="e">
         <f ca="1"/>
@@ -2034,7 +2035,7 @@
       </c>
       <c r="S30" s="4">
         <f ca="1"/>
-        <v>0.24005046089105242</v>
+        <v>0.24683784713265966</v>
       </c>
       <c r="T30" s="9" t="e">
         <f ca="1"/>
@@ -2047,7 +2048,7 @@
       </c>
       <c r="S31" s="4">
         <f ca="1"/>
-        <v>0.24683784713265966</v>
+        <v>0.25090708805825079</v>
       </c>
       <c r="T31" s="9" t="e">
         <f ca="1"/>
@@ -2060,7 +2061,7 @@
       </c>
       <c r="S32" s="4">
         <f ca="1"/>
-        <v>0.25090708805825079</v>
+        <v>0.25958386357364216</v>
       </c>
       <c r="T32" s="9" t="e">
         <f ca="1"/>
@@ -2073,7 +2074,7 @@
       </c>
       <c r="S33" s="4">
         <f ca="1"/>
-        <v>0.25958386357364216</v>
+        <v>0.26026766796149603</v>
       </c>
       <c r="T33" s="9" t="e">
         <f ca="1"/>
@@ -2086,7 +2087,7 @@
       </c>
       <c r="S34" s="4">
         <f ca="1"/>
-        <v>0.26026766796149603</v>
+        <v>0.2819709570143808</v>
       </c>
       <c r="T34" s="9" t="e">
         <f ca="1"/>
@@ -2099,7 +2100,7 @@
       </c>
       <c r="S35" s="4">
         <f ca="1"/>
-        <v>0.2819709570143808</v>
+        <v>0.28303369927876221</v>
       </c>
       <c r="T35" s="9" t="e">
         <f ca="1"/>
@@ -2112,7 +2113,7 @@
       </c>
       <c r="S36" s="4">
         <f ca="1"/>
-        <v>0.28303369927876221</v>
+        <v>0.29579294051174709</v>
       </c>
       <c r="T36" s="9" t="e">
         <f ca="1"/>
@@ -2125,7 +2126,7 @@
       </c>
       <c r="S37" s="4">
         <f ca="1"/>
-        <v>0.29579294051174709</v>
+        <v>0.30621594261281582</v>
       </c>
       <c r="T37" s="9" t="e">
         <f ca="1"/>
@@ -2138,7 +2139,7 @@
       </c>
       <c r="S38" s="4">
         <f ca="1"/>
-        <v>0.30621594261281582</v>
+        <v>0.30699880764121135</v>
       </c>
       <c r="T38" s="9" t="e">
         <f ca="1"/>
@@ -2151,7 +2152,7 @@
       </c>
       <c r="S39" s="4">
         <f ca="1"/>
-        <v>0.30699880764121135</v>
+        <v>0.30746381468864881</v>
       </c>
       <c r="T39" s="9" t="e">
         <f ca="1"/>
@@ -2164,7 +2165,7 @@
       </c>
       <c r="S40" s="4">
         <f ca="1"/>
-        <v>0.30746381468864881</v>
+        <v>0.30991009987247375</v>
       </c>
       <c r="T40" s="9" t="e">
         <f ca="1"/>
@@ -2177,7 +2178,7 @@
       </c>
       <c r="S41" s="4">
         <f ca="1"/>
-        <v>0.30991009987247375</v>
+        <v>0.34322350221251363</v>
       </c>
       <c r="T41" s="9" t="e">
         <f ca="1"/>
@@ -2190,7 +2191,7 @@
       </c>
       <c r="S42" s="4">
         <f ca="1"/>
-        <v>0.34322350221251363</v>
+        <v>0.346644941363903</v>
       </c>
       <c r="T42" s="9" t="e">
         <f ca="1"/>
@@ -2203,7 +2204,7 @@
       </c>
       <c r="S43" s="4">
         <f ca="1"/>
-        <v>0.346644941363903</v>
+        <v>0.35070608842246354</v>
       </c>
       <c r="T43" s="9" t="e">
         <f ca="1"/>
@@ -2216,7 +2217,7 @@
       </c>
       <c r="S44" s="4">
         <f ca="1"/>
-        <v>0.35070608842246354</v>
+        <v>0.35500379302962237</v>
       </c>
       <c r="T44" s="9" t="e">
         <f ca="1"/>
@@ -2229,7 +2230,7 @@
       </c>
       <c r="S45" s="4">
         <f ca="1"/>
-        <v>0.35500379302962237</v>
+        <v>0.36303952239766712</v>
       </c>
       <c r="T45" s="9" t="e">
         <f ca="1"/>
@@ -2242,7 +2243,7 @@
       </c>
       <c r="S46" s="4">
         <f ca="1"/>
-        <v>0.36303952239766712</v>
+        <v>0.37590154211670712</v>
       </c>
       <c r="T46" s="9" t="e">
         <f ca="1"/>
@@ -2255,7 +2256,7 @@
       </c>
       <c r="S47" s="4">
         <f ca="1"/>
-        <v>0.37590154211670712</v>
+        <v>0.37822251634842252</v>
       </c>
       <c r="T47" s="9" t="e">
         <f ca="1"/>
@@ -2268,7 +2269,7 @@
       </c>
       <c r="S48" s="4">
         <f ca="1"/>
-        <v>0.37822251634842252</v>
+        <v>0.38122419173045929</v>
       </c>
       <c r="T48" s="9" t="e">
         <f ca="1"/>
@@ -2281,7 +2282,7 @@
       </c>
       <c r="S49" s="4">
         <f ca="1"/>
-        <v>0.38122419173045929</v>
+        <v>0.38693032613344891</v>
       </c>
       <c r="T49" s="9" t="e">
         <f ca="1"/>
@@ -2294,7 +2295,7 @@
       </c>
       <c r="S50" s="4">
         <f ca="1"/>
-        <v>0.38693032613344891</v>
+        <v>0.38924117354343202</v>
       </c>
       <c r="T50" s="9" t="e">
         <f ca="1"/>
@@ -2307,7 +2308,7 @@
       </c>
       <c r="S51" s="4">
         <f ca="1"/>
-        <v>0.38924117354343202</v>
+        <v>0.41032128248045219</v>
       </c>
       <c r="T51" s="9" t="e">
         <f ca="1"/>
@@ -2320,7 +2321,7 @@
       </c>
       <c r="S52" s="4">
         <f ca="1"/>
-        <v>0.41032128248045219</v>
+        <v>0.43199912726020961</v>
       </c>
       <c r="T52" s="9" t="e">
         <f ca="1"/>
@@ -2333,7 +2334,7 @@
       </c>
       <c r="S53" s="4">
         <f ca="1"/>
-        <v>0.43199912726020961</v>
+        <v>0.44362993322818001</v>
       </c>
       <c r="T53" s="9" t="e">
         <f ca="1"/>
@@ -2346,7 +2347,7 @@
       </c>
       <c r="S54" s="4">
         <f ca="1"/>
-        <v>0.44362993322818001</v>
+        <v>0.44578595954200495</v>
       </c>
       <c r="T54" s="9" t="e">
         <f ca="1"/>
@@ -2359,7 +2360,7 @@
       </c>
       <c r="S55" s="4">
         <f ca="1"/>
-        <v>0.44578595954200495</v>
+        <v>0.50309865693105404</v>
       </c>
       <c r="T55" s="9" t="e">
         <f ca="1"/>
@@ -2372,7 +2373,7 @@
       </c>
       <c r="S56" s="4">
         <f ca="1"/>
-        <v>0.50309865693105404</v>
+        <v>0.55553726039846762</v>
       </c>
       <c r="T56" s="9" t="e">
         <f ca="1"/>
@@ -2385,7 +2386,7 @@
       </c>
       <c r="S57" s="4">
         <f ca="1"/>
-        <v>0.55553726039846762</v>
+        <v>0.56072877256876819</v>
       </c>
       <c r="T57" s="9" t="e">
         <f ca="1"/>
@@ -2398,7 +2399,7 @@
       </c>
       <c r="S58" s="4">
         <f ca="1"/>
-        <v>0.56072877256876819</v>
+        <v>0.56613202852270661</v>
       </c>
       <c r="T58" s="9" t="e">
         <f ca="1"/>
@@ -2411,7 +2412,7 @@
       </c>
       <c r="S59" s="4">
         <f ca="1"/>
-        <v>0.56613202852270661</v>
+        <v>0.56907031356613658</v>
       </c>
       <c r="T59" s="9" t="e">
         <f ca="1"/>
@@ -2424,7 +2425,7 @@
       </c>
       <c r="S60" s="4">
         <f ca="1"/>
-        <v>0.56907031356613658</v>
+        <v>0.57665750527755044</v>
       </c>
       <c r="T60" s="9" t="e">
         <f ca="1"/>
@@ -2437,7 +2438,7 @@
       </c>
       <c r="S61" s="4">
         <f ca="1"/>
-        <v>0.57665750527755044</v>
+        <v>0.57712158377157863</v>
       </c>
       <c r="T61" s="9" t="e">
         <f ca="1"/>
@@ -2450,7 +2451,7 @@
       </c>
       <c r="S62" s="4">
         <f ca="1"/>
-        <v>0.57712158377157863</v>
+        <v>0.58507289523339523</v>
       </c>
       <c r="T62" s="9" t="e">
         <f ca="1"/>
@@ -2463,7 +2464,7 @@
       </c>
       <c r="S63" s="4">
         <f ca="1"/>
-        <v>0.58507289523339523</v>
+        <v>0.5992299667126384</v>
       </c>
       <c r="T63" s="9" t="e">
         <f ca="1"/>
@@ -2476,7 +2477,7 @@
       </c>
       <c r="S64" s="4">
         <f ca="1"/>
-        <v>0.5992299667126384</v>
+        <v>0.60411978716231773</v>
       </c>
       <c r="T64" s="9" t="e">
         <f ca="1"/>
@@ -2489,7 +2490,7 @@
       </c>
       <c r="S65" s="4">
         <f ca="1"/>
-        <v>0.60411978716231773</v>
+        <v>0.60977631212733274</v>
       </c>
       <c r="T65" s="9" t="e">
         <f ca="1"/>
@@ -2502,7 +2503,7 @@
       </c>
       <c r="S66" s="4">
         <f ca="1"/>
-        <v>0.60977631212733274</v>
+        <v>0.61835596776400625</v>
       </c>
       <c r="T66" s="9" t="e">
         <f ca="1"/>
@@ -2515,7 +2516,7 @@
       </c>
       <c r="S67" s="4">
         <f ca="1"/>
-        <v>0.61835596776400625</v>
+        <v>0.63120330732006702</v>
       </c>
       <c r="T67" s="9" t="e">
         <f ca="1"/>

</xml_diff>

<commit_message>
* Much updating of documentation and tests.. * Add zipped tests as examples in documentation * Add build of doxygen docs for C++ API
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D53C4D-33A7-46FF-AC66-13078E028B66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC6B37D-3648-498B-8DEE-64AA36F709DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="-108" windowWidth="22296" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="864" yWindow="-108" windowWidth="22284" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
     <sheet name="Concat-Split" sheetId="2" r:id="rId2"/>
     <sheet name="Sort" sheetId="3" r:id="rId3"/>
+    <sheet name="xloRef" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -1078,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,7 +1356,7 @@
       </c>
       <c r="R5" s="7">
         <f ca="1">RAND()</f>
-        <v>0.63120330732006702</v>
+        <v>0.49178290346307407</v>
       </c>
       <c r="S5" s="4">
         <f t="array" aca="1" ref="S5:S104" ca="1">_xll.xloSort(R5:R104,"a")</f>
@@ -2360,7 +2361,7 @@
       </c>
       <c r="S55" s="4">
         <f ca="1"/>
-        <v>0.50309865693105404</v>
+        <v>0.49178290346307407</v>
       </c>
       <c r="T55" s="9" t="e">
         <f ca="1"/>
@@ -2373,7 +2374,7 @@
       </c>
       <c r="S56" s="4">
         <f ca="1"/>
-        <v>0.55553726039846762</v>
+        <v>0.50309865693105404</v>
       </c>
       <c r="T56" s="9" t="e">
         <f ca="1"/>
@@ -2386,7 +2387,7 @@
       </c>
       <c r="S57" s="4">
         <f ca="1"/>
-        <v>0.56072877256876819</v>
+        <v>0.55553726039846762</v>
       </c>
       <c r="T57" s="9" t="e">
         <f ca="1"/>
@@ -2399,7 +2400,7 @@
       </c>
       <c r="S58" s="4">
         <f ca="1"/>
-        <v>0.56613202852270661</v>
+        <v>0.56072877256876819</v>
       </c>
       <c r="T58" s="9" t="e">
         <f ca="1"/>
@@ -2412,7 +2413,7 @@
       </c>
       <c r="S59" s="4">
         <f ca="1"/>
-        <v>0.56907031356613658</v>
+        <v>0.56613202852270661</v>
       </c>
       <c r="T59" s="9" t="e">
         <f ca="1"/>
@@ -2425,7 +2426,7 @@
       </c>
       <c r="S60" s="4">
         <f ca="1"/>
-        <v>0.57665750527755044</v>
+        <v>0.56907031356613658</v>
       </c>
       <c r="T60" s="9" t="e">
         <f ca="1"/>
@@ -2438,7 +2439,7 @@
       </c>
       <c r="S61" s="4">
         <f ca="1"/>
-        <v>0.57712158377157863</v>
+        <v>0.57665750527755044</v>
       </c>
       <c r="T61" s="9" t="e">
         <f ca="1"/>
@@ -2451,7 +2452,7 @@
       </c>
       <c r="S62" s="4">
         <f ca="1"/>
-        <v>0.58507289523339523</v>
+        <v>0.57712158377157863</v>
       </c>
       <c r="T62" s="9" t="e">
         <f ca="1"/>
@@ -2464,7 +2465,7 @@
       </c>
       <c r="S63" s="4">
         <f ca="1"/>
-        <v>0.5992299667126384</v>
+        <v>0.58507289523339523</v>
       </c>
       <c r="T63" s="9" t="e">
         <f ca="1"/>
@@ -2477,7 +2478,7 @@
       </c>
       <c r="S64" s="4">
         <f ca="1"/>
-        <v>0.60411978716231773</v>
+        <v>0.5992299667126384</v>
       </c>
       <c r="T64" s="9" t="e">
         <f ca="1"/>
@@ -2490,7 +2491,7 @@
       </c>
       <c r="S65" s="4">
         <f ca="1"/>
-        <v>0.60977631212733274</v>
+        <v>0.60411978716231773</v>
       </c>
       <c r="T65" s="9" t="e">
         <f ca="1"/>
@@ -2503,7 +2504,7 @@
       </c>
       <c r="S66" s="4">
         <f ca="1"/>
-        <v>0.61835596776400625</v>
+        <v>0.60977631212733274</v>
       </c>
       <c r="T66" s="9" t="e">
         <f ca="1"/>
@@ -2516,7 +2517,7 @@
       </c>
       <c r="S67" s="4">
         <f ca="1"/>
-        <v>0.63120330732006702</v>
+        <v>0.61835596776400625</v>
       </c>
       <c r="T67" s="9" t="e">
         <f ca="1"/>
@@ -3012,4 +3013,54 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E817F54A-CCFE-4A18-A557-D52A0ED58479}">
+  <dimension ref="B2:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="str">
+        <f t="array" ref="B2">_xll.xloRef(B4:C5)</f>
+        <v>永[xlOil_Utils.xlsx]xloRef!R2C2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f t="array" ref="E4:F5">_xll.xloVal(B2)</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Utils test spreadsheet to include array functionality in xloSplit
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC6B37D-3648-498B-8DEE-64AA36F709DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD596E1E-7828-40AE-82E4-2031DD122866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="864" yWindow="-108" windowWidth="22284" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>1, 2; 3, 4;</t>
   </si>
@@ -188,6 +188,27 @@
   </si>
   <si>
     <t>Split string above on '-'</t>
+  </si>
+  <si>
+    <t>Split array of string</t>
+  </si>
+  <si>
+    <t>Gr</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Split horizontal array of string</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Ignore non-strings</t>
   </si>
 </sst>
 </file>
@@ -606,14 +627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
@@ -1077,16 +1093,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K23"/>
+  <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
@@ -1272,6 +1285,216 @@
       </c>
       <c r="H23" s="16" t="b">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="str">
+        <f t="array" ref="B27:C30">_xll.xloSplit(I5:I8,"e")</f>
+        <v>Foo</v>
+      </c>
+      <c r="C27" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G27" s="16" t="b">
+        <f>E27=B27</f>
+        <v>1</v>
+      </c>
+      <c r="H27" s="16" t="b">
+        <f>ISNA(C27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="str">
+        <v>Gr</v>
+      </c>
+      <c r="C28" s="5" t="str">
+        <v>n</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="16" t="b">
+        <f t="shared" ref="G28:G30" si="1">E28=B28</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="16" t="b">
+        <f t="shared" ref="H28" si="2">F28=C28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="C29" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G29" s="16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H29" s="16" t="b">
+        <f>ISNA(C29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="C30" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G30" s="16" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H30" s="16" t="b">
+        <f>ISNA(C30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="5" t="str">
+        <f t="array" ref="B34:D35">_xll.xloSplit(I5:K5,"a")</f>
+        <v>Foo</v>
+      </c>
+      <c r="C34" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="D34" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="E34" s="16" t="b">
+        <f>B36=B34</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="16" t="b">
+        <f t="shared" ref="F34:G34" si="3">C36=C34</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="16" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <v>r</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <v>z</v>
+      </c>
+      <c r="E35" s="16" t="b">
+        <f>ISNA(B37)</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="16" t="b">
+        <f t="shared" ref="F35" si="4">C37=C35</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="16" t="b">
+        <f t="shared" ref="G35" si="5">D37=D35</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5">
+        <f t="array" ref="C40:C42">_xll.xloSplit(B40:B42,"x")</f>
+        <v>1</v>
+      </c>
+      <c r="E40" s="16" t="b">
+        <f>C40=B40</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>2</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
+      <c r="E41" s="16" t="b">
+        <f t="shared" ref="E41:E42" si="6">C41=B41</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>3</v>
+      </c>
+      <c r="C42" s="5">
+        <v>3</v>
+      </c>
+      <c r="E42" s="16" t="b">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -1284,23 +1507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:V105"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="12" max="12" width="4.44140625" customWidth="1"/>
-    <col min="14" max="14" width="3.6640625" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.6640625" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.3">
       <c r="T1" s="11"/>
@@ -1356,7 +1565,7 @@
       </c>
       <c r="R5" s="7">
         <f ca="1">RAND()</f>
-        <v>0.49178290346307407</v>
+        <v>0.14072104298134069</v>
       </c>
       <c r="S5" s="4">
         <f t="array" aca="1" ref="S5:S104" ca="1">_xll.xloSort(R5:R104,"a")</f>
@@ -1674,7 +1883,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="14" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="E14" s="13" t="s">
         <v>44</v>
       </c>
@@ -1845,7 +2054,7 @@
       </c>
       <c r="S19" s="4">
         <f ca="1"/>
-        <v>0.15138392223952224</v>
+        <v>0.14072104298134069</v>
       </c>
       <c r="T19" s="9" t="e">
         <f ca="1"/>
@@ -1870,7 +2079,7 @@
       </c>
       <c r="S20" s="4">
         <f ca="1"/>
-        <v>0.15285256271102787</v>
+        <v>0.15138392223952224</v>
       </c>
       <c r="T20" s="9" t="e">
         <f ca="1"/>
@@ -1895,7 +2104,7 @@
       </c>
       <c r="S21" s="4">
         <f ca="1"/>
-        <v>0.15935651729819933</v>
+        <v>0.15285256271102787</v>
       </c>
       <c r="T21" s="9" t="e">
         <f ca="1"/>
@@ -1920,7 +2129,7 @@
       </c>
       <c r="S22" s="4">
         <f ca="1"/>
-        <v>0.16534127039316493</v>
+        <v>0.15935651729819933</v>
       </c>
       <c r="T22" s="9" t="e">
         <f ca="1"/>
@@ -1945,7 +2154,7 @@
       </c>
       <c r="S23" s="4">
         <f ca="1"/>
-        <v>0.18684151297687135</v>
+        <v>0.16534127039316493</v>
       </c>
       <c r="T23" s="9" t="e">
         <f ca="1"/>
@@ -1958,7 +2167,7 @@
       </c>
       <c r="S24" s="4">
         <f ca="1"/>
-        <v>0.19150797219437865</v>
+        <v>0.18684151297687135</v>
       </c>
       <c r="T24" s="9" t="e">
         <f ca="1"/>
@@ -1971,7 +2180,7 @@
       </c>
       <c r="S25" s="4">
         <f ca="1"/>
-        <v>0.19332448079141096</v>
+        <v>0.19150797219437865</v>
       </c>
       <c r="T25" s="9" t="e">
         <f ca="1"/>
@@ -1984,7 +2193,7 @@
       </c>
       <c r="S26" s="4">
         <f ca="1"/>
-        <v>0.20455886903305909</v>
+        <v>0.19332448079141096</v>
       </c>
       <c r="T26" s="9" t="e">
         <f ca="1"/>
@@ -1997,7 +2206,7 @@
       </c>
       <c r="S27" s="4">
         <f ca="1"/>
-        <v>0.21129177216442607</v>
+        <v>0.20455886903305909</v>
       </c>
       <c r="T27" s="9" t="e">
         <f ca="1"/>
@@ -2010,7 +2219,7 @@
       </c>
       <c r="S28" s="4">
         <f ca="1"/>
-        <v>0.21289020404938441</v>
+        <v>0.21129177216442607</v>
       </c>
       <c r="T28" s="9" t="e">
         <f ca="1"/>
@@ -2023,7 +2232,7 @@
       </c>
       <c r="S29" s="4">
         <f ca="1"/>
-        <v>0.24005046089105242</v>
+        <v>0.21289020404938441</v>
       </c>
       <c r="T29" s="9" t="e">
         <f ca="1"/>
@@ -2036,7 +2245,7 @@
       </c>
       <c r="S30" s="4">
         <f ca="1"/>
-        <v>0.24683784713265966</v>
+        <v>0.24005046089105242</v>
       </c>
       <c r="T30" s="9" t="e">
         <f ca="1"/>
@@ -2049,7 +2258,7 @@
       </c>
       <c r="S31" s="4">
         <f ca="1"/>
-        <v>0.25090708805825079</v>
+        <v>0.24683784713265966</v>
       </c>
       <c r="T31" s="9" t="e">
         <f ca="1"/>
@@ -2062,7 +2271,7 @@
       </c>
       <c r="S32" s="4">
         <f ca="1"/>
-        <v>0.25958386357364216</v>
+        <v>0.25090708805825079</v>
       </c>
       <c r="T32" s="9" t="e">
         <f ca="1"/>
@@ -2075,7 +2284,7 @@
       </c>
       <c r="S33" s="4">
         <f ca="1"/>
-        <v>0.26026766796149603</v>
+        <v>0.25958386357364216</v>
       </c>
       <c r="T33" s="9" t="e">
         <f ca="1"/>
@@ -2088,7 +2297,7 @@
       </c>
       <c r="S34" s="4">
         <f ca="1"/>
-        <v>0.2819709570143808</v>
+        <v>0.26026766796149603</v>
       </c>
       <c r="T34" s="9" t="e">
         <f ca="1"/>
@@ -2101,7 +2310,7 @@
       </c>
       <c r="S35" s="4">
         <f ca="1"/>
-        <v>0.28303369927876221</v>
+        <v>0.2819709570143808</v>
       </c>
       <c r="T35" s="9" t="e">
         <f ca="1"/>
@@ -2114,7 +2323,7 @@
       </c>
       <c r="S36" s="4">
         <f ca="1"/>
-        <v>0.29579294051174709</v>
+        <v>0.28303369927876221</v>
       </c>
       <c r="T36" s="9" t="e">
         <f ca="1"/>
@@ -2127,7 +2336,7 @@
       </c>
       <c r="S37" s="4">
         <f ca="1"/>
-        <v>0.30621594261281582</v>
+        <v>0.29579294051174709</v>
       </c>
       <c r="T37" s="9" t="e">
         <f ca="1"/>
@@ -2140,7 +2349,7 @@
       </c>
       <c r="S38" s="4">
         <f ca="1"/>
-        <v>0.30699880764121135</v>
+        <v>0.30621594261281582</v>
       </c>
       <c r="T38" s="9" t="e">
         <f ca="1"/>
@@ -2153,7 +2362,7 @@
       </c>
       <c r="S39" s="4">
         <f ca="1"/>
-        <v>0.30746381468864881</v>
+        <v>0.30699880764121135</v>
       </c>
       <c r="T39" s="9" t="e">
         <f ca="1"/>
@@ -2166,7 +2375,7 @@
       </c>
       <c r="S40" s="4">
         <f ca="1"/>
-        <v>0.30991009987247375</v>
+        <v>0.30746381468864881</v>
       </c>
       <c r="T40" s="9" t="e">
         <f ca="1"/>
@@ -2179,7 +2388,7 @@
       </c>
       <c r="S41" s="4">
         <f ca="1"/>
-        <v>0.34322350221251363</v>
+        <v>0.30991009987247375</v>
       </c>
       <c r="T41" s="9" t="e">
         <f ca="1"/>
@@ -2192,7 +2401,7 @@
       </c>
       <c r="S42" s="4">
         <f ca="1"/>
-        <v>0.346644941363903</v>
+        <v>0.34322350221251363</v>
       </c>
       <c r="T42" s="9" t="e">
         <f ca="1"/>
@@ -2205,7 +2414,7 @@
       </c>
       <c r="S43" s="4">
         <f ca="1"/>
-        <v>0.35070608842246354</v>
+        <v>0.346644941363903</v>
       </c>
       <c r="T43" s="9" t="e">
         <f ca="1"/>
@@ -2218,7 +2427,7 @@
       </c>
       <c r="S44" s="4">
         <f ca="1"/>
-        <v>0.35500379302962237</v>
+        <v>0.35070608842246354</v>
       </c>
       <c r="T44" s="9" t="e">
         <f ca="1"/>
@@ -2231,7 +2440,7 @@
       </c>
       <c r="S45" s="4">
         <f ca="1"/>
-        <v>0.36303952239766712</v>
+        <v>0.35500379302962237</v>
       </c>
       <c r="T45" s="9" t="e">
         <f ca="1"/>
@@ -2244,7 +2453,7 @@
       </c>
       <c r="S46" s="4">
         <f ca="1"/>
-        <v>0.37590154211670712</v>
+        <v>0.36303952239766712</v>
       </c>
       <c r="T46" s="9" t="e">
         <f ca="1"/>
@@ -2257,7 +2466,7 @@
       </c>
       <c r="S47" s="4">
         <f ca="1"/>
-        <v>0.37822251634842252</v>
+        <v>0.37590154211670712</v>
       </c>
       <c r="T47" s="9" t="e">
         <f ca="1"/>
@@ -2270,7 +2479,7 @@
       </c>
       <c r="S48" s="4">
         <f ca="1"/>
-        <v>0.38122419173045929</v>
+        <v>0.37822251634842252</v>
       </c>
       <c r="T48" s="9" t="e">
         <f ca="1"/>
@@ -2283,7 +2492,7 @@
       </c>
       <c r="S49" s="4">
         <f ca="1"/>
-        <v>0.38693032613344891</v>
+        <v>0.38122419173045929</v>
       </c>
       <c r="T49" s="9" t="e">
         <f ca="1"/>
@@ -2296,7 +2505,7 @@
       </c>
       <c r="S50" s="4">
         <f ca="1"/>
-        <v>0.38924117354343202</v>
+        <v>0.38693032613344891</v>
       </c>
       <c r="T50" s="9" t="e">
         <f ca="1"/>
@@ -2309,7 +2518,7 @@
       </c>
       <c r="S51" s="4">
         <f ca="1"/>
-        <v>0.41032128248045219</v>
+        <v>0.38924117354343202</v>
       </c>
       <c r="T51" s="9" t="e">
         <f ca="1"/>
@@ -2322,7 +2531,7 @@
       </c>
       <c r="S52" s="4">
         <f ca="1"/>
-        <v>0.43199912726020961</v>
+        <v>0.41032128248045219</v>
       </c>
       <c r="T52" s="9" t="e">
         <f ca="1"/>
@@ -2335,7 +2544,7 @@
       </c>
       <c r="S53" s="4">
         <f ca="1"/>
-        <v>0.44362993322818001</v>
+        <v>0.43199912726020961</v>
       </c>
       <c r="T53" s="9" t="e">
         <f ca="1"/>
@@ -2348,7 +2557,7 @@
       </c>
       <c r="S54" s="4">
         <f ca="1"/>
-        <v>0.44578595954200495</v>
+        <v>0.44362993322818001</v>
       </c>
       <c r="T54" s="9" t="e">
         <f ca="1"/>
@@ -2361,7 +2570,7 @@
       </c>
       <c r="S55" s="4">
         <f ca="1"/>
-        <v>0.49178290346307407</v>
+        <v>0.44578595954200495</v>
       </c>
       <c r="T55" s="9" t="e">
         <f ca="1"/>
@@ -3011,17 +3220,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E817F54A-CCFE-4A18-A557-D52A0ED58479}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
Add xloIndex function to Utils which extends the Excel INDEX function to cache refs and sub-arrays.  To support this,: * Improve handling of negative indices in ExcelArray * Add function to conveniently copy an ExcelArray to a new ExcelObj * objectCacheExpand function to simplify processing of xloref args
tests: added unit tests for ExcelArray and added xloIndex to Utils test spreadsheet
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -1,38 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD596E1E-7828-40AE-82E4-2031DD122866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5FB785-CD4B-4739-AD07-2CE9B56B546B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
     <sheet name="Concat-Split" sheetId="2" r:id="rId2"/>
     <sheet name="Sort" sheetId="3" r:id="rId3"/>
-    <sheet name="xloRef" sheetId="4" r:id="rId4"/>
+    <sheet name="xloRef-Index" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
   <si>
     <t>1, 2; 3, 4;</t>
   </si>
@@ -209,6 +201,21 @@
   </si>
   <si>
     <t>Ignore non-strings</t>
+  </si>
+  <si>
+    <t>xloRef: round trip</t>
+  </si>
+  <si>
+    <t>xloIndex: match Excel INDEX</t>
+  </si>
+  <si>
+    <t>xloIndex: negative indices</t>
+  </si>
+  <si>
+    <t>xloIndex: missing args</t>
+  </si>
+  <si>
+    <t>xloIndex: zero toCol/toRow</t>
   </si>
 </sst>
 </file>
@@ -1095,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1565,7 +1572,7 @@
       </c>
       <c r="R5" s="7">
         <f ca="1">RAND()</f>
-        <v>0.14072104298134069</v>
+        <v>0.25940116072391706</v>
       </c>
       <c r="S5" s="4">
         <f t="array" aca="1" ref="S5:S104" ca="1">_xll.xloSort(R5:R104,"a")</f>
@@ -2054,7 +2061,7 @@
       </c>
       <c r="S19" s="4">
         <f ca="1"/>
-        <v>0.14072104298134069</v>
+        <v>0.15138392223952224</v>
       </c>
       <c r="T19" s="9" t="e">
         <f ca="1"/>
@@ -2079,7 +2086,7 @@
       </c>
       <c r="S20" s="4">
         <f ca="1"/>
-        <v>0.15138392223952224</v>
+        <v>0.15285256271102787</v>
       </c>
       <c r="T20" s="9" t="e">
         <f ca="1"/>
@@ -2104,7 +2111,7 @@
       </c>
       <c r="S21" s="4">
         <f ca="1"/>
-        <v>0.15285256271102787</v>
+        <v>0.15935651729819933</v>
       </c>
       <c r="T21" s="9" t="e">
         <f ca="1"/>
@@ -2129,7 +2136,7 @@
       </c>
       <c r="S22" s="4">
         <f ca="1"/>
-        <v>0.15935651729819933</v>
+        <v>0.16534127039316493</v>
       </c>
       <c r="T22" s="9" t="e">
         <f ca="1"/>
@@ -2154,7 +2161,7 @@
       </c>
       <c r="S23" s="4">
         <f ca="1"/>
-        <v>0.16534127039316493</v>
+        <v>0.18684151297687135</v>
       </c>
       <c r="T23" s="9" t="e">
         <f ca="1"/>
@@ -2167,7 +2174,7 @@
       </c>
       <c r="S24" s="4">
         <f ca="1"/>
-        <v>0.18684151297687135</v>
+        <v>0.19150797219437865</v>
       </c>
       <c r="T24" s="9" t="e">
         <f ca="1"/>
@@ -2180,7 +2187,7 @@
       </c>
       <c r="S25" s="4">
         <f ca="1"/>
-        <v>0.19150797219437865</v>
+        <v>0.19332448079141096</v>
       </c>
       <c r="T25" s="9" t="e">
         <f ca="1"/>
@@ -2193,7 +2200,7 @@
       </c>
       <c r="S26" s="4">
         <f ca="1"/>
-        <v>0.19332448079141096</v>
+        <v>0.20455886903305909</v>
       </c>
       <c r="T26" s="9" t="e">
         <f ca="1"/>
@@ -2206,7 +2213,7 @@
       </c>
       <c r="S27" s="4">
         <f ca="1"/>
-        <v>0.20455886903305909</v>
+        <v>0.21129177216442607</v>
       </c>
       <c r="T27" s="9" t="e">
         <f ca="1"/>
@@ -2219,7 +2226,7 @@
       </c>
       <c r="S28" s="4">
         <f ca="1"/>
-        <v>0.21129177216442607</v>
+        <v>0.21289020404938441</v>
       </c>
       <c r="T28" s="9" t="e">
         <f ca="1"/>
@@ -2232,7 +2239,7 @@
       </c>
       <c r="S29" s="4">
         <f ca="1"/>
-        <v>0.21289020404938441</v>
+        <v>0.24005046089105242</v>
       </c>
       <c r="T29" s="9" t="e">
         <f ca="1"/>
@@ -2245,7 +2252,7 @@
       </c>
       <c r="S30" s="4">
         <f ca="1"/>
-        <v>0.24005046089105242</v>
+        <v>0.24683784713265966</v>
       </c>
       <c r="T30" s="9" t="e">
         <f ca="1"/>
@@ -2258,7 +2265,7 @@
       </c>
       <c r="S31" s="4">
         <f ca="1"/>
-        <v>0.24683784713265966</v>
+        <v>0.25090708805825079</v>
       </c>
       <c r="T31" s="9" t="e">
         <f ca="1"/>
@@ -2271,7 +2278,7 @@
       </c>
       <c r="S32" s="4">
         <f ca="1"/>
-        <v>0.25090708805825079</v>
+        <v>0.25940116072391706</v>
       </c>
       <c r="T32" s="9" t="e">
         <f ca="1"/>
@@ -3225,48 +3232,222 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:F5"/>
+  <dimension ref="B2:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="str">
-        <f t="array" ref="B2">_xll.xloRef(B4:C5)</f>
-        <v>永[xlOil_Utils.xlsx]xloRef!R2C2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="b">
+        <f t="array" ref="C3">SUM(0+(F3:H5=K3:M5))=9</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.xloRef(K3:M5)</f>
+        <v>永[xlOil_Utils.xlsx]xloRef-Index!R3C5</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="array" ref="F3:H5">_xll.xloVal(E3)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
         <v>2</v>
       </c>
-      <c r="E4">
-        <f t="array" ref="E4:F5">_xll.xloVal(B2)</f>
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="H3" s="5">
+        <v>3</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5">
+      <c r="M3" s="7">
         <v>3</v>
       </c>
-      <c r="C5">
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F4" s="5">
         <v>4</v>
       </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
+      <c r="G4" s="5">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6</v>
+      </c>
+      <c r="K4" s="7">
         <v>4</v>
+      </c>
+      <c r="L4" s="7">
+        <v>5</v>
+      </c>
+      <c r="M4" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F5" s="5">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5">
+        <v>9</v>
+      </c>
+      <c r="K5" s="7">
+        <v>7</v>
+      </c>
+      <c r="L5" s="7">
+        <v>8</v>
+      </c>
+      <c r="M5" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="b">
+        <f>D8=E8</f>
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f>INDEX($K$3:$M$5,2,2)</f>
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <f>_xll.xloIndex($E$3,2,2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C9" t="b">
+        <f>D9=E9</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f>INDEX($K$3:$M$5,1,2)</f>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f>_xll.xloIndex($E$3,1,2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C10" t="b">
+        <f>D10=E10</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>INDEX(K3:K5,2)</f>
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f>_xll.xloIndex(K3:K5,2)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="b">
+        <f>D13=E13</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>INDEX(K3:M5,ROWS(K3:M5),COLUMNS(K3:M5))</f>
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <f>_xll.xloIndex($E$3,-1,-1)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="b">
+        <f t="array" ref="C15">SUM(0+(D15:E15=F15:G15))=2</f>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f>K3</f>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f>L3</f>
+        <v>2</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="array" ref="F15:G15">_xll.xloIndex(E3,,,2,3)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="b">
+        <f t="array" ref="C17">SUM(0+(D17:E18=F17:G18))=4</f>
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>G4</f>
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <f>H4</f>
+        <v>6</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="array" ref="F17:G18">_xll.xloIndex($E$3,-2,-2, 0, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <f>G5</f>
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <f>H5</f>
+        <v>9</v>
+      </c>
+      <c r="F18" s="5">
+        <v>8</v>
+      </c>
+      <c r="G18" s="5">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix xlol_utils test spreadsheet
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2789321-E020-4CB5-B757-1C8C447382D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009D4D4A-3312-4876-AD55-56016D2E53D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,20 @@
     <sheet name="xloRef-Index" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="72">
   <si>
     <t>1, 2; 3, 4;</t>
   </si>
@@ -155,12 +163,6 @@
     <t>FooDs</t>
   </si>
   <si>
-    <t>Sort mixed data case insensitive</t>
-  </si>
-  <si>
-    <t>and case sensitive</t>
-  </si>
-  <si>
     <t>Sort array of doubles, no descriptors specified</t>
   </si>
   <si>
@@ -234,6 +236,18 @@
   </si>
   <si>
     <t xml:space="preserve">Repeat with xloRef </t>
+  </si>
+  <si>
+    <t>insensitive</t>
+  </si>
+  <si>
+    <t>sensitive</t>
+  </si>
+  <si>
+    <t>Sort mixed data (numbers, strings, errors)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeat passing an xloRef </t>
   </si>
 </sst>
 </file>
@@ -348,10 +362,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="38" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,24 +710,24 @@
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N3" t="e">
-        <f ca="1">N6=X6</f>
-        <v>#VALUE!</v>
+        <f>N6=X6</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="e">
-        <f t="array" ref="B4" ca="1">AND(L6:M7=V6:W7)</f>
-        <v>#VALUE!</v>
+      <c r="B4" s="15" t="b">
+        <f t="array" ref="B4">AND(L6:M7=V6:W7)</f>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -722,11 +736,11 @@
         <v>10</v>
       </c>
       <c r="N4" t="e">
-        <f ca="1">TEXT(N6, ".")</f>
-        <v>#VALUE!</v>
+        <f>TEXT(N6, ".")</f>
+        <v>#N/A</v>
       </c>
       <c r="V4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -736,17 +750,15 @@
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="4" t="e">
-        <f t="array" aca="1" ref="L6:N8" ca="1">_xll.xloBlock(E6,E7,F7,G7,H7)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M6" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L6" s="4" t="str">
+        <f t="array" ref="L6:N8">_xll.xloBlock(E6,E7,F7,G7,H7)</f>
+        <v>A</v>
+      </c>
+      <c r="M6" s="5" t="str">
+        <v>B</v>
       </c>
       <c r="N6" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="V6" s="13" t="s">
         <v>1</v>
@@ -774,17 +786,14 @@
       <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M7" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L7" s="5" t="str">
+        <v>C</v>
+      </c>
+      <c r="M7" s="5" t="str">
+        <v>D</v>
       </c>
       <c r="N7" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="V7" s="14" t="s">
         <v>3</v>
@@ -798,16 +807,13 @@
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="L8" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M8" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="N8" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="V8" s="14" t="e">
         <v>#N/A</v>
@@ -820,9 +826,9 @@
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="e">
-        <f t="array" ref="B10" ca="1">AND(P12:R15=V12:X15)</f>
-        <v>#VALUE!</v>
+      <c r="B10" s="12" t="b">
+        <f t="array" ref="B10">AND(P12:R15=V12:X15)</f>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -831,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -841,29 +847,25 @@
       <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="4" t="e">
-        <f t="array" aca="1" ref="L12:N15" ca="1">_xll.xloBlock(E12,E13:F14,G13:H14,I13,_xll.xloFill(J13,2,1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M12" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N12" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P12" s="5" t="e">
-        <f t="array" aca="1" ref="P12:R15" ca="1">_xll.xloFillNA(L12:N15,"NOPE")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q12" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R12" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L12" s="4" t="str">
+        <f t="array" ref="L12:N15">_xll.xloBlock(E12,E13:F14,G13:H14,I13,_xll.xloFill(J13,2,1))</f>
+        <v>A</v>
+      </c>
+      <c r="M12" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="N12" s="5" t="str">
+        <v>C</v>
+      </c>
+      <c r="P12" s="5" t="str">
+        <f t="array" ref="P12:R15">_xll.xloFillNA(L12:N15,"NOPE")</f>
+        <v>A</v>
+      </c>
+      <c r="Q12" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="R12" s="5" t="str">
+        <v>C</v>
       </c>
       <c r="V12" s="13" t="s">
         <v>1</v>
@@ -897,29 +899,23 @@
       <c r="J13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M13" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L13" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="M13" s="5" t="str">
+        <v>A</v>
       </c>
       <c r="N13" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P13" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q13" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R13" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="P13" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="Q13" s="5" t="str">
+        <v>A</v>
+      </c>
+      <c r="R13" s="5" t="str">
+        <v>NOPE</v>
       </c>
       <c r="V13" s="14" t="s">
         <v>1</v>
@@ -928,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="X13" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
@@ -946,29 +942,23 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="L14" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M14" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N14" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P14" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q14" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R14" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L14" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="M14" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="N14" s="5" t="str">
+        <v>F</v>
+      </c>
+      <c r="P14" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="Q14" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="R14" s="5" t="str">
+        <v>F</v>
       </c>
       <c r="V14" s="14" t="s">
         <v>2</v>
@@ -981,29 +971,23 @@
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="L15" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M15" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L15" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="M15" s="5" t="str">
+        <v>B</v>
       </c>
       <c r="N15" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P15" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q15" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R15" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="P15" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="Q15" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="R15" s="5" t="str">
+        <v/>
       </c>
       <c r="V15" s="13" t="s">
         <v>2</v>
@@ -1012,13 +996,13 @@
         <v>2</v>
       </c>
       <c r="X15" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="e">
-        <f t="array" ref="B17" ca="1">AND(L19:M20=V19:W20)</f>
-        <v>#VALUE!</v>
+      <c r="B17" s="12" t="b">
+        <f t="array" ref="B17">AND(L19:M20=V19:W20)</f>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1035,21 +1019,18 @@
       <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="4" t="e">
-        <f t="array" aca="1" ref="L19:O22" ca="1">_xll.xloBlock(E19,E20:F21,_xll.xloFill(G20,2,2),H20,I20)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M19" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L19" s="4" t="str">
+        <f t="array" ref="L19:O22">_xll.xloBlock(E19,E20:F21,_xll.xloFill(G20,2,2),H20,I20)</f>
+        <v>A</v>
+      </c>
+      <c r="M19" s="5" t="str">
+        <v>B</v>
       </c>
       <c r="N19" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="O19" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="V19" s="13" t="s">
         <v>1</v>
@@ -1068,13 +1049,12 @@
       <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="2" t="e">
-        <f t="array" aca="1" ref="E20:F21" ca="1">_xll.xloFill("A",2,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F20" s="2" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E20" s="2" t="str">
+        <f t="array" ref="E20:F21">_xll.xloFill("A",2,2)</f>
+        <v>A</v>
+      </c>
+      <c r="F20" s="2" t="str">
+        <v/>
       </c>
       <c r="G20" s="2" t="s">
         <v>2</v>
@@ -1085,21 +1065,17 @@
       <c r="I20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L20" s="5" t="str">
+        <v>C</v>
+      </c>
+      <c r="M20" s="5" t="str">
+        <v>D</v>
       </c>
       <c r="N20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="O20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="V20" s="13" t="s">
         <v>3</v>
@@ -1115,32 +1091,26 @@
       </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E21" s="2" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F21" s="2" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E21" s="2" t="str">
+        <v/>
+      </c>
+      <c r="F21" s="2" t="str">
+        <v/>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="L21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="N21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="O21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="V21" s="13" t="e">
         <v>#N/A</v>
@@ -1157,20 +1127,16 @@
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="L22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="N22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="O22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="V22" s="13" t="e">
         <v>#N/A</v>
@@ -1186,9 +1152,9 @@
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="e">
-        <f t="array" aca="1" ref="B24" ca="1">AND(IFERROR(Q26:T29=V26:Y29,ERROR.TYPE(Q26:T29)=ERROR.TYPE(V26:Y29)))</f>
-        <v>#N/A</v>
+      <c r="B24" s="12" t="b">
+        <f t="array" ref="B24">AND(IFERROR(Q26:T29=V26:Y29,ERROR.TYPE(Q26:T29)=ERROR.TYPE(V26:Y29)))</f>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -1197,7 +1163,7 @@
         <v>10</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.3">
@@ -1207,37 +1173,31 @@
       <c r="E26" t="s">
         <v>17</v>
       </c>
-      <c r="L26" s="4" t="e">
-        <f t="array" aca="1" ref="L26:O29" ca="1">_xll.xloBlock(E26,E27:F28,_xll.xloFill(G27,2,2),H27,I27)</f>
-        <v>#VALUE!</v>
+      <c r="L26" s="4" t="str">
+        <f t="array" ref="L26:O29">_xll.xloBlock(E26,E27:F28,_xll.xloFill(G27,2,2),H27,I27)</f>
+        <v>A</v>
       </c>
       <c r="M26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q26" s="5" t="e">
-        <f t="array" aca="1" ref="Q26:T29" ca="1">_xll.xloFillNA(L26:O29,".",FALSE)</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q26" s="5" t="str">
+        <f t="array" ref="Q26:T29">_xll.xloFillNA(L26:O29,".",FALSE)</f>
+        <v>A</v>
       </c>
       <c r="R26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T26" s="5" t="str">
+        <v>.</v>
       </c>
       <c r="V26" s="13" t="s">
         <v>1</v>
@@ -1249,20 +1209,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Y26" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.3">
       <c r="D27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="2" t="e">
-        <f t="array" aca="1" ref="E27:F28" ca="1">_xll.xloFill("A",2,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F27" s="2" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E27" s="2" t="str">
+        <f t="array" ref="E27:F28">_xll.xloFill("A",2,2)</f>
+        <v>A</v>
+      </c>
+      <c r="F27" s="2" t="str">
+        <v/>
       </c>
       <c r="G27" s="2" t="e">
         <f>1/0</f>
@@ -1275,39 +1234,31 @@
         <v>15</v>
       </c>
       <c r="L27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q27" s="5" t="str">
+        <v/>
       </c>
       <c r="R27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T27" s="5" t="str">
+        <v/>
       </c>
       <c r="V27" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="W27" s="13" t="e">
         <v>#DIV/0!</v>
@@ -1316,258 +1267,210 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Y27" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E28" s="2" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F28" s="2" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E28" s="2" t="str">
+        <v/>
+      </c>
+      <c r="F28" s="2" t="str">
+        <v/>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="L28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L28" s="5" t="str">
+        <v>Left</v>
       </c>
       <c r="M28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="N28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="O28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q28" s="5" t="str">
+        <v>Left</v>
+      </c>
+      <c r="R28" s="5" t="str">
+        <v/>
+      </c>
+      <c r="S28" s="5" t="str">
+        <v/>
+      </c>
+      <c r="T28" s="5" t="str">
+        <v/>
       </c>
       <c r="V28" s="13" t="s">
         <v>14</v>
       </c>
       <c r="W28" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="X28" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Y28" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="L29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="N29" s="5" t="str">
+        <v>Right</v>
       </c>
       <c r="O29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q29" s="5" t="str">
+        <v/>
+      </c>
+      <c r="R29" s="5" t="str">
+        <v/>
+      </c>
+      <c r="S29" s="5" t="str">
+        <v>Right</v>
+      </c>
+      <c r="T29" s="5" t="str">
+        <v/>
       </c>
       <c r="V29" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="W29" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>15</v>
       </c>
       <c r="Y29" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B31" s="12" t="e">
-        <f t="array" aca="1" ref="B31" ca="1">AND(IFERROR(Q33:T36=V26:Y29,ERROR.TYPE(Q33:T36)=ERROR.TYPE(V26:Y29)))</f>
-        <v>#N/A</v>
+      <c r="B31" s="12" t="b">
+        <f t="array" ref="B31">AND(IFERROR(Q33:T36=V26:Y29,ERROR.TYPE(Q33:T36)=ERROR.TYPE(V26:Y29)))</f>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="33" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="L33" s="5" t="e">
-        <f t="array" aca="1" ref="L33:O36" ca="1">_xll.xloBlock(E26,_xll.xloRef(E27:F28),_xll.xloFill(G27,2,2),_xll.xloRef(H27),I27)</f>
-        <v>#VALUE!</v>
+      <c r="L33" s="5" t="str">
+        <f t="array" ref="L33:O36">_xll.xloBlock(E26,_xll.xloRef(E27:F28),_xll.xloFill(G27,2,2),_xll.xloRef(H27),I27)</f>
+        <v>A</v>
       </c>
       <c r="M33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q33" s="5" t="e">
-        <f t="array" aca="1" ref="Q33:T36" ca="1">_xll.xloFillNA(_xll.xloRef(L33:O36),".",FALSE)</f>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q33" s="5" t="str">
+        <f t="array" ref="Q33:T36">_xll.xloFillNA(_xll.xloRef(L33:O36),".",FALSE)</f>
+        <v>A</v>
       </c>
       <c r="R33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T33" s="5" t="str">
+        <v>.</v>
       </c>
     </row>
     <row r="34" spans="12:20" x14ac:dyDescent="0.3">
       <c r="L34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="N34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q34" s="5" t="str">
+        <v/>
       </c>
       <c r="R34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T34" s="5" t="str">
+        <v/>
       </c>
     </row>
     <row r="35" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="L35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="L35" s="5" t="str">
+        <v>Left</v>
       </c>
       <c r="M35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="N35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="O35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q35" s="5" t="str">
+        <v>Left</v>
+      </c>
+      <c r="R35" s="5" t="str">
+        <v/>
+      </c>
+      <c r="S35" s="5" t="str">
+        <v/>
+      </c>
+      <c r="T35" s="5" t="str">
+        <v/>
       </c>
     </row>
     <row r="36" spans="12:20" x14ac:dyDescent="0.3">
       <c r="L36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="N36" s="5" t="str">
+        <v>Right</v>
       </c>
       <c r="O36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="Q36" s="5" t="str">
+        <v/>
+      </c>
+      <c r="R36" s="5" t="str">
+        <v/>
+      </c>
+      <c r="S36" s="5" t="str">
+        <v>Right</v>
+      </c>
+      <c r="T36" s="5" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1581,7 +1484,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1603,9 +1506,9 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="e">
-        <f ca="1">_xll.xloConcat(,I5,J5,K5)</f>
-        <v>#VALUE!</v>
+      <c r="B5" s="5" t="str">
+        <f>_xll.xloConcat(,I5,J5,K5)</f>
+        <v>FooBarBaz</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1641,9 +1544,9 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="e">
-        <f ca="1">_xll.xloConcat(",",I5:K5)</f>
-        <v>#VALUE!</v>
+      <c r="B8" s="5" t="str">
+        <f>_xll.xloConcat(",",I5:K5)</f>
+        <v>Foo,Bar,Baz</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1661,9 +1564,9 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="e">
-        <f ca="1">_xll.xloConcat("…",I5:I8,J5,K5)</f>
-        <v>#VALUE!</v>
+      <c r="B11" s="5" t="str">
+        <f>_xll.xloConcat("…",I5:I8,J5,K5)</f>
+        <v>Foo…Green…Eggs…Ham…Bar…Baz</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1676,9 +1579,9 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="e">
-        <f ca="1">_xll.xloConcat("---", I5:I8, _xll.xloConcat(",",J6:J8),J5:K5)</f>
-        <v>#VALUE!</v>
+      <c r="B14" s="5" t="str">
+        <f>_xll.xloConcat("---", I5:I8, _xll.xloConcat(",",J6:J8),J5:K5)</f>
+        <v>Foo---Green---Eggs---Ham---1,2,3---Bar---Baz</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1689,42 +1592,36 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="e">
-        <f t="array" aca="1" ref="B21:H21" ca="1">TRANSPOSE(_xll.xloSplit(B14,"-"))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B21" s="5" t="str">
+        <f t="array" ref="B21:H21">TRANSPOSE(_xll.xloSplit(B14,"-"))</f>
+        <v>Foo</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="F21" s="5" t="str">
+        <v>1,2,3</v>
+      </c>
+      <c r="G21" s="5" t="str">
+        <v>Bar</v>
+      </c>
+      <c r="H21" s="5" t="str">
+        <v>Baz</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -1754,45 +1651,44 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="12" t="e">
-        <f ca="1">B21=B22</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C23" s="12" t="e">
-        <f t="shared" ref="C23:H23" ca="1" si="0">C21=C22</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D23" s="12" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E23" s="12" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#VALUE!</v>
+      <c r="B23" s="12" t="b">
+        <f>B21=B22</f>
+        <v>1</v>
+      </c>
+      <c r="C23" s="12" t="b">
+        <f t="shared" ref="C23:H23" si="0">C21=C22</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="12" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H23" s="12" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#VALUE!</v>
+      <c r="G23" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="e">
-        <f t="array" aca="1" ref="B27:C30" ca="1">_xll.xloSplit(I5:I8,"e")</f>
-        <v>#VALUE!</v>
+      <c r="B27" s="5" t="str">
+        <f t="array" ref="B27:C30">_xll.xloSplit(I5:I8,"e")</f>
+        <v>Foo</v>
       </c>
       <c r="C27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
@@ -1800,47 +1696,43 @@
       <c r="F27" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G27" s="12" t="e">
-        <f ca="1">E27=B27</f>
-        <v>#VALUE!</v>
+      <c r="G27" s="12" t="b">
+        <f>E27=B27</f>
+        <v>1</v>
       </c>
       <c r="H27" s="12" t="b">
-        <f ca="1">ISNA(C27)</f>
-        <v>0</v>
+        <f>ISNA(C27)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B28" s="5" t="str">
+        <v>Gr</v>
+      </c>
+      <c r="C28" s="5" t="str">
+        <v>n</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="12" t="e">
-        <f t="shared" ref="G28:G30" ca="1" si="1">E28=B28</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H28" s="12" t="e">
-        <f t="shared" ref="H28" ca="1" si="2">F28=C28</f>
-        <v>#VALUE!</v>
+        <v>50</v>
+      </c>
+      <c r="G28" s="12" t="b">
+        <f t="shared" ref="G28:G30" si="1">E28=B28</f>
+        <v>1</v>
+      </c>
+      <c r="H28" s="12" t="b">
+        <f t="shared" ref="H28" si="2">F28=C28</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B29" s="5" t="str">
+        <v>Eggs</v>
       </c>
       <c r="C29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E29" t="s">
         <v>23</v>
@@ -1848,23 +1740,21 @@
       <c r="F29" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G29" s="12" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G29" s="12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H29" s="12" t="b">
-        <f ca="1">ISNA(C29)</f>
-        <v>0</v>
+        <f>ISNA(C29)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B30" s="5" t="str">
+        <v>Ham</v>
       </c>
       <c r="C30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="E30" t="s">
         <v>21</v>
@@ -1872,70 +1762,65 @@
       <c r="F30" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G30" s="12" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#VALUE!</v>
+      <c r="G30" s="12" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H30" s="12" t="b">
-        <f ca="1">ISNA(C30)</f>
-        <v>0</v>
+        <f>ISNA(C30)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="e">
-        <f t="array" aca="1" ref="B34:D35" ca="1">_xll.xloSplit(I5:K5,"a")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E34" s="12" t="e">
-        <f ca="1">B36=B34</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F34" s="12" t="e">
-        <f t="shared" ref="F34:G34" ca="1" si="3">C36=C34</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G34" s="12" t="e">
-        <f t="shared" ca="1" si="3"/>
-        <v>#VALUE!</v>
+      <c r="B34" s="5" t="str">
+        <f t="array" ref="B34:D35">_xll.xloSplit(I5:K5,"a")</f>
+        <v>Foo</v>
+      </c>
+      <c r="C34" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="D34" s="5" t="str">
+        <v>B</v>
+      </c>
+      <c r="E34" s="12" t="b">
+        <f>B36=B34</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="12" t="b">
+        <f t="shared" ref="F34:G34" si="3">C36=C34</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="12" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <v>r</v>
+      </c>
+      <c r="D35" s="5" t="str">
+        <v>z</v>
       </c>
       <c r="E35" s="12" t="b">
         <f>ISNA(B37)</f>
         <v>1</v>
       </c>
-      <c r="F35" s="12" t="e">
-        <f t="shared" ref="F35" ca="1" si="4">C37=C35</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G35" s="12" t="e">
-        <f t="shared" ref="G35" ca="1" si="5">D37=D35</f>
-        <v>#VALUE!</v>
+      <c r="F35" s="12" t="b">
+        <f t="shared" ref="F35" si="4">C37=C35</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="12" t="b">
+        <f t="shared" ref="G35" si="5">D37=D35</f>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
@@ -1954,54 +1839,52 @@
         <v>#N/A</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>1</v>
       </c>
-      <c r="C40" s="5" t="e">
-        <f t="array" aca="1" ref="C40:C42" ca="1">_xll.xloSplit(B40:B42,"x")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E40" s="12" t="e">
-        <f ca="1">C40=B40</f>
-        <v>#VALUE!</v>
+      <c r="C40" s="5">
+        <f t="array" ref="C40:C42">_xll.xloSplit(B40:B42,"x")</f>
+        <v>1</v>
+      </c>
+      <c r="E40" s="12" t="b">
+        <f>C40=B40</f>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>2</v>
       </c>
-      <c r="C41" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E41" s="12" t="e">
-        <f t="shared" ref="E41:E42" ca="1" si="6">C41=B41</f>
-        <v>#VALUE!</v>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
+      <c r="E41" s="12" t="b">
+        <f t="shared" ref="E41:E42" si="6">C41=B41</f>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>3</v>
       </c>
-      <c r="C42" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E42" s="12" t="e">
-        <f t="shared" ca="1" si="6"/>
-        <v>#VALUE!</v>
+      <c r="C42" s="5">
+        <v>3</v>
+      </c>
+      <c r="E42" s="12" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2015,16 +1898,18 @@
   <dimension ref="B2:V107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" customWidth="1"/>
-    <col min="10" max="10" width="4.6640625" customWidth="1"/>
+    <col min="10" max="10" width="2.109375" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" customWidth="1"/>
     <col min="12" max="12" width="2.44140625" customWidth="1"/>
     <col min="14" max="14" width="3" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
     <col min="16" max="16" width="2.33203125" customWidth="1"/>
     <col min="18" max="18" width="4.5546875" customWidth="1"/>
   </cols>
@@ -2034,64 +1919,77 @@
         <v>38</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="S2" s="11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.3">
       <c r="K3" s="3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="V3" s="9"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="e">
-        <f t="array" ref="B4" ca="1">AND(B19:C25=B40:C46)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C4" s="12" t="e">
-        <f t="array" ref="C4" ca="1">AND(E19:F25=B40:C46)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D4" s="12" t="e">
-        <f t="array" ref="D4" ca="1">AND(H19:I25=B40:C46)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E4" s="12" t="e">
-        <f t="array" ref="E4" ca="1">AND(B30:C36=B48:C54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F4" s="12" t="e">
-        <f t="array" ref="F4" ca="1">AND(E30:F36=B48:C54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G4" s="12" t="e">
-        <f t="array" ref="G4" ca="1">AND(H30:I36=B48:C54)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K4" s="12" t="e">
-        <f t="array" aca="1" ref="K4" ca="1">AND(IFERROR(K22:K34=K40:K52,ERROR.TYPE(K22:K34)=ERROR.TYPE(K40:K52)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M4" s="12" t="e">
-        <f t="array" aca="1" ref="M4" ca="1">AND(IFERROR(M22:M34=M40:M52,ERROR.TYPE(M22:M34)=ERROR.TYPE(M40:M52)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O4" s="12" t="e">
-        <f t="array" aca="1" ref="O4" ca="1">AND(IFERROR(O22:O34=K40:K52,ERROR.TYPE(O22:O34)=ERROR.TYPE(K40:K52)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q4" s="12" t="e">
-        <f t="array" aca="1" ref="Q4" ca="1">AND(IFERROR(Q22:Q34=K40:K52,ERROR.TYPE(Q22:Q34)=ERROR.TYPE(K40:K52)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S4" s="12" t="e">
+      <c r="B4" s="12" t="b">
+        <f t="array" ref="B4">AND(B19:C25=B40:C46)</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="b">
+        <f t="array" ref="C4">AND(E19:F25=B40:C46)</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="b">
+        <f t="array" ref="D4">AND(H19:I25=B40:C46)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="12" t="b">
+        <f t="array" ref="E4">AND(B30:C36=B48:C54)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="b">
+        <f t="array" ref="F4">AND(E30:F36=B48:C54)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="12" t="b">
+        <f t="array" ref="G4">AND(H30:I36=B48:C54)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="12" t="b">
+        <f t="array" ref="K4">AND(IFERROR(K22:K34=K40:K52,ERROR.TYPE(K22:K34)=ERROR.TYPE(K40:K52)))</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="12" t="b">
+        <f t="array" ref="M4">AND(IFERROR(M22:M34=M40:M52,ERROR.TYPE(M22:M34)=ERROR.TYPE(M40:M52)))</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="12" t="b">
+        <f t="array" ref="O4">AND(IFERROR(O22:O34=K40:K52,ERROR.TYPE(O22:O34)=ERROR.TYPE(K40:K52)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="12" t="b">
+        <f>AND(IFERROR(Q22:Q34=M40:M52,ERROR.TYPE(Q22:Q34)=ERROR.TYPE(M40:M52)))</f>
+        <v>1</v>
+      </c>
+      <c r="S4" s="12" t="b">
         <f ca="1">AND(T8=MIN(S8:S107),T107=MAX(S8:S107))</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
@@ -2126,11 +2024,11 @@
       </c>
       <c r="S8" s="7">
         <f ca="1">RAND()</f>
-        <v>2.7883143734199756E-3</v>
-      </c>
-      <c r="T8" s="4" t="e">
+        <v>6.0755901780086274E-3</v>
+      </c>
+      <c r="T8" s="4">
         <f t="array" aca="1" ref="T8:T107" ca="1">_xll.xloSort(S8:S107,"a")</f>
-        <v>#VALUE!</v>
+        <v>4.4892519097212702E-3</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
@@ -2146,9 +2044,9 @@
       <c r="S9" s="7">
         <v>1.4241351279182801E-2</v>
       </c>
-      <c r="T9" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T9" s="4">
+        <f ca="1"/>
+        <v>6.0755901780086274E-3</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
@@ -2164,9 +2062,9 @@
       <c r="S10" s="7">
         <v>0.11987234330114915</v>
       </c>
-      <c r="T10" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T10" s="4">
+        <f ca="1"/>
+        <v>8.9705088996498983E-3</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
@@ -2182,9 +2080,9 @@
       <c r="S11" s="7">
         <v>0.43199912726020961</v>
       </c>
-      <c r="T11" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T11" s="4">
+        <f ca="1"/>
+        <v>1.0142003022623358E-2</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
@@ -2201,9 +2099,9 @@
       <c r="S12" s="7">
         <v>0.44362993322818001</v>
       </c>
-      <c r="T12" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T12" s="4">
+        <f ca="1"/>
+        <v>1.4241351279182801E-2</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
@@ -2220,9 +2118,9 @@
       <c r="S13" s="7">
         <v>0.70719203131190667</v>
       </c>
-      <c r="T13" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T13" s="4">
+        <f ca="1"/>
+        <v>1.7278225187227991E-2</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
@@ -2238,9 +2136,9 @@
       <c r="S14" s="7">
         <v>0.28303369927876221</v>
       </c>
-      <c r="T14" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T14" s="4">
+        <f ca="1"/>
+        <v>4.2989156379268589E-2</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
@@ -2250,21 +2148,21 @@
       <c r="S15" s="7">
         <v>0.18684151297687135</v>
       </c>
-      <c r="T15" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T15" s="4">
+        <f ca="1"/>
+        <v>4.8199686141203735E-2</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="18"/>
       <c r="E16" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>39</v>
@@ -2272,33 +2170,32 @@
       <c r="S16" s="7">
         <v>7.6545233242765964E-2</v>
       </c>
-      <c r="T16" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T16" s="4">
+        <f ca="1"/>
+        <v>5.2437735118262885E-2</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
       <c r="K17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="S17" s="7">
         <v>0.78402600397426425</v>
       </c>
-      <c r="T17" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T17" s="4">
+        <f ca="1"/>
+        <v>6.063738431260568E-2</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="E18" t="e">
-        <f t="array" aca="1" ref="E18:F25" ca="1">_xll.xloSort(B7:C14,"a","Words")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E18" t="str">
+        <f t="array" ref="E18:F25">_xll.xloSort(B7:C14,"a","Words")</f>
+        <v>Words</v>
+      </c>
+      <c r="F18" t="str">
+        <v>Numbers</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>40</v>
@@ -2306,35 +2203,31 @@
       <c r="S18" s="7">
         <v>0.5992299667126384</v>
       </c>
-      <c r="T18" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T18" s="4">
+        <f ca="1"/>
+        <v>7.6545233242765964E-2</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="e">
-        <f t="array" aca="1" ref="B19:C25" ca="1">_xll.xloSort(B8:C14,"a",1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C19" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F19" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H19" s="5" t="e">
-        <f t="array" aca="1" ref="H19:I25" ca="1">_xll.xloSort(_xll.xloRef(B8:C14),"a",1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B19" s="5" t="str">
+        <f t="array" ref="B19:C25">_xll.xloSort(B8:C14,"a",1)</f>
+        <v>Box</v>
+      </c>
+      <c r="C19" s="5">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5" t="str">
+        <v>Box</v>
+      </c>
+      <c r="F19" s="5">
+        <v>7</v>
+      </c>
+      <c r="H19" s="5" t="str">
+        <f t="array" ref="H19:I25">_xll.xloSort(_xll.xloRef(B8:C14),"a",1)</f>
+        <v>Box</v>
+      </c>
+      <c r="I19" s="5">
+        <v>7</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>41</v>
@@ -2342,35 +2235,29 @@
       <c r="S19" s="7">
         <v>0.21129177216442607</v>
       </c>
-      <c r="T19" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T19" s="4">
+        <f ca="1"/>
+        <v>9.6043732044653662E-2</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I20" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B20" s="5" t="str">
+        <v>BOX</v>
+      </c>
+      <c r="C20" s="5">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5" t="str">
+        <v>BOX</v>
+      </c>
+      <c r="F20" s="5">
+        <v>8</v>
+      </c>
+      <c r="H20" s="5" t="str">
+        <v>BOX</v>
+      </c>
+      <c r="I20" s="5">
+        <v>8</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>42</v>
@@ -2378,1480 +2265,1358 @@
       <c r="S20" s="7">
         <v>0.56907031356613658</v>
       </c>
-      <c r="T20" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T20" s="4">
+        <f ca="1"/>
+        <v>0.10466409270245647</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I21" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>69</v>
+      <c r="B21" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="C21" s="5">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3</v>
+      </c>
+      <c r="H21" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="I21" s="5">
+        <v>3</v>
       </c>
       <c r="P21" s="3"/>
       <c r="S21" s="7">
         <v>0.70052257146975117</v>
       </c>
-      <c r="T21" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T21" s="4">
+        <f ca="1"/>
+        <v>0.11099657306935851</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I22" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K22" s="5" t="e">
-        <f t="array" aca="1" ref="K22:K34" ca="1">_xll.xloSort(K8:K20,"a",1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M22" s="5" t="e">
-        <f t="array" aca="1" ref="M22:M34" ca="1">_xll.xloSort(K8:K20,"A",1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O22" s="5" t="e">
-        <f t="array" aca="1" ref="O22:O34" ca="1">_xll.xloSort(_xll.xloRef(K8:K20),"a",1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q22" s="5" t="e">
-        <f t="array" aca="1" ref="Q22:Q34" ca="1">_xll.xloSort(_xll.xloRef(K8:K20),"A",1)</f>
-        <v>#VALUE!</v>
+      <c r="B22" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="H22" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="I22" s="5">
+        <v>3</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="array" ref="K22:K34">_xll.xloSort(K8:K20,"a",1)</f>
+        <v>4</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="array" ref="M22:M34">_xll.xloSort(K8:K20,"A",1)</f>
+        <v>4</v>
+      </c>
+      <c r="O22" s="5">
+        <f t="array" ref="O22:O34">_xll.xloSort(_xll.xloRef(K8:K20),"a",1)</f>
+        <v>4</v>
+      </c>
+      <c r="Q22" s="5">
+        <f t="array" ref="Q22:Q34">_xll.xloSort(_xll.xloRef(K8:K20),"A",1)</f>
+        <v>4</v>
       </c>
       <c r="S22" s="7">
         <v>0.96985704312068066</v>
       </c>
-      <c r="T22" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T22" s="4">
+        <f ca="1"/>
+        <v>0.11987234330114915</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q23" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B23" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="I23" s="5">
+        <v>1</v>
+      </c>
+      <c r="K23" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="M23" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="O23" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>6.2</v>
       </c>
       <c r="S23" s="7">
         <v>0.55553726039846762</v>
       </c>
-      <c r="T23" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T23" s="4">
+        <f ca="1"/>
+        <v>0.15138392223952224</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q24" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B24" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="C24" s="5">
+        <v>3</v>
+      </c>
+      <c r="E24" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="F24" s="5">
+        <v>3</v>
+      </c>
+      <c r="H24" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="I24" s="5">
+        <v>3</v>
+      </c>
+      <c r="K24" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="M24" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="O24" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>6.3</v>
       </c>
       <c r="S24" s="7">
         <v>0.346644941363903</v>
       </c>
-      <c r="T24" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T24" s="4">
+        <f ca="1"/>
+        <v>0.15285256271102787</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q25" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B25" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="C25" s="5">
+        <v>4</v>
+      </c>
+      <c r="E25" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="F25" s="5">
+        <v>4</v>
+      </c>
+      <c r="H25" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="I25" s="5">
+        <v>4</v>
+      </c>
+      <c r="K25" s="5">
+        <v>7</v>
+      </c>
+      <c r="M25" s="5">
+        <v>7</v>
+      </c>
+      <c r="O25" s="5">
+        <v>7</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>7</v>
       </c>
       <c r="S25" s="7">
         <v>0.86284631971635639</v>
       </c>
-      <c r="T25" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T25" s="4">
+        <f ca="1"/>
+        <v>0.15935651729819933</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="K26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q26" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="K26" s="5" t="str">
+        <v>Foo</v>
+      </c>
+      <c r="M26" s="5" t="str">
+        <v>FOO</v>
+      </c>
+      <c r="O26" s="5" t="str">
+        <v>Foo</v>
+      </c>
+      <c r="Q26" s="5" t="str">
+        <v>FOO</v>
       </c>
       <c r="S26" s="7">
         <v>0.25958386357364216</v>
       </c>
-      <c r="T26" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T26" s="4">
+        <f ca="1"/>
+        <v>0.16534127039316493</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B27" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="17"/>
+      <c r="B27" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="18"/>
       <c r="E27" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="K27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q27" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>67</v>
+      </c>
+      <c r="K27" s="5" t="str">
+        <v>FOO</v>
+      </c>
+      <c r="M27" s="5" t="str">
+        <v>FOOD</v>
+      </c>
+      <c r="O27" s="5" t="str">
+        <v>FOO</v>
+      </c>
+      <c r="Q27" s="5" t="str">
+        <v>FOOD</v>
       </c>
       <c r="S27" s="7">
         <v>0.44578595954200495</v>
       </c>
-      <c r="T27" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T27" s="4">
+        <f ca="1"/>
+        <v>0.18684151297687135</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="K28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q28" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="K28" s="5" t="str">
+        <v>Food</v>
+      </c>
+      <c r="M28" s="5" t="str">
+        <v>Foo</v>
+      </c>
+      <c r="O28" s="5" t="str">
+        <v>Food</v>
+      </c>
+      <c r="Q28" s="5" t="str">
+        <v>Foo</v>
       </c>
       <c r="S28" s="7">
         <v>0.35070608842246354</v>
       </c>
-      <c r="T28" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T28" s="4">
+        <f ca="1"/>
+        <v>0.19150797219437865</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="E29" t="e">
-        <f t="array" aca="1" ref="E29:F36" ca="1">_xll.xloSort(B7:C14,"d a","Numbers","Words")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F29" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q29" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="E29" t="str">
+        <f t="array" ref="E29:F36">_xll.xloSort(B7:C14,"d a","Numbers","Words")</f>
+        <v>Words</v>
+      </c>
+      <c r="F29" t="str">
+        <v>Numbers</v>
+      </c>
+      <c r="K29" s="5" t="str">
+        <v>FOOD</v>
+      </c>
+      <c r="M29" s="5" t="str">
+        <v>FooDs</v>
+      </c>
+      <c r="O29" s="5" t="str">
+        <v>FOOD</v>
+      </c>
+      <c r="Q29" s="5" t="str">
+        <v>FooDs</v>
       </c>
       <c r="S29" s="7">
         <v>0.97062641299883634</v>
       </c>
-      <c r="T29" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T29" s="4">
+        <f ca="1"/>
+        <v>0.19332448079141096</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B30" s="5" t="e">
-        <f t="array" aca="1" ref="B30:C36" ca="1">_xll.xloSort(B8:C14,"d a",2,1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H30" s="5" t="e">
-        <f t="array" aca="1" ref="H30:I36" ca="1">_xll.xloSort(_xll.xloRef(B8:C14),"d a",2,1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q30" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B30" s="5" t="str">
+        <f t="array" ref="B30:C36">_xll.xloSort(B8:C14,"d a",2,1)</f>
+        <v>BOX</v>
+      </c>
+      <c r="C30" s="5">
+        <v>8</v>
+      </c>
+      <c r="E30" s="5" t="str">
+        <v>BOX</v>
+      </c>
+      <c r="F30" s="5">
+        <v>8</v>
+      </c>
+      <c r="H30" s="5" t="str">
+        <f t="array" ref="H30:I36">_xll.xloSort(_xll.xloRef(B8:C14),"d a",2,1)</f>
+        <v>BOX</v>
+      </c>
+      <c r="I30" s="5">
+        <v>8</v>
+      </c>
+      <c r="K30" s="5" t="str">
+        <v>FooDs</v>
+      </c>
+      <c r="M30" s="5" t="str">
+        <v>Food</v>
+      </c>
+      <c r="O30" s="5" t="str">
+        <v>FooDs</v>
+      </c>
+      <c r="Q30" s="5" t="str">
+        <v>Food</v>
       </c>
       <c r="S30" s="7">
         <v>0.36303952239766712</v>
       </c>
-      <c r="T30" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T30" s="4">
+        <f ca="1"/>
+        <v>0.20455886903305909</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q31" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B31" s="5" t="str">
+        <v>Box</v>
+      </c>
+      <c r="C31" s="5">
+        <v>7</v>
+      </c>
+      <c r="E31" s="5" t="str">
+        <v>Box</v>
+      </c>
+      <c r="F31" s="5">
+        <v>7</v>
+      </c>
+      <c r="H31" s="5" t="str">
+        <v>Box</v>
+      </c>
+      <c r="I31" s="5">
+        <v>7</v>
+      </c>
+      <c r="K31" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="M31" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="O31" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="Q31" s="5" t="str">
+        <v>Green</v>
       </c>
       <c r="S31" s="7">
         <v>0.35500379302962237</v>
       </c>
-      <c r="T31" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T31" s="4">
+        <f ca="1"/>
+        <v>0.21129177216442607</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q32" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B32" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="C32" s="5">
+        <v>4</v>
+      </c>
+      <c r="E32" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="F32" s="5">
+        <v>4</v>
+      </c>
+      <c r="H32" s="5" t="str">
+        <v>Sam</v>
+      </c>
+      <c r="I32" s="5">
+        <v>4</v>
+      </c>
+      <c r="K32" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="M32" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="O32" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="Q32" s="5" t="str">
+        <v>Ham</v>
       </c>
       <c r="S32" s="7">
         <v>0.30991009987247375</v>
       </c>
-      <c r="T32" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T32" s="4">
+        <f ca="1"/>
+        <v>0.21289020404938441</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B33" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="C33" s="5">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="F33" s="5">
+        <v>3</v>
+      </c>
+      <c r="H33" s="5" t="str">
+        <v>Eggs</v>
+      </c>
+      <c r="I33" s="5">
+        <v>3</v>
       </c>
       <c r="K33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#NAME?</v>
       </c>
       <c r="M33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#NAME?</v>
       </c>
       <c r="O33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#NAME?</v>
       </c>
       <c r="Q33" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#NAME?</v>
       </c>
       <c r="S33" s="7">
         <v>0.50309865693105404</v>
       </c>
-      <c r="T33" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T33" s="4">
+        <f ca="1"/>
+        <v>0.24005046089105242</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B34" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
+      <c r="E34" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="F34" s="5">
+        <v>3</v>
+      </c>
+      <c r="H34" s="5" t="str">
+        <v>Fox</v>
+      </c>
+      <c r="I34" s="5">
+        <v>3</v>
       </c>
       <c r="K34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="M34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="O34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="Q34" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>#N/A</v>
       </c>
       <c r="S34" s="7">
         <v>0.24683784713265966</v>
       </c>
-      <c r="T34" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T34" s="4">
+        <f ca="1"/>
+        <v>0.24683784713265966</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I35" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B35" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="E35" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="F35" s="5">
+        <v>3</v>
+      </c>
+      <c r="H35" s="5" t="str">
+        <v>Ham</v>
+      </c>
+      <c r="I35" s="5">
+        <v>3</v>
       </c>
       <c r="S35" s="7">
         <v>0.21289020404938441</v>
       </c>
-      <c r="T35" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T35" s="4">
+        <f ca="1"/>
+        <v>0.25090708805825079</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I36" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="B36" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5" t="str">
+        <v>Green</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1</v>
       </c>
       <c r="S36" s="7">
         <v>0.57712158377157863</v>
       </c>
-      <c r="T36" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T36" s="4">
+        <f ca="1"/>
+        <v>0.25958386357364216</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S37" s="7">
         <v>6.063738431260568E-2</v>
       </c>
-      <c r="T37" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T37" s="4">
+        <f ca="1"/>
+        <v>0.26026766796149603</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="S38" s="7">
         <v>0.37822251634842252</v>
       </c>
-      <c r="T38" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T38" s="4">
+        <f ca="1"/>
+        <v>0.2819709570143808</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S39" s="7">
         <v>0.60977631212733274</v>
       </c>
-      <c r="T39" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T39" s="4">
+        <f ca="1"/>
+        <v>0.28303369927876221</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="17">
         <v>7</v>
       </c>
-      <c r="K40" s="18">
+      <c r="K40" s="17">
         <v>4</v>
       </c>
-      <c r="M40" s="18">
+      <c r="M40" s="17">
         <v>4</v>
       </c>
       <c r="S40" s="7">
         <v>0.20455886903305909</v>
       </c>
-      <c r="T40" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T40" s="4">
+        <f ca="1"/>
+        <v>0.29579294051174709</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="17">
         <v>8</v>
       </c>
-      <c r="K41" s="18">
+      <c r="K41" s="17">
         <v>6.2</v>
       </c>
-      <c r="M41" s="18">
+      <c r="M41" s="17">
         <v>6.2</v>
       </c>
       <c r="S41" s="7">
         <v>0.947318592329083</v>
       </c>
-      <c r="T41" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T41" s="4">
+        <f ca="1"/>
+        <v>0.30621594261281582</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="17">
         <v>3</v>
       </c>
-      <c r="K42" s="18">
+      <c r="K42" s="17">
         <v>6.3</v>
       </c>
-      <c r="M42" s="18">
+      <c r="M42" s="17">
         <v>6.3</v>
       </c>
       <c r="S42" s="7">
         <v>0.68147699048550281</v>
       </c>
-      <c r="T42" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T42" s="4">
+        <f ca="1"/>
+        <v>0.30699880764121135</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C43" s="18">
+      <c r="C43" s="17">
         <v>3</v>
       </c>
-      <c r="K43" s="18">
+      <c r="K43" s="17">
         <v>7</v>
       </c>
-      <c r="M43" s="18">
+      <c r="M43" s="17">
         <v>7</v>
       </c>
       <c r="S43" s="7">
         <v>0.90600850571232516</v>
       </c>
-      <c r="T43" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T43" s="4">
+        <f ca="1"/>
+        <v>0.30746381468864881</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="18">
-        <v>1</v>
-      </c>
-      <c r="K44" s="18" t="s">
+      <c r="C44" s="17">
+        <v>1</v>
+      </c>
+      <c r="K44" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="M44" s="18" t="s">
+      <c r="M44" s="17" t="s">
         <v>40</v>
       </c>
       <c r="S44" s="7">
         <v>0.85960749899325406</v>
       </c>
-      <c r="T44" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T44" s="4">
+        <f ca="1"/>
+        <v>0.30991009987247375</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="17">
         <v>3</v>
       </c>
-      <c r="K45" s="18" t="s">
+      <c r="K45" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="M45" s="18" t="s">
+      <c r="M45" s="17" t="s">
         <v>41</v>
       </c>
       <c r="S45" s="7">
         <v>4.2989156379268589E-2</v>
       </c>
-      <c r="T45" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T45" s="4">
+        <f ca="1"/>
+        <v>0.34322350221251363</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C46" s="18">
+      <c r="C46" s="17">
         <v>4</v>
       </c>
-      <c r="K46" s="18" t="s">
+      <c r="K46" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="M46" s="18" t="s">
+      <c r="M46" s="17" t="s">
         <v>18</v>
       </c>
       <c r="S46" s="7">
         <v>0.15285256271102787</v>
       </c>
-      <c r="T46" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T46" s="4">
+        <f ca="1"/>
+        <v>0.346644941363903</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="K47" s="18" t="s">
+      <c r="K47" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M47" s="18" t="s">
+      <c r="M47" s="17" t="s">
         <v>42</v>
       </c>
       <c r="S47" s="7">
         <v>4.4892519097212702E-3</v>
       </c>
-      <c r="T47" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T47" s="4">
+        <f ca="1"/>
+        <v>0.35070608842246354</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="18">
+      <c r="C48" s="17">
         <v>8</v>
       </c>
-      <c r="K48" s="18" t="s">
+      <c r="K48" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="M48" s="18" t="s">
+      <c r="M48" s="17" t="s">
         <v>39</v>
       </c>
       <c r="S48" s="7">
         <v>9.6043732044653662E-2</v>
       </c>
-      <c r="T48" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T48" s="4">
+        <f ca="1"/>
+        <v>0.35500379302962237</v>
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B49" s="18" t="s">
+      <c r="B49" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="17">
         <v>7</v>
       </c>
-      <c r="K49" s="18" t="s">
+      <c r="K49" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="M49" s="18" t="s">
+      <c r="M49" s="17" t="s">
         <v>22</v>
       </c>
       <c r="S49" s="7">
         <v>0.30746381468864881</v>
       </c>
-      <c r="T49" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T49" s="4">
+        <f ca="1"/>
+        <v>0.36303952239766712</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C50" s="17">
         <v>4</v>
       </c>
-      <c r="K50" s="18" t="s">
+      <c r="K50" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="M50" s="18" t="s">
+      <c r="M50" s="17" t="s">
         <v>21</v>
       </c>
       <c r="S50" s="7">
         <v>0.15935651729819933</v>
       </c>
-      <c r="T50" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T50" s="4">
+        <f ca="1"/>
+        <v>0.37590154211670712</v>
       </c>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="17">
         <v>3</v>
       </c>
-      <c r="K51" s="18" t="e">
+      <c r="K51" s="17" t="e">
         <v>#NAME?</v>
       </c>
-      <c r="M51" s="18" t="e">
+      <c r="M51" s="17" t="e">
         <v>#NAME?</v>
       </c>
       <c r="S51" s="7">
         <v>0.73492497530386436</v>
       </c>
-      <c r="T51" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T51" s="4">
+        <f ca="1"/>
+        <v>0.37822251634842252</v>
       </c>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C52" s="17">
         <v>3</v>
       </c>
-      <c r="K52" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M52" s="18" t="e">
+      <c r="K52" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M52" s="17" t="e">
         <v>#N/A</v>
       </c>
       <c r="S52" s="7">
         <v>0.93045439034459587</v>
       </c>
-      <c r="T52" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T52" s="4">
+        <f ca="1"/>
+        <v>0.38122419173045929</v>
       </c>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="17">
         <v>3</v>
       </c>
       <c r="S53" s="7">
         <v>0.70064205520622802</v>
       </c>
-      <c r="T53" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T53" s="4">
+        <f ca="1"/>
+        <v>0.38693032613344891</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C54" s="17">
         <v>1</v>
       </c>
       <c r="S54" s="7">
         <v>0.34322350221251363</v>
       </c>
-      <c r="T54" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T54" s="4">
+        <f ca="1"/>
+        <v>0.38924117354343202</v>
       </c>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S55" s="7">
         <v>0.30699880764121135</v>
       </c>
-      <c r="T55" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T55" s="4">
+        <f ca="1"/>
+        <v>0.41032128248045219</v>
       </c>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S56" s="7">
         <v>0.56072877256876819</v>
       </c>
-      <c r="T56" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T56" s="4">
+        <f ca="1"/>
+        <v>0.43199912726020961</v>
       </c>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S57" s="7">
         <v>1.0142003022623358E-2</v>
       </c>
-      <c r="T57" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T57" s="4">
+        <f ca="1"/>
+        <v>0.44362993322818001</v>
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S58" s="7">
         <v>0.38122419173045929</v>
       </c>
-      <c r="T58" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T58" s="4">
+        <f ca="1"/>
+        <v>0.44578595954200495</v>
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S59" s="7">
         <v>0.60411978716231773</v>
       </c>
-      <c r="T59" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T59" s="4">
+        <f ca="1"/>
+        <v>0.50309865693105404</v>
       </c>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S60" s="7">
         <v>0.2819709570143808</v>
       </c>
-      <c r="T60" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T60" s="4">
+        <f ca="1"/>
+        <v>0.55553726039846762</v>
       </c>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S61" s="7">
         <v>0.58507289523339523</v>
       </c>
-      <c r="T61" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T61" s="4">
+        <f ca="1"/>
+        <v>0.56072877256876819</v>
       </c>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S62" s="7">
         <v>0.38693032613344891</v>
       </c>
-      <c r="T62" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T62" s="4">
+        <f ca="1"/>
+        <v>0.56613202852270661</v>
       </c>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S63" s="7">
         <v>0.38924117354343202</v>
       </c>
-      <c r="T63" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T63" s="4">
+        <f ca="1"/>
+        <v>0.56907031356613658</v>
       </c>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S64" s="7">
         <v>0.25090708805825079</v>
       </c>
-      <c r="T64" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T64" s="4">
+        <f ca="1"/>
+        <v>0.57665750527755044</v>
       </c>
     </row>
     <row r="65" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S65" s="7">
         <v>0.99561513362173215</v>
       </c>
-      <c r="T65" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T65" s="4">
+        <f ca="1"/>
+        <v>0.57712158377157863</v>
       </c>
     </row>
     <row r="66" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S66" s="7">
         <v>0.41032128248045219</v>
       </c>
-      <c r="T66" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T66" s="4">
+        <f ca="1"/>
+        <v>0.58507289523339523</v>
       </c>
     </row>
     <row r="67" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S67" s="7">
         <v>0.10466409270245647</v>
       </c>
-      <c r="T67" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T67" s="4">
+        <f ca="1"/>
+        <v>0.5992299667126384</v>
       </c>
     </row>
     <row r="68" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S68" s="7">
         <v>0.96328079049455895</v>
       </c>
-      <c r="T68" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T68" s="4">
+        <f ca="1"/>
+        <v>0.60411978716231773</v>
       </c>
     </row>
     <row r="69" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S69" s="7">
         <v>0.99946735978378209</v>
       </c>
-      <c r="T69" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T69" s="4">
+        <f ca="1"/>
+        <v>0.60977631212733274</v>
       </c>
     </row>
     <row r="70" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S70" s="7">
         <v>0.82935893028115659</v>
       </c>
-      <c r="T70" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T70" s="4">
+        <f ca="1"/>
+        <v>0.61835596776400625</v>
       </c>
     </row>
     <row r="71" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S71" s="7">
         <v>0.15138392223952224</v>
       </c>
-      <c r="T71" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T71" s="4">
+        <f ca="1"/>
+        <v>0.64226730514312624</v>
       </c>
     </row>
     <row r="72" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S72" s="7">
         <v>0.26026766796149603</v>
       </c>
-      <c r="T72" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T72" s="4">
+        <f ca="1"/>
+        <v>0.64904570666639028</v>
       </c>
     </row>
     <row r="73" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S73" s="7">
         <v>0.56613202852270661</v>
       </c>
-      <c r="T73" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T73" s="4">
+        <f ca="1"/>
+        <v>0.67056525021684998</v>
       </c>
     </row>
     <row r="74" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S74" s="7">
         <v>0.57665750527755044</v>
       </c>
-      <c r="T74" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T74" s="4">
+        <f ca="1"/>
+        <v>0.68147699048550281</v>
       </c>
     </row>
     <row r="75" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S75" s="7">
         <v>0.83938605783476394</v>
       </c>
-      <c r="T75" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T75" s="4">
+        <f ca="1"/>
+        <v>0.70052257146975117</v>
       </c>
     </row>
     <row r="76" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S76" s="7">
         <v>0.37590154211670712</v>
       </c>
-      <c r="T76" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T76" s="4">
+        <f ca="1"/>
+        <v>0.70064205520622802</v>
       </c>
     </row>
     <row r="77" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S77" s="7">
         <v>0.95887267917531893</v>
       </c>
-      <c r="T77" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T77" s="4">
+        <f ca="1"/>
+        <v>0.70719203131190667</v>
       </c>
     </row>
     <row r="78" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S78" s="7">
         <v>0.11099657306935851</v>
       </c>
-      <c r="T78" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T78" s="4">
+        <f ca="1"/>
+        <v>0.71755405184921206</v>
       </c>
     </row>
     <row r="79" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S79" s="7">
         <v>0.67056525021684998</v>
       </c>
-      <c r="T79" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T79" s="4">
+        <f ca="1"/>
+        <v>0.73492497530386436</v>
       </c>
     </row>
     <row r="80" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S80" s="7">
         <v>0.82167610222353549</v>
       </c>
-      <c r="T80" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T80" s="4">
+        <f ca="1"/>
+        <v>0.78402600397426425</v>
       </c>
     </row>
     <row r="81" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S81" s="7">
         <v>0.79626472404113779</v>
       </c>
-      <c r="T81" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T81" s="4">
+        <f ca="1"/>
+        <v>0.79404440245310404</v>
       </c>
     </row>
     <row r="82" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S82" s="7">
         <v>0.79404440245310404</v>
       </c>
-      <c r="T82" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T82" s="4">
+        <f ca="1"/>
+        <v>0.79626472404113779</v>
       </c>
     </row>
     <row r="83" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S83" s="7">
         <v>0.24005046089105242</v>
       </c>
-      <c r="T83" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T83" s="4">
+        <f ca="1"/>
+        <v>0.79852373727417758</v>
       </c>
     </row>
     <row r="84" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S84" s="7">
         <v>1.7278225187227991E-2</v>
       </c>
-      <c r="T84" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T84" s="4">
+        <f ca="1"/>
+        <v>0.82167610222353549</v>
       </c>
     </row>
     <row r="85" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S85" s="7">
         <v>0.83233289115523368</v>
       </c>
-      <c r="T85" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T85" s="4">
+        <f ca="1"/>
+        <v>0.82935893028115659</v>
       </c>
     </row>
     <row r="86" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S86" s="7">
         <v>5.2437735118262885E-2</v>
       </c>
-      <c r="T86" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T86" s="4">
+        <f ca="1"/>
+        <v>0.83233289115523368</v>
       </c>
     </row>
     <row r="87" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S87" s="7">
         <v>0.79852373727417758</v>
       </c>
-      <c r="T87" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T87" s="4">
+        <f ca="1"/>
+        <v>0.83938605783476394</v>
       </c>
     </row>
     <row r="88" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S88" s="7">
         <v>0.88056162198032462</v>
       </c>
-      <c r="T88" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T88" s="4">
+        <f ca="1"/>
+        <v>0.85960749899325406</v>
       </c>
     </row>
     <row r="89" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S89" s="7">
         <v>0.29579294051174709</v>
       </c>
-      <c r="T89" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T89" s="4">
+        <f ca="1"/>
+        <v>0.86081826465673084</v>
       </c>
     </row>
     <row r="90" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S90" s="7">
         <v>0.71755405184921206</v>
       </c>
-      <c r="T90" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T90" s="4">
+        <f ca="1"/>
+        <v>0.86284631971635639</v>
       </c>
     </row>
     <row r="91" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S91" s="7">
         <v>0.97078869366691067</v>
       </c>
-      <c r="T91" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T91" s="4">
+        <f ca="1"/>
+        <v>0.88056162198032462</v>
       </c>
     </row>
     <row r="92" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S92" s="7">
         <v>4.8199686141203735E-2</v>
       </c>
-      <c r="T92" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T92" s="4">
+        <f ca="1"/>
+        <v>0.89299919543294648</v>
       </c>
     </row>
     <row r="93" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S93" s="7">
         <v>0.19150797219437865</v>
       </c>
-      <c r="T93" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T93" s="4">
+        <f ca="1"/>
+        <v>0.90600850571232516</v>
       </c>
     </row>
     <row r="94" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S94" s="7">
         <v>0.19332448079141096</v>
       </c>
-      <c r="T94" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T94" s="4">
+        <f ca="1"/>
+        <v>0.9287334580292661</v>
       </c>
     </row>
     <row r="95" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S95" s="7">
         <v>0.64904570666639028</v>
       </c>
-      <c r="T95" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T95" s="4">
+        <f ca="1"/>
+        <v>0.93045439034459587</v>
       </c>
     </row>
     <row r="96" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S96" s="7">
         <v>0.89299919543294648</v>
       </c>
-      <c r="T96" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T96" s="4">
+        <f ca="1"/>
+        <v>0.947318592329083</v>
       </c>
     </row>
     <row r="97" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S97" s="7">
         <v>0.98357223163047991</v>
       </c>
-      <c r="T97" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T97" s="4">
+        <f ca="1"/>
+        <v>0.94876869372932582</v>
       </c>
     </row>
     <row r="98" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S98" s="7">
         <v>0.95613469316823751</v>
       </c>
-      <c r="T98" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T98" s="4">
+        <f ca="1"/>
+        <v>0.95613469316823751</v>
       </c>
     </row>
     <row r="99" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S99" s="7">
         <v>0.97356891451331928</v>
       </c>
-      <c r="T99" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T99" s="4">
+        <f ca="1"/>
+        <v>0.95887267917531893</v>
       </c>
     </row>
     <row r="100" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S100" s="7">
         <v>0.64226730514312624</v>
       </c>
-      <c r="T100" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T100" s="4">
+        <f ca="1"/>
+        <v>0.96328079049455895</v>
       </c>
     </row>
     <row r="101" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S101" s="7">
         <v>0.61835596776400625</v>
       </c>
-      <c r="T101" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T101" s="4">
+        <f ca="1"/>
+        <v>0.96985704312068066</v>
       </c>
     </row>
     <row r="102" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S102" s="7">
         <v>0.86081826465673084</v>
       </c>
-      <c r="T102" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T102" s="4">
+        <f ca="1"/>
+        <v>0.97062641299883634</v>
       </c>
     </row>
     <row r="103" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S103" s="7">
         <v>0.16534127039316493</v>
       </c>
-      <c r="T103" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T103" s="4">
+        <f ca="1"/>
+        <v>0.97078869366691067</v>
       </c>
     </row>
     <row r="104" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S104" s="7">
         <v>0.9287334580292661</v>
       </c>
-      <c r="T104" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T104" s="4">
+        <f ca="1"/>
+        <v>0.97356891451331928</v>
       </c>
     </row>
     <row r="105" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S105" s="7">
         <v>8.9705088996498983E-3</v>
       </c>
-      <c r="T105" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T105" s="4">
+        <f ca="1"/>
+        <v>0.98357223163047991</v>
       </c>
     </row>
     <row r="106" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S106" s="7">
         <v>0.30621594261281582</v>
       </c>
-      <c r="T106" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T106" s="4">
+        <f ca="1"/>
+        <v>0.99561513362173215</v>
       </c>
     </row>
     <row r="107" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S107" s="7">
         <v>0.94876869372932582</v>
       </c>
-      <c r="T107" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="T107" s="4">
+        <f ca="1"/>
+        <v>0.99946735978378209</v>
       </c>
     </row>
   </sheetData>
@@ -3885,27 +3650,25 @@
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="e">
-        <f t="array" ref="C3" ca="1">SUM(0+(F3:H5=K3:M5))=9</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E3" t="e">
-        <f ca="1">_xll.xloRef(K3:M5)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" s="5" t="e">
-        <f t="array" aca="1" ref="F3:H5" ca="1">_xll.xloVal(E3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G3" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H3" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>55</v>
+      </c>
+      <c r="C3" t="b">
+        <f t="array" ref="C3">SUM(0+(F3:H5=K3:M5))=9</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.xloRef(K3:M5)</f>
+        <v>永[00000295DAB333B0]8004:8004,A</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="array" ref="F3:H5">_xll.xloVal(E3)</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3</v>
       </c>
       <c r="K3" s="7">
         <v>1</v>
@@ -3918,17 +3681,14 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F4" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G4" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H4" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6</v>
       </c>
       <c r="K4" s="7">
         <v>4</v>
@@ -3941,17 +3701,14 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F5" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G5" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H5" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="F5" s="5">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5">
+        <v>9</v>
       </c>
       <c r="K5" s="7">
         <v>7</v>
@@ -3965,73 +3722,73 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="e">
-        <f ca="1">D8=E8</f>
-        <v>#VALUE!</v>
+        <v>56</v>
+      </c>
+      <c r="C8" t="b">
+        <f>D8=E8</f>
+        <v>1</v>
       </c>
       <c r="D8">
         <f>INDEX($K$3:$M$5,2,2)</f>
         <v>5</v>
       </c>
-      <c r="E8" t="e">
-        <f ca="1">_xll.xloIndex($E$3,2,2)</f>
-        <v>#VALUE!</v>
+      <c r="E8">
+        <f>_xll.xloIndex($E$3,2,2)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C9" t="e">
-        <f ca="1">D9=E9</f>
-        <v>#VALUE!</v>
+      <c r="C9" t="b">
+        <f>D9=E9</f>
+        <v>1</v>
       </c>
       <c r="D9">
         <f>INDEX($K$3:$M$5,1,2)</f>
         <v>2</v>
       </c>
-      <c r="E9" t="e">
-        <f ca="1">_xll.xloIndex($E$3,1,2)</f>
-        <v>#VALUE!</v>
+      <c r="E9">
+        <f>_xll.xloIndex($E$3,1,2)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C10" t="e">
-        <f ca="1">D10=E10</f>
-        <v>#VALUE!</v>
+      <c r="C10" t="b">
+        <f>D10=E10</f>
+        <v>1</v>
       </c>
       <c r="D10">
         <f>INDEX(K3:K5,2)</f>
         <v>4</v>
       </c>
-      <c r="E10" t="e">
-        <f ca="1">_xll.xloIndex(K3:K5,2)</f>
-        <v>#VALUE!</v>
+      <c r="E10">
+        <f>_xll.xloIndex(K3:K5,2)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="e">
-        <f ca="1">D13=E13</f>
-        <v>#VALUE!</v>
+        <v>57</v>
+      </c>
+      <c r="C13" t="b">
+        <f>D13=E13</f>
+        <v>1</v>
       </c>
       <c r="D13">
         <f>INDEX(K3:M5,ROWS(K3:M5),COLUMNS(K3:M5))</f>
         <v>9</v>
       </c>
-      <c r="E13" t="e">
-        <f ca="1">_xll.xloIndex($E$3,-1,-1)</f>
-        <v>#VALUE!</v>
+      <c r="E13">
+        <f>_xll.xloIndex($E$3,-1,-1)</f>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" t="e">
-        <f t="array" ref="C15" ca="1">SUM(0+(D15:E15=F15:G15))=2</f>
-        <v>#VALUE!</v>
+        <v>58</v>
+      </c>
+      <c r="C15" t="b">
+        <f t="array" ref="C15">SUM(0+(D15:E15=F15:G15))=2</f>
+        <v>1</v>
       </c>
       <c r="D15">
         <f>K3</f>
@@ -4041,56 +3798,52 @@
         <f>L3</f>
         <v>2</v>
       </c>
-      <c r="F15" s="5" t="e">
-        <f t="array" aca="1" ref="F15:G15" ca="1">_xll.xloIndex(E3,,,2,3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G15" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="F15" s="5">
+        <f t="array" ref="F15:G15">_xll.xloIndex(E3,,,2,3)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="e">
-        <f t="array" ref="C17" ca="1">SUM(0+(D17:E18=F17:G18))=4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D17" t="e">
-        <f ca="1">G4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E17" t="e">
-        <f ca="1">H4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F17" s="5" t="e">
-        <f t="array" aca="1" ref="F17:G18" ca="1">_xll.xloIndex($E$3,-2,-2, 0, 0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G17" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+        <v>59</v>
+      </c>
+      <c r="C17" t="b">
+        <f t="array" ref="C17">SUM(0+(D17:E18=F17:G18))=4</f>
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>G4</f>
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <f>H4</f>
+        <v>6</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="array" ref="F17:G18">_xll.xloIndex($E$3,-2,-2, 0, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D18" t="e">
-        <f ca="1">G5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" t="e">
-        <f ca="1">H5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F18" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" s="5" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="D18">
+        <f>G5</f>
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <f>H5</f>
+        <v>9</v>
+      </c>
+      <c r="F18" s="5">
+        <v>8</v>
+      </c>
+      <c r="G18" s="5">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change some cell formatting in xlOil_utils
</commit_message>
<xml_diff>
--- a/tests/utils/xlOil_Utils.xlsx
+++ b/tests/utils/xlOil_Utils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009D4D4A-3312-4876-AD55-56016D2E53D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0FD8E1-0509-4473-8943-F171B6BE0490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
@@ -720,14 +720,14 @@
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.3">
       <c r="N3" t="e">
-        <f>N6=X6</f>
-        <v>#N/A</v>
+        <f ca="1">N6=X6</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="b">
-        <f t="array" ref="B4">AND(L6:M7=V6:W7)</f>
-        <v>1</v>
+      <c r="B4" s="15" t="e">
+        <f t="array" ref="B4" ca="1">AND(L6:M7=V6:W7)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -736,8 +736,8 @@
         <v>10</v>
       </c>
       <c r="N4" t="e">
-        <f>TEXT(N6, ".")</f>
-        <v>#N/A</v>
+        <f ca="1">TEXT(N6, ".")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="V4" t="s">
         <v>62</v>
@@ -750,15 +750,17 @@
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="4" t="str">
-        <f t="array" ref="L6:N8">_xll.xloBlock(E6,E7,F7,G7,H7)</f>
-        <v>A</v>
-      </c>
-      <c r="M6" s="5" t="str">
-        <v>B</v>
+      <c r="L6" s="4" t="e">
+        <f t="array" aca="1" ref="L6:N8" ca="1">_xll.xloBlock(E6,E7,F7,G7,H7)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M6" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N6" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V6" s="13" t="s">
         <v>1</v>
@@ -786,14 +788,17 @@
       <c r="H7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="5" t="str">
-        <v>C</v>
-      </c>
-      <c r="M7" s="5" t="str">
-        <v>D</v>
+      <c r="L7" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M7" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N7" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V7" s="14" t="s">
         <v>3</v>
@@ -807,13 +812,16 @@
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="L8" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M8" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N8" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V8" s="14" t="e">
         <v>#N/A</v>
@@ -826,9 +834,9 @@
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="b">
-        <f t="array" ref="B10">AND(P12:R15=V12:X15)</f>
-        <v>1</v>
+      <c r="B10" s="12" t="e">
+        <f t="array" ref="B10" ca="1">AND(P12:R15=V12:X15)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -847,25 +855,29 @@
       <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="4" t="str">
-        <f t="array" ref="L12:N15">_xll.xloBlock(E12,E13:F14,G13:H14,I13,_xll.xloFill(J13,2,1))</f>
-        <v>A</v>
-      </c>
-      <c r="M12" s="5" t="str">
-        <v>A</v>
-      </c>
-      <c r="N12" s="5" t="str">
-        <v>C</v>
-      </c>
-      <c r="P12" s="5" t="str">
-        <f t="array" ref="P12:R15">_xll.xloFillNA(L12:N15,"NOPE")</f>
-        <v>A</v>
-      </c>
-      <c r="Q12" s="5" t="str">
-        <v>A</v>
-      </c>
-      <c r="R12" s="5" t="str">
-        <v>C</v>
+      <c r="L12" s="4" t="e">
+        <f t="array" aca="1" ref="L12:N15" ca="1">_xll.xloBlock(E12,E13:F14,G13:H14,I13,_xll.xloFill(J13,2,1))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M12" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N12" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P12" s="5" t="e">
+        <f t="array" aca="1" ref="P12:R15" ca="1">_xll.xloFillNA(L12:N15,"NOPE")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q12" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R12" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V12" s="13" t="s">
         <v>1</v>
@@ -899,23 +911,29 @@
       <c r="J13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="5" t="str">
-        <v>A</v>
-      </c>
-      <c r="M13" s="5" t="str">
-        <v>A</v>
+      <c r="L13" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M13" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N13" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P13" s="5" t="str">
-        <v>A</v>
-      </c>
-      <c r="Q13" s="5" t="str">
-        <v>A</v>
-      </c>
-      <c r="R13" s="5" t="str">
-        <v>NOPE</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P13" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q13" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R13" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V13" s="14" t="s">
         <v>1</v>
@@ -942,23 +960,29 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="L14" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="M14" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="N14" s="5" t="str">
-        <v>F</v>
-      </c>
-      <c r="P14" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="Q14" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="R14" s="5" t="str">
-        <v>F</v>
+      <c r="L14" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M14" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N14" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P14" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q14" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R14" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V14" s="14" t="s">
         <v>2</v>
@@ -971,23 +995,29 @@
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="L15" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="M15" s="5" t="str">
-        <v>B</v>
+      <c r="L15" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M15" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N15" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P15" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="Q15" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="R15" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P15" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q15" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R15" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V15" s="13" t="s">
         <v>2</v>
@@ -1000,9 +1030,9 @@
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B17" s="12" t="b">
-        <f t="array" ref="B17">AND(L19:M20=V19:W20)</f>
-        <v>1</v>
+      <c r="B17" s="12" t="e">
+        <f t="array" ref="B17" ca="1">AND(L19:M20=V19:W20)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1019,18 +1049,21 @@
       <c r="E19" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="4" t="str">
-        <f t="array" ref="L19:O22">_xll.xloBlock(E19,E20:F21,_xll.xloFill(G20,2,2),H20,I20)</f>
-        <v>A</v>
-      </c>
-      <c r="M19" s="5" t="str">
-        <v>B</v>
+      <c r="L19" s="4" t="e">
+        <f t="array" aca="1" ref="L19:O22" ca="1">_xll.xloBlock(E19,E20:F21,_xll.xloFill(G20,2,2),H20,I20)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M19" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N19" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O19" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V19" s="13" t="s">
         <v>1</v>
@@ -1049,12 +1082,13 @@
       <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="2" t="str">
-        <f t="array" ref="E20:F21">_xll.xloFill("A",2,2)</f>
-        <v>A</v>
-      </c>
-      <c r="F20" s="2" t="str">
-        <v/>
+      <c r="E20" s="2" t="e">
+        <f t="array" aca="1" ref="E20:F21" ca="1">_xll.xloFill("A",2,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" s="2" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>2</v>
@@ -1065,17 +1099,21 @@
       <c r="I20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L20" s="5" t="str">
-        <v>C</v>
-      </c>
-      <c r="M20" s="5" t="str">
-        <v>D</v>
+      <c r="L20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N20" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O20" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V20" s="13" t="s">
         <v>3</v>
@@ -1091,26 +1129,32 @@
       </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E21" s="2" t="str">
-        <v/>
-      </c>
-      <c r="F21" s="2" t="str">
-        <v/>
+      <c r="E21" s="2" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F21" s="2" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="L21" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M21" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N21" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O21" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V21" s="13" t="e">
         <v>#N/A</v>
@@ -1127,16 +1171,20 @@
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="L22" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M22" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N22" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O22" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V22" s="13" t="e">
         <v>#N/A</v>
@@ -1152,9 +1200,9 @@
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B24" s="12" t="b">
-        <f t="array" ref="B24">AND(IFERROR(Q26:T29=V26:Y29,ERROR.TYPE(Q26:T29)=ERROR.TYPE(V26:Y29)))</f>
-        <v>1</v>
+      <c r="B24" s="12" t="e">
+        <f t="array" aca="1" ref="B24" ca="1">AND(IFERROR(Q26:T29=V26:Y29,ERROR.TYPE(Q26:T29)=ERROR.TYPE(V26:Y29)))</f>
+        <v>#N/A</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -1173,31 +1221,37 @@
       <c r="E26" t="s">
         <v>17</v>
       </c>
-      <c r="L26" s="4" t="str">
-        <f t="array" ref="L26:O29">_xll.xloBlock(E26,E27:F28,_xll.xloFill(G27,2,2),H27,I27)</f>
-        <v>A</v>
+      <c r="L26" s="4" t="e">
+        <f t="array" aca="1" ref="L26:O29" ca="1">_xll.xloBlock(E26,E27:F28,_xll.xloFill(G27,2,2),H27,I27)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M26" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N26" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O26" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q26" s="5" t="str">
-        <f t="array" ref="Q26:T29">_xll.xloFillNA(L26:O29,".",FALSE)</f>
-        <v>A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q26" s="5" t="e">
+        <f t="array" aca="1" ref="Q26:T29" ca="1">_xll.xloFillNA(L26:O29,".",FALSE)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="R26" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S26" s="5" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T26" s="5" t="str">
-        <v>.</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T26" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V26" s="13" t="s">
         <v>1</v>
@@ -1216,12 +1270,13 @@
       <c r="D27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="2" t="str">
-        <f t="array" ref="E27:F28">_xll.xloFill("A",2,2)</f>
-        <v>A</v>
-      </c>
-      <c r="F27" s="2" t="str">
-        <v/>
+      <c r="E27" s="2" t="e">
+        <f t="array" aca="1" ref="E27:F28" ca="1">_xll.xloFill("A",2,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F27" s="2" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="G27" s="2" t="e">
         <f>1/0</f>
@@ -1234,28 +1289,36 @@
         <v>15</v>
       </c>
       <c r="L27" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M27" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N27" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O27" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q27" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q27" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="R27" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S27" s="5" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T27" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T27" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V27" s="13" t="s">
         <v>64</v>
@@ -1271,38 +1334,48 @@
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E28" s="2" t="str">
-        <v/>
-      </c>
-      <c r="F28" s="2" t="str">
-        <v/>
+      <c r="E28" s="2" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F28" s="2" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="L28" s="5" t="str">
-        <v>Left</v>
+      <c r="L28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M28" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N28" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O28" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q28" s="5" t="str">
-        <v>Left</v>
-      </c>
-      <c r="R28" s="5" t="str">
-        <v/>
-      </c>
-      <c r="S28" s="5" t="str">
-        <v/>
-      </c>
-      <c r="T28" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V28" s="13" t="s">
         <v>14</v>
@@ -1319,28 +1392,36 @@
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="L29" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M29" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N29" s="5" t="str">
-        <v>Right</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O29" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q29" s="5" t="str">
-        <v/>
-      </c>
-      <c r="R29" s="5" t="str">
-        <v/>
-      </c>
-      <c r="S29" s="5" t="str">
-        <v>Right</v>
-      </c>
-      <c r="T29" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="V29" s="13" t="s">
         <v>64</v>
@@ -1356,9 +1437,9 @@
       </c>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B31" s="12" t="b">
-        <f t="array" ref="B31">AND(IFERROR(Q33:T36=V26:Y29,ERROR.TYPE(Q33:T36)=ERROR.TYPE(V26:Y29)))</f>
-        <v>1</v>
+      <c r="B31" s="12" t="e">
+        <f t="array" aca="1" ref="B31" ca="1">AND(IFERROR(Q33:T36=V26:Y29,ERROR.TYPE(Q33:T36)=ERROR.TYPE(V26:Y29)))</f>
+        <v>#N/A</v>
       </c>
       <c r="D31" t="s">
         <v>60</v>
@@ -1368,109 +1449,139 @@
       </c>
     </row>
     <row r="33" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="L33" s="5" t="str">
-        <f t="array" ref="L33:O36">_xll.xloBlock(E26,_xll.xloRef(E27:F28),_xll.xloFill(G27,2,2),_xll.xloRef(H27),I27)</f>
-        <v>A</v>
+      <c r="L33" s="5" t="e">
+        <f t="array" aca="1" ref="L33:O36" ca="1">_xll.xloBlock(E26,_xll.xloRef(E27:F28),_xll.xloFill(G27,2,2),_xll.xloRef(H27),I27)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="M33" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N33" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O33" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q33" s="5" t="str">
-        <f t="array" ref="Q33:T36">_xll.xloFillNA(_xll.xloRef(L33:O36),".",FALSE)</f>
-        <v>A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q33" s="5" t="e">
+        <f t="array" aca="1" ref="Q33:T36" ca="1">_xll.xloFillNA(_xll.xloRef(L33:O36),".",FALSE)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="R33" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S33" s="5" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T33" s="5" t="str">
-        <v>.</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T33" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="12:20" x14ac:dyDescent="0.3">
       <c r="L34" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M34" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N34" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O34" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q34" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="R34" s="5" t="e">
-        <v>#DIV/0!</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S34" s="5" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T34" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="12:20" x14ac:dyDescent="0.3">
-      <c r="L35" s="5" t="str">
-        <v>Left</v>
+      <c r="L35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M35" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="N35" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O35" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q35" s="5" t="str">
-        <v>Left</v>
-      </c>
-      <c r="R35" s="5" t="str">
-        <v/>
-      </c>
-      <c r="S35" s="5" t="str">
-        <v/>
-      </c>
-      <c r="T35" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="12:20" x14ac:dyDescent="0.3">
       <c r="L36" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M36" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N36" s="5" t="str">
-        <v>Right</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O36" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q36" s="5" t="str">
-        <v/>
-      </c>
-      <c r="R36" s="5" t="str">
-        <v/>
-      </c>
-      <c r="S36" s="5" t="str">
-        <v>Right</v>
-      </c>
-      <c r="T36" s="5" t="str">
-        <v/>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -1506,9 +1617,9 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="str">
-        <f>_xll.xloConcat(,I5,J5,K5)</f>
-        <v>FooBarBaz</v>
+      <c r="B5" s="5" t="e">
+        <f ca="1">_xll.xloConcat(,I5,J5,K5)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1544,9 +1655,9 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="str">
-        <f>_xll.xloConcat(",",I5:K5)</f>
-        <v>Foo,Bar,Baz</v>
+      <c r="B8" s="5" t="e">
+        <f ca="1">_xll.xloConcat(",",I5:K5)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1564,9 +1675,9 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="str">
-        <f>_xll.xloConcat("…",I5:I8,J5,K5)</f>
-        <v>Foo…Green…Eggs…Ham…Bar…Baz</v>
+      <c r="B11" s="5" t="e">
+        <f ca="1">_xll.xloConcat("…",I5:I8,J5,K5)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1579,9 +1690,9 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="str">
-        <f>_xll.xloConcat("---", I5:I8, _xll.xloConcat(",",J6:J8),J5:K5)</f>
-        <v>Foo---Green---Eggs---Ham---1,2,3---Bar---Baz</v>
+      <c r="B14" s="5" t="e">
+        <f ca="1">_xll.xloConcat("---", I5:I8, _xll.xloConcat(",",J6:J8),J5:K5)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1601,27 +1712,33 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="str">
-        <f t="array" ref="B21:H21">TRANSPOSE(_xll.xloSplit(B14,"-"))</f>
-        <v>Foo</v>
-      </c>
-      <c r="C21" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="D21" s="5" t="str">
-        <v>Eggs</v>
-      </c>
-      <c r="E21" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="F21" s="5" t="str">
-        <v>1,2,3</v>
-      </c>
-      <c r="G21" s="5" t="str">
-        <v>Bar</v>
-      </c>
-      <c r="H21" s="5" t="str">
-        <v>Baz</v>
+      <c r="B21" s="5" t="e">
+        <f t="array" aca="1" ref="B21:H21" ca="1">TRANSPOSE(_xll.xloSplit(B14,"-"))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -1651,30 +1768,30 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="12" t="b">
-        <f>B21=B22</f>
-        <v>1</v>
-      </c>
-      <c r="C23" s="12" t="b">
-        <f t="shared" ref="C23:H23" si="0">C21=C22</f>
-        <v>1</v>
-      </c>
-      <c r="D23" s="12" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="12" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="B23" s="12" t="e">
+        <f ca="1">B21=B22</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C23" s="12" t="e">
+        <f t="shared" ref="C23:H23" ca="1" si="0">C21=C22</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D23" s="12" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E23" s="12" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="12" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23" s="12" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="G23" s="12" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H23" s="12" t="e">
+        <f t="shared" ca="1" si="0"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
@@ -1683,12 +1800,13 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="str">
-        <f t="array" ref="B27:C30">_xll.xloSplit(I5:I8,"e")</f>
-        <v>Foo</v>
+      <c r="B27" s="5" t="e">
+        <f t="array" aca="1" ref="B27:C30" ca="1">_xll.xloSplit(I5:I8,"e")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="C27" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E27" t="s">
         <v>18</v>
@@ -1696,21 +1814,23 @@
       <c r="F27" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G27" s="12" t="b">
-        <f>E27=B27</f>
-        <v>1</v>
+      <c r="G27" s="12" t="e">
+        <f ca="1">E27=B27</f>
+        <v>#VALUE!</v>
       </c>
       <c r="H27" s="12" t="b">
-        <f>ISNA(C27)</f>
-        <v>1</v>
+        <f ca="1">ISNA(C27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="str">
-        <v>Gr</v>
-      </c>
-      <c r="C28" s="5" t="str">
-        <v>n</v>
+      <c r="B28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E28" t="s">
         <v>49</v>
@@ -1718,21 +1838,23 @@
       <c r="F28" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="12" t="b">
-        <f t="shared" ref="G28:G30" si="1">E28=B28</f>
-        <v>1</v>
-      </c>
-      <c r="H28" s="12" t="b">
-        <f t="shared" ref="H28" si="2">F28=C28</f>
-        <v>1</v>
+      <c r="G28" s="12" t="e">
+        <f t="shared" ref="G28:G30" ca="1" si="1">E28=B28</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H28" s="12" t="e">
+        <f t="shared" ref="H28" ca="1" si="2">F28=C28</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="str">
-        <v>Eggs</v>
+      <c r="B29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="C29" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E29" t="s">
         <v>23</v>
@@ -1740,21 +1862,23 @@
       <c r="F29" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G29" s="12" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="G29" s="12" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H29" s="12" t="b">
-        <f>ISNA(C29)</f>
-        <v>1</v>
+        <f ca="1">ISNA(C29)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="5" t="str">
-        <v>Ham</v>
+      <c r="B30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="C30" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E30" t="s">
         <v>21</v>
@@ -1762,13 +1886,13 @@
       <c r="F30" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G30" s="12" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="G30" s="12" t="e">
+        <f t="shared" ca="1" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="H30" s="12" t="b">
-        <f>ISNA(C30)</f>
-        <v>1</v>
+        <f ca="1">ISNA(C30)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -1777,50 +1901,55 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="str">
-        <f t="array" ref="B34:D35">_xll.xloSplit(I5:K5,"a")</f>
-        <v>Foo</v>
-      </c>
-      <c r="C34" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="D34" s="5" t="str">
-        <v>B</v>
-      </c>
-      <c r="E34" s="12" t="b">
-        <f>B36=B34</f>
-        <v>1</v>
-      </c>
-      <c r="F34" s="12" t="b">
-        <f t="shared" ref="F34:G34" si="3">C36=C34</f>
-        <v>1</v>
-      </c>
-      <c r="G34" s="12" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
+      <c r="B34" s="5" t="e">
+        <f t="array" aca="1" ref="B34:D35" ca="1">_xll.xloSplit(I5:K5,"a")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E34" s="12" t="e">
+        <f ca="1">B36=B34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F34" s="12" t="e">
+        <f t="shared" ref="F34:G34" ca="1" si="3">C36=C34</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G34" s="12" t="e">
+        <f t="shared" ca="1" si="3"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="C35" s="5" t="str">
-        <v>r</v>
-      </c>
-      <c r="D35" s="5" t="str">
-        <v>z</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E35" s="12" t="b">
         <f>ISNA(B37)</f>
         <v>1</v>
       </c>
-      <c r="F35" s="12" t="b">
-        <f t="shared" ref="F35" si="4">C37=C35</f>
-        <v>1</v>
-      </c>
-      <c r="G35" s="12" t="b">
-        <f t="shared" ref="G35" si="5">D37=D35</f>
-        <v>1</v>
+      <c r="F35" s="12" t="e">
+        <f t="shared" ref="F35" ca="1" si="4">C37=C35</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G35" s="12" t="e">
+        <f t="shared" ref="G35" ca="1" si="5">D37=D35</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
@@ -1854,37 +1983,39 @@
       <c r="B40" s="2">
         <v>1</v>
       </c>
-      <c r="C40" s="5">
-        <f t="array" ref="C40:C42">_xll.xloSplit(B40:B42,"x")</f>
-        <v>1</v>
-      </c>
-      <c r="E40" s="12" t="b">
-        <f>C40=B40</f>
-        <v>1</v>
+      <c r="C40" s="5" t="e">
+        <f t="array" aca="1" ref="C40:C42" ca="1">_xll.xloSplit(B40:B42,"x")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E40" s="12" t="e">
+        <f ca="1">C40=B40</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>2</v>
       </c>
-      <c r="C41" s="5">
-        <v>2</v>
-      </c>
-      <c r="E41" s="12" t="b">
-        <f t="shared" ref="E41:E42" si="6">C41=B41</f>
-        <v>1</v>
+      <c r="C41" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E41" s="12" t="e">
+        <f t="shared" ref="E41:E42" ca="1" si="6">C41=B41</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>3</v>
       </c>
-      <c r="C42" s="5">
-        <v>3</v>
-      </c>
-      <c r="E42" s="12" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
+      <c r="C42" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E42" s="12" t="e">
+        <f t="shared" ca="1" si="6"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -1897,8 +2028,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:V107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,49 +2078,49 @@
       <c r="V3" s="9"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="b">
-        <f t="array" ref="B4">AND(B19:C25=B40:C46)</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="b">
-        <f t="array" ref="C4">AND(E19:F25=B40:C46)</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="12" t="b">
-        <f t="array" ref="D4">AND(H19:I25=B40:C46)</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="12" t="b">
-        <f t="array" ref="E4">AND(B30:C36=B48:C54)</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="12" t="b">
-        <f t="array" ref="F4">AND(E30:F36=B48:C54)</f>
-        <v>1</v>
-      </c>
-      <c r="G4" s="12" t="b">
-        <f t="array" ref="G4">AND(H30:I36=B48:C54)</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="12" t="b">
-        <f t="array" ref="K4">AND(IFERROR(K22:K34=K40:K52,ERROR.TYPE(K22:K34)=ERROR.TYPE(K40:K52)))</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="12" t="b">
-        <f t="array" ref="M4">AND(IFERROR(M22:M34=M40:M52,ERROR.TYPE(M22:M34)=ERROR.TYPE(M40:M52)))</f>
-        <v>1</v>
-      </c>
-      <c r="O4" s="12" t="b">
-        <f t="array" ref="O4">AND(IFERROR(O22:O34=K40:K52,ERROR.TYPE(O22:O34)=ERROR.TYPE(K40:K52)))</f>
-        <v>1</v>
+      <c r="B4" s="12" t="e">
+        <f t="array" ref="B4" ca="1">AND(B19:C25=B40:C46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C4" s="12" t="e">
+        <f t="array" ref="C4" ca="1">AND(E19:F25=B40:C46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" s="12" t="e">
+        <f t="array" ref="D4" ca="1">AND(H19:I25=B40:C46)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E4" s="12" t="e">
+        <f t="array" ref="E4" ca="1">AND(B30:C36=B48:C54)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" s="12" t="e">
+        <f t="array" ref="F4" ca="1">AND(E30:F36=B48:C54)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G4" s="12" t="e">
+        <f t="array" ref="G4" ca="1">AND(H30:I36=B48:C54)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K4" s="12" t="e">
+        <f t="array" aca="1" ref="K4" ca="1">AND(IFERROR(K22:K34=K40:K52,ERROR.TYPE(K22:K34)=ERROR.TYPE(K40:K52)))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M4" s="12" t="e">
+        <f t="array" aca="1" ref="M4" ca="1">AND(IFERROR(M22:M34=M40:M52,ERROR.TYPE(M22:M34)=ERROR.TYPE(M40:M52)))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O4" s="12" t="e">
+        <f t="array" aca="1" ref="O4" ca="1">AND(IFERROR(O22:O34=K40:K52,ERROR.TYPE(O22:O34)=ERROR.TYPE(K40:K52)))</f>
+        <v>#N/A</v>
       </c>
       <c r="Q4" s="12" t="b">
         <f>AND(IFERROR(Q22:Q34=M40:M52,ERROR.TYPE(Q22:Q34)=ERROR.TYPE(M40:M52)))</f>
         <v>1</v>
       </c>
-      <c r="S4" s="12" t="b">
+      <c r="S4" s="12" t="e">
         <f ca="1">AND(T8=MIN(S8:S107),T107=MAX(S8:S107))</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
@@ -2024,11 +2155,11 @@
       </c>
       <c r="S8" s="7">
         <f ca="1">RAND()</f>
-        <v>6.0755901780086274E-3</v>
-      </c>
-      <c r="T8" s="4">
+        <v>0.96078521459195632</v>
+      </c>
+      <c r="T8" s="4" t="e">
         <f t="array" aca="1" ref="T8:T107" ca="1">_xll.xloSort(S8:S107,"a")</f>
-        <v>4.4892519097212702E-3</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
@@ -2044,9 +2175,9 @@
       <c r="S9" s="7">
         <v>1.4241351279182801E-2</v>
       </c>
-      <c r="T9" s="4">
-        <f ca="1"/>
-        <v>6.0755901780086274E-3</v>
+      <c r="T9" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
@@ -2062,9 +2193,9 @@
       <c r="S10" s="7">
         <v>0.11987234330114915</v>
       </c>
-      <c r="T10" s="4">
-        <f ca="1"/>
-        <v>8.9705088996498983E-3</v>
+      <c r="T10" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
@@ -2080,9 +2211,9 @@
       <c r="S11" s="7">
         <v>0.43199912726020961</v>
       </c>
-      <c r="T11" s="4">
-        <f ca="1"/>
-        <v>1.0142003022623358E-2</v>
+      <c r="T11" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
@@ -2099,9 +2230,9 @@
       <c r="S12" s="7">
         <v>0.44362993322818001</v>
       </c>
-      <c r="T12" s="4">
-        <f ca="1"/>
-        <v>1.4241351279182801E-2</v>
+      <c r="T12" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
@@ -2118,9 +2249,9 @@
       <c r="S13" s="7">
         <v>0.70719203131190667</v>
       </c>
-      <c r="T13" s="4">
-        <f ca="1"/>
-        <v>1.7278225187227991E-2</v>
+      <c r="T13" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
@@ -2136,9 +2267,9 @@
       <c r="S14" s="7">
         <v>0.28303369927876221</v>
       </c>
-      <c r="T14" s="4">
-        <f ca="1"/>
-        <v>4.2989156379268589E-2</v>
+      <c r="T14" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
@@ -2148,9 +2279,9 @@
       <c r="S15" s="7">
         <v>0.18684151297687135</v>
       </c>
-      <c r="T15" s="4">
-        <f ca="1"/>
-        <v>4.8199686141203735E-2</v>
+      <c r="T15" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.3">
@@ -2170,9 +2301,9 @@
       <c r="S16" s="7">
         <v>7.6545233242765964E-2</v>
       </c>
-      <c r="T16" s="4">
-        <f ca="1"/>
-        <v>5.2437735118262885E-2</v>
+      <c r="T16" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.3">
@@ -2184,18 +2315,19 @@
       <c r="S17" s="7">
         <v>0.78402600397426425</v>
       </c>
-      <c r="T17" s="4">
-        <f ca="1"/>
-        <v>6.063738431260568E-2</v>
+      <c r="T17" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="E18" t="str">
-        <f t="array" ref="E18:F25">_xll.xloSort(B7:C14,"a","Words")</f>
-        <v>Words</v>
-      </c>
-      <c r="F18" t="str">
-        <v>Numbers</v>
+      <c r="E18" t="e">
+        <f t="array" aca="1" ref="E18:F25" ca="1">_xll.xloSort(B7:C14,"a","Words")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>40</v>
@@ -2203,31 +2335,35 @@
       <c r="S18" s="7">
         <v>0.5992299667126384</v>
       </c>
-      <c r="T18" s="4">
-        <f ca="1"/>
-        <v>7.6545233242765964E-2</v>
+      <c r="T18" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B19" s="5" t="str">
-        <f t="array" ref="B19:C25">_xll.xloSort(B8:C14,"a",1)</f>
-        <v>Box</v>
-      </c>
-      <c r="C19" s="5">
-        <v>7</v>
-      </c>
-      <c r="E19" s="5" t="str">
-        <v>Box</v>
-      </c>
-      <c r="F19" s="5">
-        <v>7</v>
-      </c>
-      <c r="H19" s="5" t="str">
-        <f t="array" ref="H19:I25">_xll.xloSort(_xll.xloRef(B8:C14),"a",1)</f>
-        <v>Box</v>
-      </c>
-      <c r="I19" s="5">
-        <v>7</v>
+      <c r="B19" s="5" t="e">
+        <f t="array" aca="1" ref="B19:C25" ca="1">_xll.xloSort(B8:C14,"a",1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C19" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F19" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H19" s="5" t="e">
+        <f t="array" aca="1" ref="H19:I25" ca="1">_xll.xloSort(_xll.xloRef(B8:C14),"a",1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I19" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>41</v>
@@ -2235,29 +2371,35 @@
       <c r="S19" s="7">
         <v>0.21129177216442607</v>
       </c>
-      <c r="T19" s="4">
-        <f ca="1"/>
-        <v>9.6043732044653662E-2</v>
+      <c r="T19" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="str">
-        <v>BOX</v>
-      </c>
-      <c r="C20" s="5">
-        <v>8</v>
-      </c>
-      <c r="E20" s="5" t="str">
-        <v>BOX</v>
-      </c>
-      <c r="F20" s="5">
-        <v>8</v>
-      </c>
-      <c r="H20" s="5" t="str">
-        <v>BOX</v>
-      </c>
-      <c r="I20" s="5">
-        <v>8</v>
+      <c r="B20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I20" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>42</v>
@@ -2265,218 +2407,264 @@
       <c r="S20" s="7">
         <v>0.56907031356613658</v>
       </c>
-      <c r="T20" s="4">
-        <f ca="1"/>
-        <v>0.10466409270245647</v>
+      <c r="T20" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B21" s="5" t="str">
-        <v>Eggs</v>
-      </c>
-      <c r="C21" s="5">
-        <v>3</v>
-      </c>
-      <c r="E21" s="5" t="str">
-        <v>Eggs</v>
-      </c>
-      <c r="F21" s="5">
-        <v>3</v>
-      </c>
-      <c r="H21" s="5" t="str">
-        <v>Eggs</v>
-      </c>
-      <c r="I21" s="5">
-        <v>3</v>
+      <c r="B21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I21" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="P21" s="3"/>
       <c r="S21" s="7">
         <v>0.70052257146975117</v>
       </c>
-      <c r="T21" s="4">
-        <f ca="1"/>
-        <v>0.11099657306935851</v>
+      <c r="T21" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="str">
-        <v>Fox</v>
-      </c>
-      <c r="C22" s="5">
-        <v>3</v>
-      </c>
-      <c r="E22" s="5" t="str">
-        <v>Fox</v>
-      </c>
-      <c r="F22" s="5">
-        <v>3</v>
-      </c>
-      <c r="H22" s="5" t="str">
-        <v>Fox</v>
-      </c>
-      <c r="I22" s="5">
-        <v>3</v>
-      </c>
-      <c r="K22" s="5">
-        <f t="array" ref="K22:K34">_xll.xloSort(K8:K20,"a",1)</f>
-        <v>4</v>
-      </c>
-      <c r="M22" s="5">
-        <f t="array" ref="M22:M34">_xll.xloSort(K8:K20,"A",1)</f>
-        <v>4</v>
-      </c>
-      <c r="O22" s="5">
-        <f t="array" ref="O22:O34">_xll.xloSort(_xll.xloRef(K8:K20),"a",1)</f>
-        <v>4</v>
-      </c>
-      <c r="Q22" s="5">
-        <f t="array" ref="Q22:Q34">_xll.xloSort(_xll.xloRef(K8:K20),"A",1)</f>
-        <v>4</v>
+      <c r="B22" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C22" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E22" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F22" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H22" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I22" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K22" s="5" t="e">
+        <f t="array" aca="1" ref="K22:K34" ca="1">_xll.xloSort(K8:K20,"a",1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M22" s="5" t="e">
+        <f t="array" aca="1" ref="M22:M34" ca="1">_xll.xloSort(K8:K20,"A",1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O22" s="5" t="e">
+        <f t="array" aca="1" ref="O22:O34" ca="1">_xll.xloSort(_xll.xloRef(K8:K20),"a",1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q22" s="5" t="e">
+        <f t="array" aca="1" ref="Q22:Q34" ca="1">_xll.xloSort(_xll.xloRef(K8:K20),"A",1)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="S22" s="7">
         <v>0.96985704312068066</v>
       </c>
-      <c r="T22" s="4">
-        <f ca="1"/>
-        <v>0.11987234330114915</v>
+      <c r="T22" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B23" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1</v>
-      </c>
-      <c r="H23" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="I23" s="5">
-        <v>1</v>
-      </c>
-      <c r="K23" s="5">
-        <v>6.2</v>
-      </c>
-      <c r="M23" s="5">
-        <v>6.2</v>
-      </c>
-      <c r="O23" s="5">
-        <v>6.2</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>6.2</v>
+      <c r="B23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q23" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S23" s="7">
         <v>0.55553726039846762</v>
       </c>
-      <c r="T23" s="4">
-        <f ca="1"/>
-        <v>0.15138392223952224</v>
+      <c r="T23" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B24" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="C24" s="5">
-        <v>3</v>
-      </c>
-      <c r="E24" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="F24" s="5">
-        <v>3</v>
-      </c>
-      <c r="H24" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="I24" s="5">
-        <v>3</v>
-      </c>
-      <c r="K24" s="5">
-        <v>6.3</v>
-      </c>
-      <c r="M24" s="5">
-        <v>6.3</v>
-      </c>
-      <c r="O24" s="5">
-        <v>6.3</v>
-      </c>
-      <c r="Q24" s="5">
-        <v>6.3</v>
+      <c r="B24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q24" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S24" s="7">
         <v>0.346644941363903</v>
       </c>
-      <c r="T24" s="4">
-        <f ca="1"/>
-        <v>0.15285256271102787</v>
+      <c r="T24" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="str">
-        <v>Sam</v>
-      </c>
-      <c r="C25" s="5">
-        <v>4</v>
-      </c>
-      <c r="E25" s="5" t="str">
-        <v>Sam</v>
-      </c>
-      <c r="F25" s="5">
-        <v>4</v>
-      </c>
-      <c r="H25" s="5" t="str">
-        <v>Sam</v>
-      </c>
-      <c r="I25" s="5">
-        <v>4</v>
-      </c>
-      <c r="K25" s="5">
-        <v>7</v>
-      </c>
-      <c r="M25" s="5">
-        <v>7</v>
-      </c>
-      <c r="O25" s="5">
-        <v>7</v>
-      </c>
-      <c r="Q25" s="5">
-        <v>7</v>
+      <c r="B25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q25" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S25" s="7">
         <v>0.86284631971635639</v>
       </c>
-      <c r="T25" s="4">
-        <f ca="1"/>
-        <v>0.15935651729819933</v>
+      <c r="T25" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="K26" s="5" t="str">
-        <v>Foo</v>
-      </c>
-      <c r="M26" s="5" t="str">
-        <v>FOO</v>
-      </c>
-      <c r="O26" s="5" t="str">
-        <v>Foo</v>
-      </c>
-      <c r="Q26" s="5" t="str">
-        <v>FOO</v>
+      <c r="K26" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M26" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O26" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q26" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S26" s="7">
         <v>0.25958386357364216</v>
       </c>
-      <c r="T26" s="4">
-        <f ca="1"/>
-        <v>0.16534127039316493</v>
+      <c r="T26" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.3">
@@ -2490,335 +2678,408 @@
       <c r="H27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K27" s="5" t="str">
-        <v>FOO</v>
-      </c>
-      <c r="M27" s="5" t="str">
-        <v>FOOD</v>
-      </c>
-      <c r="O27" s="5" t="str">
-        <v>FOO</v>
-      </c>
-      <c r="Q27" s="5" t="str">
-        <v>FOOD</v>
+      <c r="K27" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M27" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O27" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q27" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S27" s="7">
         <v>0.44578595954200495</v>
       </c>
-      <c r="T27" s="4">
-        <f ca="1"/>
-        <v>0.18684151297687135</v>
+      <c r="T27" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
-      <c r="K28" s="5" t="str">
-        <v>Food</v>
-      </c>
-      <c r="M28" s="5" t="str">
-        <v>Foo</v>
-      </c>
-      <c r="O28" s="5" t="str">
-        <v>Food</v>
-      </c>
-      <c r="Q28" s="5" t="str">
-        <v>Foo</v>
+      <c r="K28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q28" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S28" s="7">
         <v>0.35070608842246354</v>
       </c>
-      <c r="T28" s="4">
-        <f ca="1"/>
-        <v>0.19150797219437865</v>
+      <c r="T28" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="E29" t="str">
-        <f t="array" ref="E29:F36">_xll.xloSort(B7:C14,"d a","Numbers","Words")</f>
-        <v>Words</v>
-      </c>
-      <c r="F29" t="str">
-        <v>Numbers</v>
-      </c>
-      <c r="K29" s="5" t="str">
-        <v>FOOD</v>
-      </c>
-      <c r="M29" s="5" t="str">
-        <v>FooDs</v>
-      </c>
-      <c r="O29" s="5" t="str">
-        <v>FOOD</v>
-      </c>
-      <c r="Q29" s="5" t="str">
-        <v>FooDs</v>
+      <c r="E29" t="e">
+        <f t="array" aca="1" ref="E29:F36" ca="1">_xll.xloSort(B7:C14,"d a","Numbers","Words")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F29" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q29" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S29" s="7">
         <v>0.97062641299883634</v>
       </c>
-      <c r="T29" s="4">
-        <f ca="1"/>
-        <v>0.19332448079141096</v>
+      <c r="T29" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B30" s="5" t="str">
-        <f t="array" ref="B30:C36">_xll.xloSort(B8:C14,"d a",2,1)</f>
-        <v>BOX</v>
-      </c>
-      <c r="C30" s="5">
-        <v>8</v>
-      </c>
-      <c r="E30" s="5" t="str">
-        <v>BOX</v>
-      </c>
-      <c r="F30" s="5">
-        <v>8</v>
-      </c>
-      <c r="H30" s="5" t="str">
-        <f t="array" ref="H30:I36">_xll.xloSort(_xll.xloRef(B8:C14),"d a",2,1)</f>
-        <v>BOX</v>
-      </c>
-      <c r="I30" s="5">
-        <v>8</v>
-      </c>
-      <c r="K30" s="5" t="str">
-        <v>FooDs</v>
-      </c>
-      <c r="M30" s="5" t="str">
-        <v>Food</v>
-      </c>
-      <c r="O30" s="5" t="str">
-        <v>FooDs</v>
-      </c>
-      <c r="Q30" s="5" t="str">
-        <v>Food</v>
+      <c r="B30" s="5" t="e">
+        <f t="array" aca="1" ref="B30:C36" ca="1">_xll.xloSort(B8:C14,"d a",2,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H30" s="5" t="e">
+        <f t="array" aca="1" ref="H30:I36" ca="1">_xll.xloSort(_xll.xloRef(B8:C14),"d a",2,1)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q30" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S30" s="7">
         <v>0.36303952239766712</v>
       </c>
-      <c r="T30" s="4">
-        <f ca="1"/>
-        <v>0.20455886903305909</v>
+      <c r="T30" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="str">
-        <v>Box</v>
-      </c>
-      <c r="C31" s="5">
-        <v>7</v>
-      </c>
-      <c r="E31" s="5" t="str">
-        <v>Box</v>
-      </c>
-      <c r="F31" s="5">
-        <v>7</v>
-      </c>
-      <c r="H31" s="5" t="str">
-        <v>Box</v>
-      </c>
-      <c r="I31" s="5">
-        <v>7</v>
-      </c>
-      <c r="K31" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="M31" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="O31" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="Q31" s="5" t="str">
-        <v>Green</v>
+      <c r="B31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q31" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S31" s="7">
         <v>0.35500379302962237</v>
       </c>
-      <c r="T31" s="4">
-        <f ca="1"/>
-        <v>0.21129177216442607</v>
+      <c r="T31" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="str">
-        <v>Sam</v>
-      </c>
-      <c r="C32" s="5">
-        <v>4</v>
-      </c>
-      <c r="E32" s="5" t="str">
-        <v>Sam</v>
-      </c>
-      <c r="F32" s="5">
-        <v>4</v>
-      </c>
-      <c r="H32" s="5" t="str">
-        <v>Sam</v>
-      </c>
-      <c r="I32" s="5">
-        <v>4</v>
-      </c>
-      <c r="K32" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="M32" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="O32" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="Q32" s="5" t="str">
-        <v>Ham</v>
+      <c r="B32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q32" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S32" s="7">
         <v>0.30991009987247375</v>
       </c>
-      <c r="T32" s="4">
-        <f ca="1"/>
-        <v>0.21289020404938441</v>
+      <c r="T32" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B33" s="5" t="str">
-        <v>Eggs</v>
-      </c>
-      <c r="C33" s="5">
-        <v>3</v>
-      </c>
-      <c r="E33" s="5" t="str">
-        <v>Eggs</v>
-      </c>
-      <c r="F33" s="5">
-        <v>3</v>
-      </c>
-      <c r="H33" s="5" t="str">
-        <v>Eggs</v>
-      </c>
-      <c r="I33" s="5">
-        <v>3</v>
+      <c r="B33" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C33" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E33" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F33" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H33" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I33" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K33" s="5" t="e">
-        <v>#NAME?</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M33" s="5" t="e">
-        <v>#NAME?</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O33" s="5" t="e">
-        <v>#NAME?</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="Q33" s="5" t="e">
-        <v>#NAME?</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S33" s="7">
         <v>0.50309865693105404</v>
       </c>
-      <c r="T33" s="4">
-        <f ca="1"/>
-        <v>0.24005046089105242</v>
+      <c r="T33" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="str">
-        <v>Fox</v>
-      </c>
-      <c r="C34" s="5">
-        <v>3</v>
-      </c>
-      <c r="E34" s="5" t="str">
-        <v>Fox</v>
-      </c>
-      <c r="F34" s="5">
-        <v>3</v>
-      </c>
-      <c r="H34" s="5" t="str">
-        <v>Fox</v>
-      </c>
-      <c r="I34" s="5">
-        <v>3</v>
+      <c r="B34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I34" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K34" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="M34" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="O34" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="Q34" s="5" t="e">
-        <v>#N/A</v>
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S34" s="7">
         <v>0.24683784713265966</v>
       </c>
-      <c r="T34" s="4">
-        <f ca="1"/>
-        <v>0.24683784713265966</v>
+      <c r="T34" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B35" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="C35" s="5">
-        <v>3</v>
-      </c>
-      <c r="E35" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="F35" s="5">
-        <v>3</v>
-      </c>
-      <c r="H35" s="5" t="str">
-        <v>Ham</v>
-      </c>
-      <c r="I35" s="5">
-        <v>3</v>
+      <c r="B35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I35" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S35" s="7">
         <v>0.21289020404938441</v>
       </c>
-      <c r="T35" s="4">
-        <f ca="1"/>
-        <v>0.25090708805825079</v>
+      <c r="T35" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B36" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="C36" s="5">
-        <v>1</v>
-      </c>
-      <c r="E36" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="F36" s="5">
-        <v>1</v>
-      </c>
-      <c r="H36" s="5" t="str">
-        <v>Green</v>
-      </c>
-      <c r="I36" s="5">
-        <v>1</v>
+      <c r="B36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I36" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="S36" s="7">
         <v>0.57712158377157863</v>
       </c>
-      <c r="T36" s="4">
-        <f ca="1"/>
-        <v>0.25958386357364216</v>
+      <c r="T36" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S37" s="7">
         <v>6.063738431260568E-2</v>
       </c>
-      <c r="T37" s="4">
-        <f ca="1"/>
-        <v>0.26026766796149603</v>
+      <c r="T37" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.3">
@@ -2831,18 +3092,18 @@
       <c r="S38" s="7">
         <v>0.37822251634842252</v>
       </c>
-      <c r="T38" s="4">
-        <f ca="1"/>
-        <v>0.2819709570143808</v>
+      <c r="T38" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S39" s="7">
         <v>0.60977631212733274</v>
       </c>
-      <c r="T39" s="4">
-        <f ca="1"/>
-        <v>0.28303369927876221</v>
+      <c r="T39" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.3">
@@ -2861,9 +3122,9 @@
       <c r="S40" s="7">
         <v>0.20455886903305909</v>
       </c>
-      <c r="T40" s="4">
-        <f ca="1"/>
-        <v>0.29579294051174709</v>
+      <c r="T40" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.3">
@@ -2882,9 +3143,9 @@
       <c r="S41" s="7">
         <v>0.947318592329083</v>
       </c>
-      <c r="T41" s="4">
-        <f ca="1"/>
-        <v>0.30621594261281582</v>
+      <c r="T41" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.3">
@@ -2903,9 +3164,9 @@
       <c r="S42" s="7">
         <v>0.68147699048550281</v>
       </c>
-      <c r="T42" s="4">
-        <f ca="1"/>
-        <v>0.30699880764121135</v>
+      <c r="T42" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.3">
@@ -2924,9 +3185,9 @@
       <c r="S43" s="7">
         <v>0.90600850571232516</v>
       </c>
-      <c r="T43" s="4">
-        <f ca="1"/>
-        <v>0.30746381468864881</v>
+      <c r="T43" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.3">
@@ -2945,9 +3206,9 @@
       <c r="S44" s="7">
         <v>0.85960749899325406</v>
       </c>
-      <c r="T44" s="4">
-        <f ca="1"/>
-        <v>0.30991009987247375</v>
+      <c r="T44" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.3">
@@ -2966,9 +3227,9 @@
       <c r="S45" s="7">
         <v>4.2989156379268589E-2</v>
       </c>
-      <c r="T45" s="4">
-        <f ca="1"/>
-        <v>0.34322350221251363</v>
+      <c r="T45" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.3">
@@ -2987,9 +3248,9 @@
       <c r="S46" s="7">
         <v>0.15285256271102787</v>
       </c>
-      <c r="T46" s="4">
-        <f ca="1"/>
-        <v>0.346644941363903</v>
+      <c r="T46" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.3">
@@ -3002,9 +3263,9 @@
       <c r="S47" s="7">
         <v>4.4892519097212702E-3</v>
       </c>
-      <c r="T47" s="4">
-        <f ca="1"/>
-        <v>0.35070608842246354</v>
+      <c r="T47" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.3">
@@ -3023,9 +3284,9 @@
       <c r="S48" s="7">
         <v>9.6043732044653662E-2</v>
       </c>
-      <c r="T48" s="4">
-        <f ca="1"/>
-        <v>0.35500379302962237</v>
+      <c r="T48" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.3">
@@ -3044,9 +3305,9 @@
       <c r="S49" s="7">
         <v>0.30746381468864881</v>
       </c>
-      <c r="T49" s="4">
-        <f ca="1"/>
-        <v>0.36303952239766712</v>
+      <c r="T49" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.3">
@@ -3065,9 +3326,9 @@
       <c r="S50" s="7">
         <v>0.15935651729819933</v>
       </c>
-      <c r="T50" s="4">
-        <f ca="1"/>
-        <v>0.37590154211670712</v>
+      <c r="T50" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.3">
@@ -3086,9 +3347,9 @@
       <c r="S51" s="7">
         <v>0.73492497530386436</v>
       </c>
-      <c r="T51" s="4">
-        <f ca="1"/>
-        <v>0.37822251634842252</v>
+      <c r="T51" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.3">
@@ -3107,9 +3368,9 @@
       <c r="S52" s="7">
         <v>0.93045439034459587</v>
       </c>
-      <c r="T52" s="4">
-        <f ca="1"/>
-        <v>0.38122419173045929</v>
+      <c r="T52" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.3">
@@ -3122,9 +3383,9 @@
       <c r="S53" s="7">
         <v>0.70064205520622802</v>
       </c>
-      <c r="T53" s="4">
-        <f ca="1"/>
-        <v>0.38693032613344891</v>
+      <c r="T53" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.3">
@@ -3137,486 +3398,486 @@
       <c r="S54" s="7">
         <v>0.34322350221251363</v>
       </c>
-      <c r="T54" s="4">
-        <f ca="1"/>
-        <v>0.38924117354343202</v>
+      <c r="T54" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S55" s="7">
         <v>0.30699880764121135</v>
       </c>
-      <c r="T55" s="4">
-        <f ca="1"/>
-        <v>0.41032128248045219</v>
+      <c r="T55" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S56" s="7">
         <v>0.56072877256876819</v>
       </c>
-      <c r="T56" s="4">
-        <f ca="1"/>
-        <v>0.43199912726020961</v>
+      <c r="T56" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S57" s="7">
         <v>1.0142003022623358E-2</v>
       </c>
-      <c r="T57" s="4">
-        <f ca="1"/>
-        <v>0.44362993322818001</v>
+      <c r="T57" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S58" s="7">
         <v>0.38122419173045929</v>
       </c>
-      <c r="T58" s="4">
-        <f ca="1"/>
-        <v>0.44578595954200495</v>
+      <c r="T58" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S59" s="7">
         <v>0.60411978716231773</v>
       </c>
-      <c r="T59" s="4">
-        <f ca="1"/>
-        <v>0.50309865693105404</v>
+      <c r="T59" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S60" s="7">
         <v>0.2819709570143808</v>
       </c>
-      <c r="T60" s="4">
-        <f ca="1"/>
-        <v>0.55553726039846762</v>
+      <c r="T60" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S61" s="7">
         <v>0.58507289523339523</v>
       </c>
-      <c r="T61" s="4">
-        <f ca="1"/>
-        <v>0.56072877256876819</v>
+      <c r="T61" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S62" s="7">
         <v>0.38693032613344891</v>
       </c>
-      <c r="T62" s="4">
-        <f ca="1"/>
-        <v>0.56613202852270661</v>
+      <c r="T62" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S63" s="7">
         <v>0.38924117354343202</v>
       </c>
-      <c r="T63" s="4">
-        <f ca="1"/>
-        <v>0.56907031356613658</v>
+      <c r="T63" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.3">
       <c r="S64" s="7">
         <v>0.25090708805825079</v>
       </c>
-      <c r="T64" s="4">
-        <f ca="1"/>
-        <v>0.57665750527755044</v>
+      <c r="T64" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="65" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S65" s="7">
         <v>0.99561513362173215</v>
       </c>
-      <c r="T65" s="4">
-        <f ca="1"/>
-        <v>0.57712158377157863</v>
+      <c r="T65" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="66" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S66" s="7">
         <v>0.41032128248045219</v>
       </c>
-      <c r="T66" s="4">
-        <f ca="1"/>
-        <v>0.58507289523339523</v>
+      <c r="T66" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="67" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S67" s="7">
         <v>0.10466409270245647</v>
       </c>
-      <c r="T67" s="4">
-        <f ca="1"/>
-        <v>0.5992299667126384</v>
+      <c r="T67" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="68" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S68" s="7">
         <v>0.96328079049455895</v>
       </c>
-      <c r="T68" s="4">
-        <f ca="1"/>
-        <v>0.60411978716231773</v>
+      <c r="T68" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="69" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S69" s="7">
         <v>0.99946735978378209</v>
       </c>
-      <c r="T69" s="4">
-        <f ca="1"/>
-        <v>0.60977631212733274</v>
+      <c r="T69" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="70" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S70" s="7">
         <v>0.82935893028115659</v>
       </c>
-      <c r="T70" s="4">
-        <f ca="1"/>
-        <v>0.61835596776400625</v>
+      <c r="T70" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S71" s="7">
         <v>0.15138392223952224</v>
       </c>
-      <c r="T71" s="4">
-        <f ca="1"/>
-        <v>0.64226730514312624</v>
+      <c r="T71" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S72" s="7">
         <v>0.26026766796149603</v>
       </c>
-      <c r="T72" s="4">
-        <f ca="1"/>
-        <v>0.64904570666639028</v>
+      <c r="T72" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="73" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S73" s="7">
         <v>0.56613202852270661</v>
       </c>
-      <c r="T73" s="4">
-        <f ca="1"/>
-        <v>0.67056525021684998</v>
+      <c r="T73" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="74" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S74" s="7">
         <v>0.57665750527755044</v>
       </c>
-      <c r="T74" s="4">
-        <f ca="1"/>
-        <v>0.68147699048550281</v>
+      <c r="T74" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="75" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S75" s="7">
         <v>0.83938605783476394</v>
       </c>
-      <c r="T75" s="4">
-        <f ca="1"/>
-        <v>0.70052257146975117</v>
+      <c r="T75" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="76" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S76" s="7">
         <v>0.37590154211670712</v>
       </c>
-      <c r="T76" s="4">
-        <f ca="1"/>
-        <v>0.70064205520622802</v>
+      <c r="T76" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="77" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S77" s="7">
         <v>0.95887267917531893</v>
       </c>
-      <c r="T77" s="4">
-        <f ca="1"/>
-        <v>0.70719203131190667</v>
+      <c r="T77" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="78" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S78" s="7">
         <v>0.11099657306935851</v>
       </c>
-      <c r="T78" s="4">
-        <f ca="1"/>
-        <v>0.71755405184921206</v>
+      <c r="T78" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="79" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S79" s="7">
         <v>0.67056525021684998</v>
       </c>
-      <c r="T79" s="4">
-        <f ca="1"/>
-        <v>0.73492497530386436</v>
+      <c r="T79" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="80" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S80" s="7">
         <v>0.82167610222353549</v>
       </c>
-      <c r="T80" s="4">
-        <f ca="1"/>
-        <v>0.78402600397426425</v>
+      <c r="T80" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="81" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S81" s="7">
         <v>0.79626472404113779</v>
       </c>
-      <c r="T81" s="4">
-        <f ca="1"/>
-        <v>0.79404440245310404</v>
+      <c r="T81" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="82" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S82" s="7">
         <v>0.79404440245310404</v>
       </c>
-      <c r="T82" s="4">
-        <f ca="1"/>
-        <v>0.79626472404113779</v>
+      <c r="T82" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="83" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S83" s="7">
         <v>0.24005046089105242</v>
       </c>
-      <c r="T83" s="4">
-        <f ca="1"/>
-        <v>0.79852373727417758</v>
+      <c r="T83" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="84" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S84" s="7">
         <v>1.7278225187227991E-2</v>
       </c>
-      <c r="T84" s="4">
-        <f ca="1"/>
-        <v>0.82167610222353549</v>
+      <c r="T84" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="85" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S85" s="7">
         <v>0.83233289115523368</v>
       </c>
-      <c r="T85" s="4">
-        <f ca="1"/>
-        <v>0.82935893028115659</v>
+      <c r="T85" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="86" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S86" s="7">
         <v>5.2437735118262885E-2</v>
       </c>
-      <c r="T86" s="4">
-        <f ca="1"/>
-        <v>0.83233289115523368</v>
+      <c r="T86" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="87" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S87" s="7">
         <v>0.79852373727417758</v>
       </c>
-      <c r="T87" s="4">
-        <f ca="1"/>
-        <v>0.83938605783476394</v>
+      <c r="T87" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="88" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S88" s="7">
         <v>0.88056162198032462</v>
       </c>
-      <c r="T88" s="4">
-        <f ca="1"/>
-        <v>0.85960749899325406</v>
+      <c r="T88" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="89" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S89" s="7">
         <v>0.29579294051174709</v>
       </c>
-      <c r="T89" s="4">
-        <f ca="1"/>
-        <v>0.86081826465673084</v>
+      <c r="T89" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="90" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S90" s="7">
         <v>0.71755405184921206</v>
       </c>
-      <c r="T90" s="4">
-        <f ca="1"/>
-        <v>0.86284631971635639</v>
+      <c r="T90" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="91" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S91" s="7">
         <v>0.97078869366691067</v>
       </c>
-      <c r="T91" s="4">
-        <f ca="1"/>
-        <v>0.88056162198032462</v>
+      <c r="T91" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="92" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S92" s="7">
         <v>4.8199686141203735E-2</v>
       </c>
-      <c r="T92" s="4">
-        <f ca="1"/>
-        <v>0.89299919543294648</v>
+      <c r="T92" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="93" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S93" s="7">
         <v>0.19150797219437865</v>
       </c>
-      <c r="T93" s="4">
-        <f ca="1"/>
-        <v>0.90600850571232516</v>
+      <c r="T93" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="94" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S94" s="7">
         <v>0.19332448079141096</v>
       </c>
-      <c r="T94" s="4">
-        <f ca="1"/>
-        <v>0.9287334580292661</v>
+      <c r="T94" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="95" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S95" s="7">
         <v>0.64904570666639028</v>
       </c>
-      <c r="T95" s="4">
-        <f ca="1"/>
-        <v>0.93045439034459587</v>
+      <c r="T95" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="96" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S96" s="7">
         <v>0.89299919543294648</v>
       </c>
-      <c r="T96" s="4">
-        <f ca="1"/>
-        <v>0.947318592329083</v>
+      <c r="T96" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="97" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S97" s="7">
         <v>0.98357223163047991</v>
       </c>
-      <c r="T97" s="4">
-        <f ca="1"/>
-        <v>0.94876869372932582</v>
+      <c r="T97" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="98" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S98" s="7">
         <v>0.95613469316823751</v>
       </c>
-      <c r="T98" s="4">
-        <f ca="1"/>
-        <v>0.95613469316823751</v>
+      <c r="T98" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="99" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S99" s="7">
         <v>0.97356891451331928</v>
       </c>
-      <c r="T99" s="4">
-        <f ca="1"/>
-        <v>0.95887267917531893</v>
+      <c r="T99" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="100" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S100" s="7">
         <v>0.64226730514312624</v>
       </c>
-      <c r="T100" s="4">
-        <f ca="1"/>
-        <v>0.96328079049455895</v>
+      <c r="T100" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="101" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S101" s="7">
         <v>0.61835596776400625</v>
       </c>
-      <c r="T101" s="4">
-        <f ca="1"/>
-        <v>0.96985704312068066</v>
+      <c r="T101" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="102" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S102" s="7">
         <v>0.86081826465673084</v>
       </c>
-      <c r="T102" s="4">
-        <f ca="1"/>
-        <v>0.97062641299883634</v>
+      <c r="T102" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="103" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S103" s="7">
         <v>0.16534127039316493</v>
       </c>
-      <c r="T103" s="4">
-        <f ca="1"/>
-        <v>0.97078869366691067</v>
+      <c r="T103" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="104" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S104" s="7">
         <v>0.9287334580292661</v>
       </c>
-      <c r="T104" s="4">
-        <f ca="1"/>
-        <v>0.97356891451331928</v>
+      <c r="T104" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="105" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S105" s="7">
         <v>8.9705088996498983E-3</v>
       </c>
-      <c r="T105" s="4">
-        <f ca="1"/>
-        <v>0.98357223163047991</v>
+      <c r="T105" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="106" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S106" s="7">
         <v>0.30621594261281582</v>
       </c>
-      <c r="T106" s="4">
-        <f ca="1"/>
-        <v>0.99561513362173215</v>
+      <c r="T106" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="107" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S107" s="7">
         <v>0.94876869372932582</v>
       </c>
-      <c r="T107" s="4">
-        <f ca="1"/>
-        <v>0.99946735978378209</v>
+      <c r="T107" s="4" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -3634,13 +3895,14 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
@@ -3652,23 +3914,25 @@
       <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="b">
-        <f t="array" ref="C3">SUM(0+(F3:H5=K3:M5))=9</f>
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <f>_xll.xloRef(K3:M5)</f>
-        <v>永[00000295DAB333B0]8004:8004,A</v>
-      </c>
-      <c r="F3" s="5">
-        <f t="array" ref="F3:H5">_xll.xloVal(E3)</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>2</v>
-      </c>
-      <c r="H3" s="5">
-        <v>3</v>
+      <c r="C3" s="12" t="e">
+        <f t="array" ref="C3" ca="1">SUM(0+(F3:H5=K3:M5))=9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E3" t="e">
+        <f ca="1">_xll.xloRef(K3:M5)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3" s="5" t="e">
+        <f t="array" aca="1" ref="F3:H5" ca="1">_xll.xloVal(E3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G3" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K3" s="7">
         <v>1</v>
@@ -3681,14 +3945,17 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F4" s="5">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5">
-        <v>5</v>
-      </c>
-      <c r="H4" s="5">
-        <v>6</v>
+      <c r="F4" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G4" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H4" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K4" s="7">
         <v>4</v>
@@ -3701,14 +3968,17 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F5" s="5">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5">
-        <v>8</v>
-      </c>
-      <c r="H5" s="5">
-        <v>9</v>
+      <c r="F5" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G5" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H5" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="K5" s="7">
         <v>7</v>
@@ -3724,71 +3994,74 @@
       <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="C8" t="b">
-        <f>D8=E8</f>
-        <v>1</v>
+      <c r="C8" s="12" t="e">
+        <f ca="1">D8=E8</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D8">
         <f>INDEX($K$3:$M$5,2,2)</f>
         <v>5</v>
       </c>
-      <c r="E8">
-        <f>_xll.xloIndex($E$3,2,2)</f>
-        <v>5</v>
+      <c r="E8" t="e">
+        <f ca="1">_xll.xloIndex($E$3,2,2)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C9" t="b">
-        <f>D9=E9</f>
-        <v>1</v>
+      <c r="C9" s="12" t="e">
+        <f ca="1">D9=E9</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D9">
         <f>INDEX($K$3:$M$5,1,2)</f>
         <v>2</v>
       </c>
-      <c r="E9">
-        <f>_xll.xloIndex($E$3,1,2)</f>
-        <v>2</v>
+      <c r="E9" t="e">
+        <f ca="1">_xll.xloIndex($E$3,1,2)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="C10" t="b">
-        <f>D10=E10</f>
-        <v>1</v>
+      <c r="C10" s="12" t="e">
+        <f ca="1">D10=E10</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D10">
         <f>INDEX(K3:K5,2)</f>
         <v>4</v>
       </c>
-      <c r="E10">
-        <f>_xll.xloIndex(K3:K5,2)</f>
-        <v>4</v>
+      <c r="E10" t="e">
+        <f ca="1">_xll.xloIndex(K3:K5,2)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="b">
-        <f>D13=E13</f>
-        <v>1</v>
+      <c r="C13" s="12" t="e">
+        <f ca="1">D13=E13</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D13">
         <f>INDEX(K3:M5,ROWS(K3:M5),COLUMNS(K3:M5))</f>
         <v>9</v>
       </c>
-      <c r="E13">
-        <f>_xll.xloIndex($E$3,-1,-1)</f>
-        <v>9</v>
-      </c>
+      <c r="E13" t="e">
+        <f ca="1">_xll.xloIndex($E$3,-1,-1)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="b">
-        <f t="array" ref="C15">SUM(0+(D15:E15=F15:G15))=2</f>
-        <v>1</v>
+      <c r="C15" s="12" t="e">
+        <f t="array" ref="C15" ca="1">SUM(0+(D15:E15=F15:G15))=2</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D15">
         <f>K3</f>
@@ -3798,52 +4071,56 @@
         <f>L3</f>
         <v>2</v>
       </c>
-      <c r="F15" s="5">
-        <f t="array" ref="F15:G15">_xll.xloIndex(E3,,,2,3)</f>
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>2</v>
+      <c r="F15" s="5" t="e">
+        <f t="array" aca="1" ref="F15:G15" ca="1">_xll.xloIndex(E3,,,2,3)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="b">
-        <f t="array" ref="C17">SUM(0+(D17:E18=F17:G18))=4</f>
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <f>G4</f>
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <f>H4</f>
-        <v>6</v>
-      </c>
-      <c r="F17" s="5">
-        <f t="array" ref="F17:G18">_xll.xloIndex($E$3,-2,-2, 0, 0)</f>
-        <v>5</v>
-      </c>
-      <c r="G17" s="5">
-        <v>6</v>
+      <c r="C17" s="12" t="e">
+        <f t="array" ref="C17" ca="1">SUM(0+(D17:E18=F17:G18))=4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D17" t="e">
+        <f ca="1">G4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E17" t="e">
+        <f ca="1">H4</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F17" s="5" t="e">
+        <f t="array" aca="1" ref="F17:G18" ca="1">_xll.xloIndex($E$3,-2,-2, 0, 0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G17" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D18">
-        <f>G5</f>
-        <v>8</v>
-      </c>
-      <c r="E18">
-        <f>H5</f>
-        <v>9</v>
-      </c>
-      <c r="F18" s="5">
-        <v>8</v>
-      </c>
-      <c r="G18" s="5">
-        <v>9</v>
+      <c r="D18" t="e">
+        <f ca="1">G5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" t="e">
+        <f ca="1">H5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F18" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="5" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>